<commit_message>
Update returns data through 6/30/2021
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\RMP\EquityHedging\data\update_strats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcz5chn\Documents\Projects\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -394,32 +394,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -469,7 +469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44189</v>
       </c>
@@ -519,7 +519,7 @@
         <v>341.29</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44190</v>
       </c>
@@ -569,7 +569,7 @@
         <v>341.29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44193</v>
       </c>
@@ -619,7 +619,7 @@
         <v>341.42</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44194</v>
       </c>
@@ -669,7 +669,7 @@
         <v>341.79</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44195</v>
       </c>
@@ -719,7 +719,7 @@
         <v>341.9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44196</v>
       </c>
@@ -769,7 +769,7 @@
         <v>341.99</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44197</v>
       </c>
@@ -819,7 +819,7 @@
         <v>341.99</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44200</v>
       </c>
@@ -869,7 +869,7 @@
         <v>340.27</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44201</v>
       </c>
@@ -919,7 +919,7 @@
         <v>341.21</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44202</v>
       </c>
@@ -969,7 +969,7 @@
         <v>341.71</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44203</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>341.82</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44204</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>341.91</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44207</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>342.46</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44208</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>342.75</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44209</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>342.71</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44210</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>342.55</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44211</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>342.9</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44214</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>342.9</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44215</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>343.72</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44216</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>343.34</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44217</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>343.78</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44218</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>344.12</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44221</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>344.65</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>44222</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>345.1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44223</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>346.49</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44224</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>346.56</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44225</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>347.42</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>44228</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>346.91</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44229</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>346.34</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>44230</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>346.25</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44231</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>346.06</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>44232</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>346.16</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>44235</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>346.13</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>44236</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>346.28</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>44237</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>346.53</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>44238</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>347.36</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>44239</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>348.1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>44242</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>348.1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>44243</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>348.89</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>44244</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>349.44</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>44245</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>349.44</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>44246</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>350.1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>44249</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>350.45</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44250</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>350.79</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44251</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>350.25</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>44252</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>347.56</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>44253</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>348.93</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>44256</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>349.2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>44257</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>349.6</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>44258</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>350.15</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>44259</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>348.97</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>44260</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>349.39</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>44263</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>350.05</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>44264</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>349.76</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44265</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>349.65</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44266</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>349.15</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44267</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>349.42</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44270</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>349.38</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44271</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>349.54</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44272</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>349.63</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44273</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>348.15</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44274</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>349.6</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44277</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>349.68</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44278</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>349.81</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44279</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>350.19</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44280</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>350.56</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>44281</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>349.66</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>44284</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>350.36</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>44285</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>350.61</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>44286</v>
       </c>
@@ -3967,6 +3967,3256 @@
       </c>
       <c r="P71">
         <v>350.77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B72">
+        <v>8335.9089999999997</v>
+      </c>
+      <c r="C72">
+        <v>8575.74</v>
+      </c>
+      <c r="D72">
+        <v>346.89</v>
+      </c>
+      <c r="E72">
+        <v>4906.5200000000004</v>
+      </c>
+      <c r="F72">
+        <v>189.63</v>
+      </c>
+      <c r="G72">
+        <v>120.7552</v>
+      </c>
+      <c r="H72">
+        <v>173.5</v>
+      </c>
+      <c r="I72">
+        <v>113.489</v>
+      </c>
+      <c r="J72">
+        <v>113.9833</v>
+      </c>
+      <c r="K72">
+        <v>864.88</v>
+      </c>
+      <c r="L72">
+        <v>1116.8499999999999</v>
+      </c>
+      <c r="M72">
+        <v>298.89229999999998</v>
+      </c>
+      <c r="N72">
+        <v>293.60000000000002</v>
+      </c>
+      <c r="O72">
+        <v>381.4</v>
+      </c>
+      <c r="P72">
+        <v>350.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>44288</v>
+      </c>
+      <c r="B73">
+        <v>8335.9089999999997</v>
+      </c>
+      <c r="C73">
+        <v>8575.74</v>
+      </c>
+      <c r="D73">
+        <v>347.18</v>
+      </c>
+      <c r="E73">
+        <v>4887.8900000000003</v>
+      </c>
+      <c r="F73">
+        <v>188.29</v>
+      </c>
+      <c r="G73">
+        <v>120.7552</v>
+      </c>
+      <c r="H73">
+        <v>173.5</v>
+      </c>
+      <c r="I73">
+        <v>113.489</v>
+      </c>
+      <c r="J73">
+        <v>113.9833</v>
+      </c>
+      <c r="K73">
+        <v>864.88</v>
+      </c>
+      <c r="L73">
+        <v>1116.8499999999999</v>
+      </c>
+      <c r="M73">
+        <v>298.89229999999998</v>
+      </c>
+      <c r="N73">
+        <v>293.60000000000002</v>
+      </c>
+      <c r="O73">
+        <v>381.4</v>
+      </c>
+      <c r="P73">
+        <v>350.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>44291</v>
+      </c>
+      <c r="B74">
+        <v>8457.3970000000008</v>
+      </c>
+      <c r="C74">
+        <v>8575.74</v>
+      </c>
+      <c r="D74">
+        <v>350.52</v>
+      </c>
+      <c r="E74">
+        <v>4889.01</v>
+      </c>
+      <c r="F74">
+        <v>188.6</v>
+      </c>
+      <c r="G74">
+        <v>121.0033</v>
+      </c>
+      <c r="H74">
+        <v>173.6</v>
+      </c>
+      <c r="I74">
+        <v>113.4701</v>
+      </c>
+      <c r="J74">
+        <v>113.9593</v>
+      </c>
+      <c r="K74">
+        <v>862.82</v>
+      </c>
+      <c r="L74">
+        <v>1116.3800000000001</v>
+      </c>
+      <c r="M74">
+        <v>298.58440000000002</v>
+      </c>
+      <c r="N74">
+        <v>293.14</v>
+      </c>
+      <c r="O74">
+        <v>380.72</v>
+      </c>
+      <c r="P74">
+        <v>349.91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B75">
+        <v>8449.5419999999995</v>
+      </c>
+      <c r="C75">
+        <v>8634.7000000000007</v>
+      </c>
+      <c r="D75">
+        <v>351.16</v>
+      </c>
+      <c r="E75">
+        <v>4913.8</v>
+      </c>
+      <c r="F75">
+        <v>190.16</v>
+      </c>
+      <c r="G75">
+        <v>120.9764</v>
+      </c>
+      <c r="H75">
+        <v>173.58</v>
+      </c>
+      <c r="I75">
+        <v>113.47020000000001</v>
+      </c>
+      <c r="J75">
+        <v>113.95399999999999</v>
+      </c>
+      <c r="K75">
+        <v>862.9</v>
+      </c>
+      <c r="L75">
+        <v>1112.81</v>
+      </c>
+      <c r="M75">
+        <v>298.44839999999999</v>
+      </c>
+      <c r="N75">
+        <v>293.32</v>
+      </c>
+      <c r="O75">
+        <v>380.76</v>
+      </c>
+      <c r="P75">
+        <v>350.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>44293</v>
+      </c>
+      <c r="B76">
+        <v>8462.1749999999993</v>
+      </c>
+      <c r="C76">
+        <v>8605.0300000000007</v>
+      </c>
+      <c r="D76">
+        <v>351.42</v>
+      </c>
+      <c r="E76">
+        <v>4890.3100000000004</v>
+      </c>
+      <c r="F76">
+        <v>188.39</v>
+      </c>
+      <c r="G76">
+        <v>120.81229999999999</v>
+      </c>
+      <c r="H76">
+        <v>173.59</v>
+      </c>
+      <c r="I76">
+        <v>113.45950000000001</v>
+      </c>
+      <c r="J76">
+        <v>113.94880000000001</v>
+      </c>
+      <c r="K76">
+        <v>862.91</v>
+      </c>
+      <c r="L76">
+        <v>1113.53</v>
+      </c>
+      <c r="M76">
+        <v>298.52859999999998</v>
+      </c>
+      <c r="N76">
+        <v>293.44</v>
+      </c>
+      <c r="O76">
+        <v>381.02</v>
+      </c>
+      <c r="P76">
+        <v>350.3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>44294</v>
+      </c>
+      <c r="B77">
+        <v>8499.85</v>
+      </c>
+      <c r="C77">
+        <v>8650.83</v>
+      </c>
+      <c r="D77">
+        <v>353.16</v>
+      </c>
+      <c r="E77">
+        <v>4921.3999999999996</v>
+      </c>
+      <c r="F77">
+        <v>190.36</v>
+      </c>
+      <c r="G77">
+        <v>120.8325</v>
+      </c>
+      <c r="H77">
+        <v>173.7</v>
+      </c>
+      <c r="I77">
+        <v>113.4415</v>
+      </c>
+      <c r="J77">
+        <v>113.9301</v>
+      </c>
+      <c r="K77">
+        <v>862.4</v>
+      </c>
+      <c r="L77">
+        <v>1112.8</v>
+      </c>
+      <c r="M77">
+        <v>298.34910000000002</v>
+      </c>
+      <c r="N77">
+        <v>293.5</v>
+      </c>
+      <c r="O77">
+        <v>381.18</v>
+      </c>
+      <c r="P77">
+        <v>350.44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B78">
+        <v>8565.5730000000003</v>
+      </c>
+      <c r="C78">
+        <v>8653.02</v>
+      </c>
+      <c r="D78">
+        <v>354.27</v>
+      </c>
+      <c r="E78">
+        <v>4908.43</v>
+      </c>
+      <c r="F78">
+        <v>189.6</v>
+      </c>
+      <c r="G78">
+        <v>121.0616</v>
+      </c>
+      <c r="H78">
+        <v>173.8</v>
+      </c>
+      <c r="I78">
+        <v>113.44240000000001</v>
+      </c>
+      <c r="J78">
+        <v>113.9335</v>
+      </c>
+      <c r="K78">
+        <v>861.46</v>
+      </c>
+      <c r="L78">
+        <v>1110.94</v>
+      </c>
+      <c r="M78">
+        <v>298.18029999999999</v>
+      </c>
+      <c r="N78">
+        <v>293.33</v>
+      </c>
+      <c r="O78">
+        <v>381.03</v>
+      </c>
+      <c r="P78">
+        <v>350.36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B79">
+        <v>8564.0300000000007</v>
+      </c>
+      <c r="C79">
+        <v>8616.17</v>
+      </c>
+      <c r="D79">
+        <v>353.7</v>
+      </c>
+      <c r="E79">
+        <v>4909.63</v>
+      </c>
+      <c r="F79">
+        <v>189.6</v>
+      </c>
+      <c r="G79">
+        <v>121.0535</v>
+      </c>
+      <c r="H79">
+        <v>173.71</v>
+      </c>
+      <c r="I79">
+        <v>113.44070000000001</v>
+      </c>
+      <c r="J79">
+        <v>113.9335</v>
+      </c>
+      <c r="K79">
+        <v>861.58</v>
+      </c>
+      <c r="L79">
+        <v>1111.6500000000001</v>
+      </c>
+      <c r="M79">
+        <v>297.95429999999999</v>
+      </c>
+      <c r="N79">
+        <v>293.8</v>
+      </c>
+      <c r="O79">
+        <v>381.15</v>
+      </c>
+      <c r="P79">
+        <v>350.69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>44299</v>
+      </c>
+      <c r="B80">
+        <v>8592.2459999999992</v>
+      </c>
+      <c r="C80">
+        <v>8627.25</v>
+      </c>
+      <c r="D80">
+        <v>354.92</v>
+      </c>
+      <c r="E80">
+        <v>4933.3500000000004</v>
+      </c>
+      <c r="F80">
+        <v>191.2</v>
+      </c>
+      <c r="G80">
+        <v>121.1113</v>
+      </c>
+      <c r="H80">
+        <v>173.78</v>
+      </c>
+      <c r="I80">
+        <v>113.4277</v>
+      </c>
+      <c r="J80">
+        <v>113.9072</v>
+      </c>
+      <c r="K80">
+        <v>861.32</v>
+      </c>
+      <c r="L80">
+        <v>1113.1099999999999</v>
+      </c>
+      <c r="M80">
+        <v>297.9178</v>
+      </c>
+      <c r="N80">
+        <v>293.94</v>
+      </c>
+      <c r="O80">
+        <v>381.22</v>
+      </c>
+      <c r="P80">
+        <v>350.83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B81">
+        <v>8558.1560000000009</v>
+      </c>
+      <c r="C81">
+        <v>8647.4599999999991</v>
+      </c>
+      <c r="D81">
+        <v>354.88</v>
+      </c>
+      <c r="E81">
+        <v>4929.9799999999996</v>
+      </c>
+      <c r="F81">
+        <v>190.48</v>
+      </c>
+      <c r="G81">
+        <v>121.0989</v>
+      </c>
+      <c r="H81">
+        <v>173.71</v>
+      </c>
+      <c r="I81">
+        <v>113.4306</v>
+      </c>
+      <c r="J81">
+        <v>113.9105</v>
+      </c>
+      <c r="K81">
+        <v>861.62</v>
+      </c>
+      <c r="L81">
+        <v>1114.24</v>
+      </c>
+      <c r="M81">
+        <v>297.99560000000002</v>
+      </c>
+      <c r="N81">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="O81">
+        <v>381.37</v>
+      </c>
+      <c r="P81">
+        <v>351.01</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>44301</v>
+      </c>
+      <c r="B82">
+        <v>8653.2870000000003</v>
+      </c>
+      <c r="C82">
+        <v>8684.76</v>
+      </c>
+      <c r="D82">
+        <v>358.06</v>
+      </c>
+      <c r="E82">
+        <v>4984.13</v>
+      </c>
+      <c r="F82">
+        <v>194.52</v>
+      </c>
+      <c r="G82">
+        <v>121.33199999999999</v>
+      </c>
+      <c r="H82">
+        <v>173.9</v>
+      </c>
+      <c r="I82">
+        <v>113.4161</v>
+      </c>
+      <c r="J82">
+        <v>113.89870000000001</v>
+      </c>
+      <c r="K82">
+        <v>860.41</v>
+      </c>
+      <c r="L82">
+        <v>1113.18</v>
+      </c>
+      <c r="M82">
+        <v>298.1583</v>
+      </c>
+      <c r="N82">
+        <v>293.64</v>
+      </c>
+      <c r="O82">
+        <v>380.9</v>
+      </c>
+      <c r="P82">
+        <v>350.29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B83">
+        <v>8684.5059999999994</v>
+      </c>
+      <c r="C83">
+        <v>8771.83</v>
+      </c>
+      <c r="D83">
+        <v>359.56</v>
+      </c>
+      <c r="E83">
+        <v>4942.8999999999996</v>
+      </c>
+      <c r="F83">
+        <v>192.71</v>
+      </c>
+      <c r="G83">
+        <v>121.4357</v>
+      </c>
+      <c r="H83">
+        <v>173.82</v>
+      </c>
+      <c r="I83">
+        <v>113.40219999999999</v>
+      </c>
+      <c r="J83">
+        <v>113.8879</v>
+      </c>
+      <c r="K83">
+        <v>860.13</v>
+      </c>
+      <c r="L83">
+        <v>1110.25</v>
+      </c>
+      <c r="M83">
+        <v>297.96129999999999</v>
+      </c>
+      <c r="N83">
+        <v>293.72000000000003</v>
+      </c>
+      <c r="O83">
+        <v>381.24</v>
+      </c>
+      <c r="P83">
+        <v>350.88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B84">
+        <v>8638.4210000000003</v>
+      </c>
+      <c r="C84">
+        <v>8746.0400000000009</v>
+      </c>
+      <c r="D84">
+        <v>358.62</v>
+      </c>
+      <c r="E84">
+        <v>4919.93</v>
+      </c>
+      <c r="F84">
+        <v>191.98</v>
+      </c>
+      <c r="G84">
+        <v>121.39319999999999</v>
+      </c>
+      <c r="H84">
+        <v>173.77</v>
+      </c>
+      <c r="I84">
+        <v>113.43219999999999</v>
+      </c>
+      <c r="J84">
+        <v>113.90219999999999</v>
+      </c>
+      <c r="K84">
+        <v>860.61</v>
+      </c>
+      <c r="L84">
+        <v>1110.76</v>
+      </c>
+      <c r="M84">
+        <v>298.1379</v>
+      </c>
+      <c r="N84">
+        <v>293.68</v>
+      </c>
+      <c r="O84">
+        <v>381.4</v>
+      </c>
+      <c r="P84">
+        <v>351.06</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B85">
+        <v>8579.9470000000001</v>
+      </c>
+      <c r="C85">
+        <v>8578.0400000000009</v>
+      </c>
+      <c r="D85">
+        <v>355.61</v>
+      </c>
+      <c r="E85">
+        <v>4931.4399999999996</v>
+      </c>
+      <c r="F85">
+        <v>193.07</v>
+      </c>
+      <c r="G85">
+        <v>121.31489999999999</v>
+      </c>
+      <c r="H85">
+        <v>173.61</v>
+      </c>
+      <c r="I85">
+        <v>113.4479</v>
+      </c>
+      <c r="J85">
+        <v>113.935</v>
+      </c>
+      <c r="K85">
+        <v>861.29</v>
+      </c>
+      <c r="L85">
+        <v>1111.06</v>
+      </c>
+      <c r="M85">
+        <v>297.75510000000003</v>
+      </c>
+      <c r="N85">
+        <v>293.27</v>
+      </c>
+      <c r="O85">
+        <v>380.47</v>
+      </c>
+      <c r="P85">
+        <v>350.79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B86">
+        <v>8659.7990000000009</v>
+      </c>
+      <c r="C86">
+        <v>8656.2900000000009</v>
+      </c>
+      <c r="D86">
+        <v>357.08</v>
+      </c>
+      <c r="E86">
+        <v>4942.47</v>
+      </c>
+      <c r="F86">
+        <v>193.54</v>
+      </c>
+      <c r="G86">
+        <v>121.32429999999999</v>
+      </c>
+      <c r="H86">
+        <v>173.89</v>
+      </c>
+      <c r="I86">
+        <v>113.32210000000001</v>
+      </c>
+      <c r="J86">
+        <v>113.8466</v>
+      </c>
+      <c r="K86">
+        <v>860.26</v>
+      </c>
+      <c r="L86">
+        <v>1109.55</v>
+      </c>
+      <c r="M86">
+        <v>298.09469999999999</v>
+      </c>
+      <c r="N86">
+        <v>293.02</v>
+      </c>
+      <c r="O86">
+        <v>380.55</v>
+      </c>
+      <c r="P86">
+        <v>350.16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B87">
+        <v>8580.7309999999998</v>
+      </c>
+      <c r="C87">
+        <v>8739.86</v>
+      </c>
+      <c r="D87">
+        <v>356.3</v>
+      </c>
+      <c r="E87">
+        <v>4960.1000000000004</v>
+      </c>
+      <c r="F87">
+        <v>194.63</v>
+      </c>
+      <c r="G87">
+        <v>121.39100000000001</v>
+      </c>
+      <c r="H87">
+        <v>173.85</v>
+      </c>
+      <c r="I87">
+        <v>113.337</v>
+      </c>
+      <c r="J87">
+        <v>113.84180000000001</v>
+      </c>
+      <c r="K87">
+        <v>861.16</v>
+      </c>
+      <c r="L87">
+        <v>1108.73</v>
+      </c>
+      <c r="M87">
+        <v>298.94110000000001</v>
+      </c>
+      <c r="N87">
+        <v>292.91000000000003</v>
+      </c>
+      <c r="O87">
+        <v>380.1</v>
+      </c>
+      <c r="P87">
+        <v>349.59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B88">
+        <v>8674.7960000000003</v>
+      </c>
+      <c r="C88">
+        <v>8736.68</v>
+      </c>
+      <c r="D88">
+        <v>359.06</v>
+      </c>
+      <c r="E88">
+        <v>4961.5200000000004</v>
+      </c>
+      <c r="F88">
+        <v>194.13</v>
+      </c>
+      <c r="G88">
+        <v>121.4926</v>
+      </c>
+      <c r="H88">
+        <v>173.94</v>
+      </c>
+      <c r="I88">
+        <v>113.2437</v>
+      </c>
+      <c r="J88">
+        <v>113.76909999999999</v>
+      </c>
+      <c r="K88">
+        <v>860</v>
+      </c>
+      <c r="L88">
+        <v>1106.18</v>
+      </c>
+      <c r="M88">
+        <v>299.935</v>
+      </c>
+      <c r="N88">
+        <v>291.97000000000003</v>
+      </c>
+      <c r="O88">
+        <v>379.43</v>
+      </c>
+      <c r="P88">
+        <v>349.34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B89">
+        <v>8690.2569999999996</v>
+      </c>
+      <c r="C89">
+        <v>8752.98</v>
+      </c>
+      <c r="D89">
+        <v>360.39</v>
+      </c>
+      <c r="E89">
+        <v>4960.92</v>
+      </c>
+      <c r="F89">
+        <v>193.85</v>
+      </c>
+      <c r="G89">
+        <v>121.5487</v>
+      </c>
+      <c r="H89">
+        <v>173.77</v>
+      </c>
+      <c r="I89">
+        <v>113.2484</v>
+      </c>
+      <c r="J89">
+        <v>113.7435</v>
+      </c>
+      <c r="K89">
+        <v>859.84</v>
+      </c>
+      <c r="L89">
+        <v>1105.49</v>
+      </c>
+      <c r="M89">
+        <v>299.76490000000001</v>
+      </c>
+      <c r="N89">
+        <v>292.11</v>
+      </c>
+      <c r="O89">
+        <v>379.6</v>
+      </c>
+      <c r="P89">
+        <v>349.56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B90">
+        <v>8688.4519999999993</v>
+      </c>
+      <c r="C90">
+        <v>8735.7099999999991</v>
+      </c>
+      <c r="D90">
+        <v>360.01</v>
+      </c>
+      <c r="E90">
+        <v>4928.96</v>
+      </c>
+      <c r="F90">
+        <v>191.72</v>
+      </c>
+      <c r="G90">
+        <v>121.5352</v>
+      </c>
+      <c r="H90">
+        <v>173.74</v>
+      </c>
+      <c r="I90">
+        <v>113.2137</v>
+      </c>
+      <c r="J90">
+        <v>113.7321</v>
+      </c>
+      <c r="K90">
+        <v>859.95</v>
+      </c>
+      <c r="L90">
+        <v>1104.2</v>
+      </c>
+      <c r="M90">
+        <v>299.67090000000002</v>
+      </c>
+      <c r="N90">
+        <v>292.27</v>
+      </c>
+      <c r="O90">
+        <v>379.63</v>
+      </c>
+      <c r="P90">
+        <v>349.81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B91">
+        <v>8681.1659999999993</v>
+      </c>
+      <c r="C91">
+        <v>8746.7800000000007</v>
+      </c>
+      <c r="D91">
+        <v>360.13</v>
+      </c>
+      <c r="E91">
+        <v>4928.79</v>
+      </c>
+      <c r="F91">
+        <v>191.81</v>
+      </c>
+      <c r="G91">
+        <v>121.4949</v>
+      </c>
+      <c r="H91">
+        <v>173.87</v>
+      </c>
+      <c r="I91">
+        <v>113.2032</v>
+      </c>
+      <c r="J91">
+        <v>113.7062</v>
+      </c>
+      <c r="K91">
+        <v>860.11</v>
+      </c>
+      <c r="L91">
+        <v>1101.9100000000001</v>
+      </c>
+      <c r="M91">
+        <v>299.71129999999999</v>
+      </c>
+      <c r="N91">
+        <v>292.45</v>
+      </c>
+      <c r="O91">
+        <v>379.95</v>
+      </c>
+      <c r="P91">
+        <v>349.94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B92">
+        <v>8740.3490000000002</v>
+      </c>
+      <c r="C92">
+        <v>8710.86</v>
+      </c>
+      <c r="D92">
+        <v>361.36</v>
+      </c>
+      <c r="E92">
+        <v>4917.3599999999997</v>
+      </c>
+      <c r="F92">
+        <v>191.06</v>
+      </c>
+      <c r="G92">
+        <v>121.63590000000001</v>
+      </c>
+      <c r="H92">
+        <v>173.93</v>
+      </c>
+      <c r="I92">
+        <v>113.2081</v>
+      </c>
+      <c r="J92">
+        <v>113.6996</v>
+      </c>
+      <c r="K92">
+        <v>859.29</v>
+      </c>
+      <c r="L92">
+        <v>1099.8499999999999</v>
+      </c>
+      <c r="M92">
+        <v>299.65230000000003</v>
+      </c>
+      <c r="N92">
+        <v>292.45999999999998</v>
+      </c>
+      <c r="O92">
+        <v>379.94</v>
+      </c>
+      <c r="P92">
+        <v>349.79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B93">
+        <v>8678.1610000000001</v>
+      </c>
+      <c r="C93">
+        <v>8670.31</v>
+      </c>
+      <c r="D93">
+        <v>358.21</v>
+      </c>
+      <c r="E93">
+        <v>4926.78</v>
+      </c>
+      <c r="F93">
+        <v>191.75</v>
+      </c>
+      <c r="G93">
+        <v>121.5433</v>
+      </c>
+      <c r="H93">
+        <v>173.97</v>
+      </c>
+      <c r="I93">
+        <v>113.2397</v>
+      </c>
+      <c r="J93">
+        <v>113.7281</v>
+      </c>
+      <c r="K93">
+        <v>859.95</v>
+      </c>
+      <c r="L93">
+        <v>1096.8</v>
+      </c>
+      <c r="M93">
+        <v>299.80110000000002</v>
+      </c>
+      <c r="N93">
+        <v>292.62</v>
+      </c>
+      <c r="O93">
+        <v>380.03</v>
+      </c>
+      <c r="P93">
+        <v>349.72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B94">
+        <v>8702.0249999999996</v>
+      </c>
+      <c r="C94">
+        <v>8727.89</v>
+      </c>
+      <c r="D94">
+        <v>358.98</v>
+      </c>
+      <c r="E94">
+        <v>4935.8100000000004</v>
+      </c>
+      <c r="F94">
+        <v>191.72</v>
+      </c>
+      <c r="G94">
+        <v>121.5368</v>
+      </c>
+      <c r="H94">
+        <v>173.88</v>
+      </c>
+      <c r="I94">
+        <v>113.1788</v>
+      </c>
+      <c r="J94">
+        <v>113.6776</v>
+      </c>
+      <c r="K94">
+        <v>859.69</v>
+      </c>
+      <c r="L94">
+        <v>1095</v>
+      </c>
+      <c r="M94">
+        <v>300.09649999999999</v>
+      </c>
+      <c r="N94">
+        <v>292.94</v>
+      </c>
+      <c r="O94">
+        <v>380.17</v>
+      </c>
+      <c r="P94">
+        <v>350.29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B95">
+        <v>8643.9130000000005</v>
+      </c>
+      <c r="C95">
+        <v>8565</v>
+      </c>
+      <c r="D95">
+        <v>356.08</v>
+      </c>
+      <c r="E95">
+        <v>4952.1899999999996</v>
+      </c>
+      <c r="F95">
+        <v>193.34</v>
+      </c>
+      <c r="G95">
+        <v>121.5112</v>
+      </c>
+      <c r="H95">
+        <v>173.77</v>
+      </c>
+      <c r="I95">
+        <v>113.3082</v>
+      </c>
+      <c r="J95">
+        <v>113.7818</v>
+      </c>
+      <c r="K95">
+        <v>860.3</v>
+      </c>
+      <c r="L95">
+        <v>1102.18</v>
+      </c>
+      <c r="M95">
+        <v>300.33010000000002</v>
+      </c>
+      <c r="N95">
+        <v>291.69</v>
+      </c>
+      <c r="O95">
+        <v>378.3</v>
+      </c>
+      <c r="P95">
+        <v>348.92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B96">
+        <v>8650.0380000000005</v>
+      </c>
+      <c r="C96">
+        <v>8743.33</v>
+      </c>
+      <c r="D96">
+        <v>357.13</v>
+      </c>
+      <c r="E96">
+        <v>4961.95</v>
+      </c>
+      <c r="F96">
+        <v>193.77</v>
+      </c>
+      <c r="G96">
+        <v>121.366</v>
+      </c>
+      <c r="H96">
+        <v>173.71</v>
+      </c>
+      <c r="I96">
+        <v>112.9803</v>
+      </c>
+      <c r="J96">
+        <v>113.5692</v>
+      </c>
+      <c r="K96">
+        <v>860.31</v>
+      </c>
+      <c r="L96">
+        <v>1099.48</v>
+      </c>
+      <c r="M96">
+        <v>300.50110000000001</v>
+      </c>
+      <c r="N96">
+        <v>292.02</v>
+      </c>
+      <c r="O96">
+        <v>378.71</v>
+      </c>
+      <c r="P96">
+        <v>349.3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B97">
+        <v>8722.0360000000001</v>
+      </c>
+      <c r="C97">
+        <v>8744.7000000000007</v>
+      </c>
+      <c r="D97">
+        <v>359.51</v>
+      </c>
+      <c r="E97">
+        <v>4972.8100000000004</v>
+      </c>
+      <c r="F97">
+        <v>194.09</v>
+      </c>
+      <c r="G97">
+        <v>121.4905</v>
+      </c>
+      <c r="H97">
+        <v>173.88</v>
+      </c>
+      <c r="I97">
+        <v>112.9833</v>
+      </c>
+      <c r="J97">
+        <v>113.61450000000001</v>
+      </c>
+      <c r="K97">
+        <v>859.12</v>
+      </c>
+      <c r="L97">
+        <v>1100.8900000000001</v>
+      </c>
+      <c r="M97">
+        <v>300.02409999999998</v>
+      </c>
+      <c r="N97">
+        <v>291.99</v>
+      </c>
+      <c r="O97">
+        <v>378.88</v>
+      </c>
+      <c r="P97">
+        <v>349.16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B98">
+        <v>8787.8150000000005</v>
+      </c>
+      <c r="C98">
+        <v>8830.2900000000009</v>
+      </c>
+      <c r="D98">
+        <v>362.74</v>
+      </c>
+      <c r="E98">
+        <v>4964.7</v>
+      </c>
+      <c r="F98">
+        <v>192.85</v>
+      </c>
+      <c r="G98">
+        <v>121.4953</v>
+      </c>
+      <c r="H98">
+        <v>173.98</v>
+      </c>
+      <c r="I98">
+        <v>112.8158</v>
+      </c>
+      <c r="J98">
+        <v>113.37779999999999</v>
+      </c>
+      <c r="K98">
+        <v>858.24</v>
+      </c>
+      <c r="L98">
+        <v>1098.17</v>
+      </c>
+      <c r="M98">
+        <v>299.40910000000002</v>
+      </c>
+      <c r="N98">
+        <v>291.69</v>
+      </c>
+      <c r="O98">
+        <v>378.7</v>
+      </c>
+      <c r="P98">
+        <v>349.01</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>44326</v>
+      </c>
+      <c r="B99">
+        <v>8696.2939999999999</v>
+      </c>
+      <c r="C99">
+        <v>8814.3799999999992</v>
+      </c>
+      <c r="D99">
+        <v>360.82</v>
+      </c>
+      <c r="E99">
+        <v>4930.2299999999996</v>
+      </c>
+      <c r="F99">
+        <v>190.24</v>
+      </c>
+      <c r="G99">
+        <v>121.4025</v>
+      </c>
+      <c r="H99">
+        <v>173.78</v>
+      </c>
+      <c r="I99">
+        <v>112.7985</v>
+      </c>
+      <c r="J99">
+        <v>113.33240000000001</v>
+      </c>
+      <c r="K99">
+        <v>859.37</v>
+      </c>
+      <c r="L99">
+        <v>1103.03</v>
+      </c>
+      <c r="M99">
+        <v>300.23509999999999</v>
+      </c>
+      <c r="N99">
+        <v>291.23</v>
+      </c>
+      <c r="O99">
+        <v>378.73</v>
+      </c>
+      <c r="P99">
+        <v>348.89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>44327</v>
+      </c>
+      <c r="B100">
+        <v>8620.9789999999994</v>
+      </c>
+      <c r="C100">
+        <v>8645.06</v>
+      </c>
+      <c r="D100">
+        <v>356.71</v>
+      </c>
+      <c r="E100">
+        <v>4896.78</v>
+      </c>
+      <c r="F100">
+        <v>188.75</v>
+      </c>
+      <c r="G100">
+        <v>121.5484</v>
+      </c>
+      <c r="H100">
+        <v>173.97</v>
+      </c>
+      <c r="I100">
+        <v>112.94199999999999</v>
+      </c>
+      <c r="J100">
+        <v>113.43470000000001</v>
+      </c>
+      <c r="K100">
+        <v>860.1</v>
+      </c>
+      <c r="L100">
+        <v>1102.3900000000001</v>
+      </c>
+      <c r="M100">
+        <v>299.27280000000002</v>
+      </c>
+      <c r="N100">
+        <v>290.89</v>
+      </c>
+      <c r="O100">
+        <v>377.64</v>
+      </c>
+      <c r="P100">
+        <v>349.04</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>44328</v>
+      </c>
+      <c r="B101">
+        <v>8437.2350000000006</v>
+      </c>
+      <c r="C101">
+        <v>8648.0400000000009</v>
+      </c>
+      <c r="D101">
+        <v>350.78</v>
+      </c>
+      <c r="E101">
+        <v>4858.63</v>
+      </c>
+      <c r="F101">
+        <v>186.25</v>
+      </c>
+      <c r="G101">
+        <v>122.12909999999999</v>
+      </c>
+      <c r="H101">
+        <v>174.44</v>
+      </c>
+      <c r="I101">
+        <v>113.8556</v>
+      </c>
+      <c r="J101">
+        <v>114.1996</v>
+      </c>
+      <c r="K101">
+        <v>862.52</v>
+      </c>
+      <c r="L101">
+        <v>1102.8599999999999</v>
+      </c>
+      <c r="M101">
+        <v>296.9699</v>
+      </c>
+      <c r="N101">
+        <v>290.93</v>
+      </c>
+      <c r="O101">
+        <v>376.52</v>
+      </c>
+      <c r="P101">
+        <v>351.05</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B102">
+        <v>8541.3860000000004</v>
+      </c>
+      <c r="C102">
+        <v>8666.07</v>
+      </c>
+      <c r="D102">
+        <v>351.76</v>
+      </c>
+      <c r="E102">
+        <v>4871.3100000000004</v>
+      </c>
+      <c r="F102">
+        <v>186.39</v>
+      </c>
+      <c r="G102">
+        <v>121.53619999999999</v>
+      </c>
+      <c r="H102">
+        <v>174.04</v>
+      </c>
+      <c r="I102">
+        <v>111.74290000000001</v>
+      </c>
+      <c r="J102">
+        <v>113.09569999999999</v>
+      </c>
+      <c r="K102">
+        <v>860.98</v>
+      </c>
+      <c r="L102">
+        <v>1102.82</v>
+      </c>
+      <c r="M102">
+        <v>300.01900000000001</v>
+      </c>
+      <c r="N102">
+        <v>290.23</v>
+      </c>
+      <c r="O102">
+        <v>376.11</v>
+      </c>
+      <c r="P102">
+        <v>349.99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>44330</v>
+      </c>
+      <c r="B103">
+        <v>8669.49</v>
+      </c>
+      <c r="C103">
+        <v>8808.57</v>
+      </c>
+      <c r="D103">
+        <v>357.19</v>
+      </c>
+      <c r="E103">
+        <v>4912.92</v>
+      </c>
+      <c r="F103">
+        <v>188.68</v>
+      </c>
+      <c r="G103">
+        <v>121.49120000000001</v>
+      </c>
+      <c r="H103">
+        <v>173.95</v>
+      </c>
+      <c r="I103">
+        <v>110.4988</v>
+      </c>
+      <c r="J103">
+        <v>111.7259</v>
+      </c>
+      <c r="K103">
+        <v>859.02</v>
+      </c>
+      <c r="L103">
+        <v>1101.06</v>
+      </c>
+      <c r="M103">
+        <v>297.88369999999998</v>
+      </c>
+      <c r="N103">
+        <v>289.48</v>
+      </c>
+      <c r="O103">
+        <v>376.39</v>
+      </c>
+      <c r="P103">
+        <v>350.15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B104">
+        <v>8647.5689999999995</v>
+      </c>
+      <c r="C104">
+        <v>8788.17</v>
+      </c>
+      <c r="D104">
+        <v>356.86</v>
+      </c>
+      <c r="E104">
+        <v>4910.83</v>
+      </c>
+      <c r="F104">
+        <v>188.19</v>
+      </c>
+      <c r="G104">
+        <v>121.755</v>
+      </c>
+      <c r="H104">
+        <v>173.94</v>
+      </c>
+      <c r="I104">
+        <v>110.59059999999999</v>
+      </c>
+      <c r="J104">
+        <v>111.7753</v>
+      </c>
+      <c r="K104">
+        <v>859.34</v>
+      </c>
+      <c r="L104">
+        <v>1101.79</v>
+      </c>
+      <c r="M104">
+        <v>298.36360000000002</v>
+      </c>
+      <c r="N104">
+        <v>289.66000000000003</v>
+      </c>
+      <c r="O104">
+        <v>376.78</v>
+      </c>
+      <c r="P104">
+        <v>350.52</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>44334</v>
+      </c>
+      <c r="B105">
+        <v>8574.9779999999992</v>
+      </c>
+      <c r="C105">
+        <v>8784.8799999999992</v>
+      </c>
+      <c r="D105">
+        <v>357.05</v>
+      </c>
+      <c r="E105">
+        <v>4898.68</v>
+      </c>
+      <c r="F105">
+        <v>187.54</v>
+      </c>
+      <c r="G105">
+        <v>121.7811</v>
+      </c>
+      <c r="H105">
+        <v>173.83</v>
+      </c>
+      <c r="I105">
+        <v>110.43089999999999</v>
+      </c>
+      <c r="J105">
+        <v>111.6026</v>
+      </c>
+      <c r="K105">
+        <v>860.53</v>
+      </c>
+      <c r="L105">
+        <v>1098.98</v>
+      </c>
+      <c r="M105">
+        <v>297.73919999999998</v>
+      </c>
+      <c r="N105">
+        <v>289.82</v>
+      </c>
+      <c r="O105">
+        <v>376.65</v>
+      </c>
+      <c r="P105">
+        <v>350.98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>44335</v>
+      </c>
+      <c r="B106">
+        <v>8550.9449999999997</v>
+      </c>
+      <c r="C106">
+        <v>8634.43</v>
+      </c>
+      <c r="D106">
+        <v>355</v>
+      </c>
+      <c r="E106">
+        <v>4877.21</v>
+      </c>
+      <c r="F106">
+        <v>187.1</v>
+      </c>
+      <c r="G106">
+        <v>121.7508</v>
+      </c>
+      <c r="H106">
+        <v>174.02</v>
+      </c>
+      <c r="I106">
+        <v>110.7838</v>
+      </c>
+      <c r="J106">
+        <v>112.0804</v>
+      </c>
+      <c r="K106">
+        <v>860.36</v>
+      </c>
+      <c r="L106">
+        <v>1100.67</v>
+      </c>
+      <c r="M106">
+        <v>297.1465</v>
+      </c>
+      <c r="N106">
+        <v>289.44</v>
+      </c>
+      <c r="O106">
+        <v>376.13</v>
+      </c>
+      <c r="P106">
+        <v>350.41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B107">
+        <v>8641.98</v>
+      </c>
+      <c r="C107">
+        <v>8774.26</v>
+      </c>
+      <c r="D107">
+        <v>358.44</v>
+      </c>
+      <c r="E107">
+        <v>4915.72</v>
+      </c>
+      <c r="F107">
+        <v>189.07</v>
+      </c>
+      <c r="G107">
+        <v>121.85380000000001</v>
+      </c>
+      <c r="H107">
+        <v>174.17</v>
+      </c>
+      <c r="I107">
+        <v>109.98099999999999</v>
+      </c>
+      <c r="J107">
+        <v>110.8154</v>
+      </c>
+      <c r="K107">
+        <v>858.66</v>
+      </c>
+      <c r="L107">
+        <v>1098.52</v>
+      </c>
+      <c r="M107">
+        <v>297.82990000000001</v>
+      </c>
+      <c r="N107">
+        <v>289.14999999999998</v>
+      </c>
+      <c r="O107">
+        <v>375.94</v>
+      </c>
+      <c r="P107">
+        <v>350.08</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>44337</v>
+      </c>
+      <c r="B108">
+        <v>8635.5460000000003</v>
+      </c>
+      <c r="C108">
+        <v>8831.01</v>
+      </c>
+      <c r="D108">
+        <v>358.57</v>
+      </c>
+      <c r="E108">
+        <v>4930.88</v>
+      </c>
+      <c r="F108">
+        <v>189.89</v>
+      </c>
+      <c r="G108">
+        <v>121.7799</v>
+      </c>
+      <c r="H108">
+        <v>174.07</v>
+      </c>
+      <c r="I108">
+        <v>109.8492</v>
+      </c>
+      <c r="J108">
+        <v>110.6514</v>
+      </c>
+      <c r="K108">
+        <v>858.93</v>
+      </c>
+      <c r="L108">
+        <v>1097.6099999999999</v>
+      </c>
+      <c r="M108">
+        <v>297.65839999999997</v>
+      </c>
+      <c r="N108">
+        <v>289.16000000000003</v>
+      </c>
+      <c r="O108">
+        <v>376.09</v>
+      </c>
+      <c r="P108">
+        <v>350.36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B109">
+        <v>8721.9989999999998</v>
+      </c>
+      <c r="C109">
+        <v>8860.27</v>
+      </c>
+      <c r="D109">
+        <v>360.99</v>
+      </c>
+      <c r="E109">
+        <v>4949.04</v>
+      </c>
+      <c r="F109">
+        <v>190.75</v>
+      </c>
+      <c r="G109">
+        <v>121.6478</v>
+      </c>
+      <c r="H109">
+        <v>174.26</v>
+      </c>
+      <c r="I109">
+        <v>109.69110000000001</v>
+      </c>
+      <c r="J109">
+        <v>110.52030000000001</v>
+      </c>
+      <c r="K109">
+        <v>857.68</v>
+      </c>
+      <c r="L109">
+        <v>1097.1300000000001</v>
+      </c>
+      <c r="M109">
+        <v>297.41410000000002</v>
+      </c>
+      <c r="N109">
+        <v>289.20999999999998</v>
+      </c>
+      <c r="O109">
+        <v>375.44</v>
+      </c>
+      <c r="P109">
+        <v>349.98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B110">
+        <v>8703.59</v>
+      </c>
+      <c r="C110">
+        <v>8861.2999999999993</v>
+      </c>
+      <c r="D110">
+        <v>361.56</v>
+      </c>
+      <c r="E110">
+        <v>4987.17</v>
+      </c>
+      <c r="F110">
+        <v>193.17</v>
+      </c>
+      <c r="G110">
+        <v>121.5958</v>
+      </c>
+      <c r="H110">
+        <v>174.24</v>
+      </c>
+      <c r="I110">
+        <v>109.69759999999999</v>
+      </c>
+      <c r="J110">
+        <v>110.5187</v>
+      </c>
+      <c r="K110">
+        <v>858.07</v>
+      </c>
+      <c r="L110">
+        <v>1096.52</v>
+      </c>
+      <c r="M110">
+        <v>297.38499999999999</v>
+      </c>
+      <c r="N110">
+        <v>289.31</v>
+      </c>
+      <c r="O110">
+        <v>375.32</v>
+      </c>
+      <c r="P110">
+        <v>350.15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B111">
+        <v>8720.0390000000007</v>
+      </c>
+      <c r="C111">
+        <v>8851.7000000000007</v>
+      </c>
+      <c r="D111">
+        <v>362.21</v>
+      </c>
+      <c r="E111">
+        <v>4980.7299999999996</v>
+      </c>
+      <c r="F111">
+        <v>192.81</v>
+      </c>
+      <c r="G111">
+        <v>121.3578</v>
+      </c>
+      <c r="H111">
+        <v>174.13</v>
+      </c>
+      <c r="I111">
+        <v>109.6078</v>
+      </c>
+      <c r="J111">
+        <v>110.4577</v>
+      </c>
+      <c r="K111">
+        <v>858.11</v>
+      </c>
+      <c r="L111">
+        <v>1096.71</v>
+      </c>
+      <c r="M111">
+        <v>297.65289999999999</v>
+      </c>
+      <c r="N111">
+        <v>289.39</v>
+      </c>
+      <c r="O111">
+        <v>375.63</v>
+      </c>
+      <c r="P111">
+        <v>350.06</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B112">
+        <v>8730.9680000000008</v>
+      </c>
+      <c r="C112">
+        <v>8868.24</v>
+      </c>
+      <c r="D112">
+        <v>362.45</v>
+      </c>
+      <c r="E112">
+        <v>4964.47</v>
+      </c>
+      <c r="F112">
+        <v>191.73</v>
+      </c>
+      <c r="G112">
+        <v>121.1572</v>
+      </c>
+      <c r="H112">
+        <v>173.95</v>
+      </c>
+      <c r="I112">
+        <v>109.5603</v>
+      </c>
+      <c r="J112">
+        <v>110.3869</v>
+      </c>
+      <c r="K112">
+        <v>858.11</v>
+      </c>
+      <c r="L112">
+        <v>1097.3399999999999</v>
+      </c>
+      <c r="M112">
+        <v>298.15820000000002</v>
+      </c>
+      <c r="N112">
+        <v>289.5</v>
+      </c>
+      <c r="O112">
+        <v>375.82</v>
+      </c>
+      <c r="P112">
+        <v>350.26</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B113">
+        <v>8738.7720000000008</v>
+      </c>
+      <c r="C113">
+        <v>8937.7999999999993</v>
+      </c>
+      <c r="D113">
+        <v>363.62</v>
+      </c>
+      <c r="E113">
+        <v>4980.32</v>
+      </c>
+      <c r="F113">
+        <v>192.76</v>
+      </c>
+      <c r="G113">
+        <v>121.0762</v>
+      </c>
+      <c r="H113">
+        <v>174.13</v>
+      </c>
+      <c r="I113">
+        <v>109.55719999999999</v>
+      </c>
+      <c r="J113">
+        <v>110.3798</v>
+      </c>
+      <c r="K113">
+        <v>858</v>
+      </c>
+      <c r="L113">
+        <v>1095.49</v>
+      </c>
+      <c r="M113">
+        <v>297.73309999999998</v>
+      </c>
+      <c r="N113">
+        <v>289.54000000000002</v>
+      </c>
+      <c r="O113">
+        <v>375.89</v>
+      </c>
+      <c r="P113">
+        <v>350.59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B114">
+        <v>8738.7720000000008</v>
+      </c>
+      <c r="C114">
+        <v>8869.85</v>
+      </c>
+      <c r="D114">
+        <v>363.79</v>
+      </c>
+      <c r="E114">
+        <v>4980.32</v>
+      </c>
+      <c r="F114">
+        <v>192.76</v>
+      </c>
+      <c r="G114">
+        <v>121.0762</v>
+      </c>
+      <c r="H114">
+        <v>174.13</v>
+      </c>
+      <c r="I114">
+        <v>109.55719999999999</v>
+      </c>
+      <c r="J114">
+        <v>110.3798</v>
+      </c>
+      <c r="K114">
+        <v>858</v>
+      </c>
+      <c r="L114">
+        <v>1095.49</v>
+      </c>
+      <c r="M114">
+        <v>297.73309999999998</v>
+      </c>
+      <c r="N114">
+        <v>289.54000000000002</v>
+      </c>
+      <c r="O114">
+        <v>375.89</v>
+      </c>
+      <c r="P114">
+        <v>350.59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B115">
+        <v>8734.7440000000006</v>
+      </c>
+      <c r="C115">
+        <v>8940.76</v>
+      </c>
+      <c r="D115">
+        <v>364.97</v>
+      </c>
+      <c r="E115">
+        <v>4962.33</v>
+      </c>
+      <c r="F115">
+        <v>191.29</v>
+      </c>
+      <c r="G115">
+        <v>121.2259</v>
+      </c>
+      <c r="H115">
+        <v>174.33</v>
+      </c>
+      <c r="I115">
+        <v>109.569</v>
+      </c>
+      <c r="J115">
+        <v>110.3884</v>
+      </c>
+      <c r="K115">
+        <v>858.07</v>
+      </c>
+      <c r="L115">
+        <v>1096.01</v>
+      </c>
+      <c r="M115">
+        <v>297.89109999999999</v>
+      </c>
+      <c r="N115">
+        <v>290.05</v>
+      </c>
+      <c r="O115">
+        <v>376.09</v>
+      </c>
+      <c r="P115">
+        <v>351.06</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B116">
+        <v>8748.2970000000005</v>
+      </c>
+      <c r="C116">
+        <v>8978.9</v>
+      </c>
+      <c r="D116">
+        <v>365.34</v>
+      </c>
+      <c r="E116">
+        <v>4972.57</v>
+      </c>
+      <c r="F116">
+        <v>191.72</v>
+      </c>
+      <c r="G116">
+        <v>121.3348</v>
+      </c>
+      <c r="H116">
+        <v>174.39</v>
+      </c>
+      <c r="I116">
+        <v>109.5534</v>
+      </c>
+      <c r="J116">
+        <v>110.3857</v>
+      </c>
+      <c r="K116">
+        <v>857.95</v>
+      </c>
+      <c r="L116">
+        <v>1096.53</v>
+      </c>
+      <c r="M116">
+        <v>297.83429999999998</v>
+      </c>
+      <c r="N116">
+        <v>290.44</v>
+      </c>
+      <c r="O116">
+        <v>376.63</v>
+      </c>
+      <c r="P116">
+        <v>351.13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B117">
+        <v>8717.973</v>
+      </c>
+      <c r="C117">
+        <v>8958.57</v>
+      </c>
+      <c r="D117">
+        <v>363.82</v>
+      </c>
+      <c r="E117">
+        <v>4954.05</v>
+      </c>
+      <c r="F117">
+        <v>190.93</v>
+      </c>
+      <c r="G117">
+        <v>121.4174</v>
+      </c>
+      <c r="H117">
+        <v>174.34</v>
+      </c>
+      <c r="I117">
+        <v>109.5641</v>
+      </c>
+      <c r="J117">
+        <v>110.3939</v>
+      </c>
+      <c r="K117">
+        <v>858.45</v>
+      </c>
+      <c r="L117">
+        <v>1097.44</v>
+      </c>
+      <c r="M117">
+        <v>297.91300000000001</v>
+      </c>
+      <c r="N117">
+        <v>290.56</v>
+      </c>
+      <c r="O117">
+        <v>376.64</v>
+      </c>
+      <c r="P117">
+        <v>350.66</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B118">
+        <v>8795.0759999999991</v>
+      </c>
+      <c r="C118">
+        <v>8980.83</v>
+      </c>
+      <c r="D118">
+        <v>366.36</v>
+      </c>
+      <c r="E118">
+        <v>5005.07</v>
+      </c>
+      <c r="F118">
+        <v>194.28</v>
+      </c>
+      <c r="G118">
+        <v>121.4074</v>
+      </c>
+      <c r="H118">
+        <v>174.29</v>
+      </c>
+      <c r="I118">
+        <v>109.4988</v>
+      </c>
+      <c r="J118">
+        <v>110.3267</v>
+      </c>
+      <c r="K118">
+        <v>857.22</v>
+      </c>
+      <c r="L118">
+        <v>1097.53</v>
+      </c>
+      <c r="M118">
+        <v>298.18759999999997</v>
+      </c>
+      <c r="N118">
+        <v>290.17</v>
+      </c>
+      <c r="O118">
+        <v>376.44</v>
+      </c>
+      <c r="P118">
+        <v>350.78</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B119">
+        <v>8788.2790000000005</v>
+      </c>
+      <c r="C119">
+        <v>8998.99</v>
+      </c>
+      <c r="D119">
+        <v>366.72</v>
+      </c>
+      <c r="E119">
+        <v>4995.88</v>
+      </c>
+      <c r="F119">
+        <v>193.56</v>
+      </c>
+      <c r="G119">
+        <v>121.2696</v>
+      </c>
+      <c r="H119">
+        <v>174.23</v>
+      </c>
+      <c r="I119">
+        <v>109.4913</v>
+      </c>
+      <c r="J119">
+        <v>110.3229</v>
+      </c>
+      <c r="K119">
+        <v>857.45</v>
+      </c>
+      <c r="L119">
+        <v>1098.03</v>
+      </c>
+      <c r="M119">
+        <v>298.00740000000002</v>
+      </c>
+      <c r="N119">
+        <v>290.29000000000002</v>
+      </c>
+      <c r="O119">
+        <v>376.72</v>
+      </c>
+      <c r="P119">
+        <v>351.12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B120">
+        <v>8789.9959999999992</v>
+      </c>
+      <c r="C120">
+        <v>8995.39</v>
+      </c>
+      <c r="D120">
+        <v>366.72</v>
+      </c>
+      <c r="E120">
+        <v>5021.16</v>
+      </c>
+      <c r="F120">
+        <v>195.21</v>
+      </c>
+      <c r="G120">
+        <v>121.18899999999999</v>
+      </c>
+      <c r="H120">
+        <v>174.22</v>
+      </c>
+      <c r="I120">
+        <v>109.4873</v>
+      </c>
+      <c r="J120">
+        <v>110.31440000000001</v>
+      </c>
+      <c r="K120">
+        <v>857.39</v>
+      </c>
+      <c r="L120">
+        <v>1096.71</v>
+      </c>
+      <c r="M120">
+        <v>297.86680000000001</v>
+      </c>
+      <c r="N120">
+        <v>290.41000000000003</v>
+      </c>
+      <c r="O120">
+        <v>376.61</v>
+      </c>
+      <c r="P120">
+        <v>351.48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B121">
+        <v>8774.3130000000001</v>
+      </c>
+      <c r="C121">
+        <v>8997.23</v>
+      </c>
+      <c r="D121">
+        <v>366.02</v>
+      </c>
+      <c r="E121">
+        <v>5056.16</v>
+      </c>
+      <c r="F121">
+        <v>197.47</v>
+      </c>
+      <c r="G121">
+        <v>121.2273</v>
+      </c>
+      <c r="H121">
+        <v>174.27</v>
+      </c>
+      <c r="I121">
+        <v>109.4979</v>
+      </c>
+      <c r="J121">
+        <v>110.3231</v>
+      </c>
+      <c r="K121">
+        <v>857.58</v>
+      </c>
+      <c r="L121">
+        <v>1094.82</v>
+      </c>
+      <c r="M121">
+        <v>297.88560000000001</v>
+      </c>
+      <c r="N121">
+        <v>290.51</v>
+      </c>
+      <c r="O121">
+        <v>376.62</v>
+      </c>
+      <c r="P121">
+        <v>351.98</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A122" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B122">
+        <v>8815.5619999999999</v>
+      </c>
+      <c r="C122">
+        <v>8995.5400000000009</v>
+      </c>
+      <c r="D122">
+        <v>367.39</v>
+      </c>
+      <c r="E122">
+        <v>5089.83</v>
+      </c>
+      <c r="F122">
+        <v>198.91</v>
+      </c>
+      <c r="G122">
+        <v>120.8612</v>
+      </c>
+      <c r="H122">
+        <v>174.16</v>
+      </c>
+      <c r="I122">
+        <v>109.4508</v>
+      </c>
+      <c r="J122">
+        <v>110.28530000000001</v>
+      </c>
+      <c r="K122">
+        <v>857.03</v>
+      </c>
+      <c r="L122">
+        <v>1097.26</v>
+      </c>
+      <c r="M122">
+        <v>297.91680000000002</v>
+      </c>
+      <c r="N122">
+        <v>290.64</v>
+      </c>
+      <c r="O122">
+        <v>377.04</v>
+      </c>
+      <c r="P122">
+        <v>352.6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B123">
+        <v>8832.9439999999995</v>
+      </c>
+      <c r="C123">
+        <v>9062.7900000000009</v>
+      </c>
+      <c r="D123">
+        <v>368.07</v>
+      </c>
+      <c r="E123">
+        <v>5090.16</v>
+      </c>
+      <c r="F123">
+        <v>198.55</v>
+      </c>
+      <c r="G123">
+        <v>120.8047</v>
+      </c>
+      <c r="H123">
+        <v>174.07</v>
+      </c>
+      <c r="I123">
+        <v>109.4336</v>
+      </c>
+      <c r="J123">
+        <v>110.2634</v>
+      </c>
+      <c r="K123">
+        <v>856.77</v>
+      </c>
+      <c r="L123">
+        <v>1094.74</v>
+      </c>
+      <c r="M123">
+        <v>297.88080000000002</v>
+      </c>
+      <c r="N123">
+        <v>290.64</v>
+      </c>
+      <c r="O123">
+        <v>377.16</v>
+      </c>
+      <c r="P123">
+        <v>352.93</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B124">
+        <v>8851.1659999999993</v>
+      </c>
+      <c r="C124">
+        <v>9075.9</v>
+      </c>
+      <c r="D124">
+        <v>368.91</v>
+      </c>
+      <c r="E124">
+        <v>5064.68</v>
+      </c>
+      <c r="F124">
+        <v>196.58</v>
+      </c>
+      <c r="G124">
+        <v>120.96639999999999</v>
+      </c>
+      <c r="H124">
+        <v>174.22</v>
+      </c>
+      <c r="I124">
+        <v>109.4378</v>
+      </c>
+      <c r="J124">
+        <v>110.26690000000001</v>
+      </c>
+      <c r="K124">
+        <v>856.52</v>
+      </c>
+      <c r="L124">
+        <v>1095.46</v>
+      </c>
+      <c r="M124">
+        <v>297.6934</v>
+      </c>
+      <c r="N124">
+        <v>290.77</v>
+      </c>
+      <c r="O124">
+        <v>377.35</v>
+      </c>
+      <c r="P124">
+        <v>353.25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B125">
+        <v>8833.6749999999993</v>
+      </c>
+      <c r="C125">
+        <v>9099.74</v>
+      </c>
+      <c r="D125">
+        <v>368.48</v>
+      </c>
+      <c r="E125">
+        <v>5065.03</v>
+      </c>
+      <c r="F125">
+        <v>196.25</v>
+      </c>
+      <c r="G125">
+        <v>121.0968</v>
+      </c>
+      <c r="H125">
+        <v>174.21</v>
+      </c>
+      <c r="I125">
+        <v>109.4452</v>
+      </c>
+      <c r="J125">
+        <v>110.26819999999999</v>
+      </c>
+      <c r="K125">
+        <v>856.79</v>
+      </c>
+      <c r="L125">
+        <v>1094.92</v>
+      </c>
+      <c r="M125">
+        <v>297.74520000000001</v>
+      </c>
+      <c r="N125">
+        <v>290.72000000000003</v>
+      </c>
+      <c r="O125">
+        <v>376.99</v>
+      </c>
+      <c r="P125">
+        <v>353.39</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B126">
+        <v>8786.1779999999999</v>
+      </c>
+      <c r="C126">
+        <v>9117.82</v>
+      </c>
+      <c r="D126">
+        <v>367.26</v>
+      </c>
+      <c r="E126">
+        <v>5062.07</v>
+      </c>
+      <c r="F126">
+        <v>196.47</v>
+      </c>
+      <c r="G126">
+        <v>120.8896</v>
+      </c>
+      <c r="H126">
+        <v>173.9</v>
+      </c>
+      <c r="I126">
+        <v>109.4374</v>
+      </c>
+      <c r="J126">
+        <v>110.2713</v>
+      </c>
+      <c r="K126">
+        <v>857.61</v>
+      </c>
+      <c r="L126">
+        <v>1093.8399999999999</v>
+      </c>
+      <c r="M126">
+        <v>297.60570000000001</v>
+      </c>
+      <c r="N126">
+        <v>290.58</v>
+      </c>
+      <c r="O126">
+        <v>376.67</v>
+      </c>
+      <c r="P126">
+        <v>354.19</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B127">
+        <v>8782.5840000000007</v>
+      </c>
+      <c r="C127">
+        <v>9131.83</v>
+      </c>
+      <c r="D127">
+        <v>365.77</v>
+      </c>
+      <c r="E127">
+        <v>5120.5600000000004</v>
+      </c>
+      <c r="F127">
+        <v>200.35</v>
+      </c>
+      <c r="G127">
+        <v>120.6842</v>
+      </c>
+      <c r="H127">
+        <v>174</v>
+      </c>
+      <c r="I127">
+        <v>109.43940000000001</v>
+      </c>
+      <c r="J127">
+        <v>110.2629</v>
+      </c>
+      <c r="K127">
+        <v>857.71</v>
+      </c>
+      <c r="L127">
+        <v>1097.43</v>
+      </c>
+      <c r="M127">
+        <v>297.6737</v>
+      </c>
+      <c r="N127">
+        <v>291.77</v>
+      </c>
+      <c r="O127">
+        <v>377.93</v>
+      </c>
+      <c r="P127">
+        <v>354.81</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B128">
+        <v>8667.7630000000008</v>
+      </c>
+      <c r="C128">
+        <v>8967.6299999999992</v>
+      </c>
+      <c r="D128">
+        <v>361.22</v>
+      </c>
+      <c r="E128">
+        <v>5182.59</v>
+      </c>
+      <c r="F128">
+        <v>205.38</v>
+      </c>
+      <c r="G128">
+        <v>120.7809</v>
+      </c>
+      <c r="H128">
+        <v>173.7</v>
+      </c>
+      <c r="I128">
+        <v>109.5359</v>
+      </c>
+      <c r="J128">
+        <v>110.3416</v>
+      </c>
+      <c r="K128">
+        <v>859.86</v>
+      </c>
+      <c r="L128">
+        <v>1095.44</v>
+      </c>
+      <c r="M128">
+        <v>297.8621</v>
+      </c>
+      <c r="N128">
+        <v>292.04000000000002</v>
+      </c>
+      <c r="O128">
+        <v>377.68</v>
+      </c>
+      <c r="P128">
+        <v>353.96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B129">
+        <v>8789.5220000000008</v>
+      </c>
+      <c r="C129">
+        <v>9031.24</v>
+      </c>
+      <c r="D129">
+        <v>363.84</v>
+      </c>
+      <c r="E129">
+        <v>5124.8900000000003</v>
+      </c>
+      <c r="F129">
+        <v>200.95</v>
+      </c>
+      <c r="G129">
+        <v>120.7722</v>
+      </c>
+      <c r="H129">
+        <v>174.1</v>
+      </c>
+      <c r="I129">
+        <v>109.35899999999999</v>
+      </c>
+      <c r="J129">
+        <v>110.2222</v>
+      </c>
+      <c r="K129">
+        <v>857.37</v>
+      </c>
+      <c r="L129">
+        <v>1094.6600000000001</v>
+      </c>
+      <c r="M129">
+        <v>298.83780000000002</v>
+      </c>
+      <c r="N129">
+        <v>292.36</v>
+      </c>
+      <c r="O129">
+        <v>376.93</v>
+      </c>
+      <c r="P129">
+        <v>354.33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A130" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B130">
+        <v>8834.5580000000009</v>
+      </c>
+      <c r="C130">
+        <v>9054.94</v>
+      </c>
+      <c r="D130">
+        <v>365.73</v>
+      </c>
+      <c r="E130">
+        <v>5129.8100000000004</v>
+      </c>
+      <c r="F130">
+        <v>201.32</v>
+      </c>
+      <c r="G130">
+        <v>120.7295</v>
+      </c>
+      <c r="H130">
+        <v>174.09</v>
+      </c>
+      <c r="I130">
+        <v>109.277</v>
+      </c>
+      <c r="J130">
+        <v>110.14749999999999</v>
+      </c>
+      <c r="K130">
+        <v>856.55</v>
+      </c>
+      <c r="L130">
+        <v>1095.07</v>
+      </c>
+      <c r="M130">
+        <v>297.66680000000002</v>
+      </c>
+      <c r="N130">
+        <v>292.5</v>
+      </c>
+      <c r="O130">
+        <v>377.04</v>
+      </c>
+      <c r="P130">
+        <v>354.28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>44370</v>
+      </c>
+      <c r="B131">
+        <v>8825.0139999999992</v>
+      </c>
+      <c r="C131">
+        <v>8952.2999999999993</v>
+      </c>
+      <c r="D131">
+        <v>365.88</v>
+      </c>
+      <c r="E131">
+        <v>5118.3500000000004</v>
+      </c>
+      <c r="F131">
+        <v>200.76</v>
+      </c>
+      <c r="G131">
+        <v>120.5309</v>
+      </c>
+      <c r="H131">
+        <v>173.9</v>
+      </c>
+      <c r="I131">
+        <v>109.2426</v>
+      </c>
+      <c r="J131">
+        <v>110.0603</v>
+      </c>
+      <c r="K131">
+        <v>856.76</v>
+      </c>
+      <c r="L131">
+        <v>1095.1099999999999</v>
+      </c>
+      <c r="M131">
+        <v>297.6533</v>
+      </c>
+      <c r="N131">
+        <v>292.60000000000002</v>
+      </c>
+      <c r="O131">
+        <v>377.24</v>
+      </c>
+      <c r="P131">
+        <v>354.32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A132" s="1">
+        <v>44371</v>
+      </c>
+      <c r="B132">
+        <v>8877.0650000000005</v>
+      </c>
+      <c r="C132">
+        <v>9058.2800000000007</v>
+      </c>
+      <c r="D132">
+        <v>367.81</v>
+      </c>
+      <c r="E132">
+        <v>5126.43</v>
+      </c>
+      <c r="F132">
+        <v>201.16</v>
+      </c>
+      <c r="G132">
+        <v>120.6216</v>
+      </c>
+      <c r="H132">
+        <v>173.97</v>
+      </c>
+      <c r="I132">
+        <v>109.22929999999999</v>
+      </c>
+      <c r="J132">
+        <v>110.0475</v>
+      </c>
+      <c r="K132">
+        <v>855.92</v>
+      </c>
+      <c r="L132">
+        <v>1095.82</v>
+      </c>
+      <c r="M132">
+        <v>297.42090000000002</v>
+      </c>
+      <c r="N132">
+        <v>292.52</v>
+      </c>
+      <c r="O132">
+        <v>377.25</v>
+      </c>
+      <c r="P132">
+        <v>354.26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>44372</v>
+      </c>
+      <c r="B133">
+        <v>8906.7909999999993</v>
+      </c>
+      <c r="C133">
+        <v>9054.4</v>
+      </c>
+      <c r="D133">
+        <v>369.47</v>
+      </c>
+      <c r="E133">
+        <v>5100.28</v>
+      </c>
+      <c r="F133">
+        <v>198.5</v>
+      </c>
+      <c r="G133">
+        <v>120.6726</v>
+      </c>
+      <c r="H133">
+        <v>174.14</v>
+      </c>
+      <c r="I133">
+        <v>109.22320000000001</v>
+      </c>
+      <c r="J133">
+        <v>110.04510000000001</v>
+      </c>
+      <c r="K133">
+        <v>855.39</v>
+      </c>
+      <c r="L133">
+        <v>1096.45</v>
+      </c>
+      <c r="M133">
+        <v>297.25790000000001</v>
+      </c>
+      <c r="N133">
+        <v>292.41000000000003</v>
+      </c>
+      <c r="O133">
+        <v>377.13</v>
+      </c>
+      <c r="P133">
+        <v>354.19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A134" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B134">
+        <v>8927.4009999999998</v>
+      </c>
+      <c r="C134">
+        <v>8986.83</v>
+      </c>
+      <c r="D134">
+        <v>369.56</v>
+      </c>
+      <c r="E134">
+        <v>5141.03</v>
+      </c>
+      <c r="F134">
+        <v>201.1</v>
+      </c>
+      <c r="G134">
+        <v>120.7411</v>
+      </c>
+      <c r="H134">
+        <v>174.18</v>
+      </c>
+      <c r="I134">
+        <v>109.22329999999999</v>
+      </c>
+      <c r="J134">
+        <v>110.0395</v>
+      </c>
+      <c r="K134">
+        <v>855.09</v>
+      </c>
+      <c r="L134">
+        <v>1098.97</v>
+      </c>
+      <c r="M134">
+        <v>297.2448</v>
+      </c>
+      <c r="N134">
+        <v>292.56</v>
+      </c>
+      <c r="O134">
+        <v>377.21</v>
+      </c>
+      <c r="P134">
+        <v>354.35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A135" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B135">
+        <v>8930.6659999999993</v>
+      </c>
+      <c r="C135">
+        <v>9025.51</v>
+      </c>
+      <c r="D135">
+        <v>369.41</v>
+      </c>
+      <c r="E135">
+        <v>5150.9799999999996</v>
+      </c>
+      <c r="F135">
+        <v>201.57</v>
+      </c>
+      <c r="G135">
+        <v>120.8948</v>
+      </c>
+      <c r="H135">
+        <v>174.27</v>
+      </c>
+      <c r="I135">
+        <v>109.2261</v>
+      </c>
+      <c r="J135">
+        <v>110.0406</v>
+      </c>
+      <c r="K135">
+        <v>854.97</v>
+      </c>
+      <c r="L135">
+        <v>1097.0999999999999</v>
+      </c>
+      <c r="M135">
+        <v>297.42020000000002</v>
+      </c>
+      <c r="N135">
+        <v>292.8</v>
+      </c>
+      <c r="O135">
+        <v>377.37</v>
+      </c>
+      <c r="P135">
+        <v>354.57</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A136" s="1">
+        <v>44377</v>
+      </c>
+      <c r="B136">
+        <v>8942.777</v>
+      </c>
+      <c r="C136">
+        <v>8930.5499999999993</v>
+      </c>
+      <c r="D136">
+        <v>368.58</v>
+      </c>
+      <c r="E136">
+        <v>5164.47</v>
+      </c>
+      <c r="F136">
+        <v>202.74</v>
+      </c>
+      <c r="G136">
+        <v>120.9892</v>
+      </c>
+      <c r="H136">
+        <v>174.23</v>
+      </c>
+      <c r="I136">
+        <v>109.2259</v>
+      </c>
+      <c r="J136">
+        <v>110.04510000000001</v>
+      </c>
+      <c r="K136">
+        <v>854.8</v>
+      </c>
+      <c r="L136">
+        <v>1097.47</v>
+      </c>
+      <c r="M136">
+        <v>297.43029999999999</v>
+      </c>
+      <c r="N136">
+        <v>292.83999999999997</v>
+      </c>
+      <c r="O136">
+        <v>377.74</v>
+      </c>
+      <c r="P136">
+        <v>354.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update returns data for 3/31/2022
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE47546-223A-48FF-9363-919DF6B45038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC76ACA-EF7B-4CFE-988D-1B767EE7594C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="24">
   <si>
     <t>SPTR Index</t>
   </si>
@@ -572,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,10 +597,9 @@
     <col min="15" max="15" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -649,11 +648,8 @@
       <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -705,11 +701,8 @@
       <c r="Q2">
         <v>345.76</v>
       </c>
-      <c r="R2">
-        <v>169.35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44564</v>
       </c>
@@ -761,11 +754,8 @@
       <c r="Q3">
         <v>345.74</v>
       </c>
-      <c r="R3">
-        <v>169.51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44565</v>
       </c>
@@ -817,11 +807,8 @@
       <c r="Q4">
         <v>345.97</v>
       </c>
-      <c r="R4">
-        <v>169.61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44566</v>
       </c>
@@ -873,11 +860,8 @@
       <c r="Q5">
         <v>345.31</v>
       </c>
-      <c r="R5">
-        <v>169.42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44567</v>
       </c>
@@ -929,11 +913,8 @@
       <c r="Q6">
         <v>345.61</v>
       </c>
-      <c r="R6">
-        <v>169.39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44568</v>
       </c>
@@ -985,11 +966,8 @@
       <c r="Q7">
         <v>346.13</v>
       </c>
-      <c r="R7">
-        <v>169.88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44571</v>
       </c>
@@ -1041,11 +1019,8 @@
       <c r="Q8">
         <v>344.15</v>
       </c>
-      <c r="R8">
-        <v>169.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44572</v>
       </c>
@@ -1097,11 +1072,8 @@
       <c r="Q9">
         <v>344.14</v>
       </c>
-      <c r="R9">
-        <v>169.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44573</v>
       </c>
@@ -1153,11 +1125,8 @@
       <c r="Q10">
         <v>344.4</v>
       </c>
-      <c r="R10">
-        <v>169.18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44574</v>
       </c>
@@ -1209,11 +1178,8 @@
       <c r="Q11">
         <v>343.42</v>
       </c>
-      <c r="R11">
-        <v>168.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44575</v>
       </c>
@@ -1265,11 +1231,8 @@
       <c r="Q12">
         <v>344</v>
       </c>
-      <c r="R12">
-        <v>168.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44578</v>
       </c>
@@ -1321,11 +1284,8 @@
       <c r="Q13">
         <v>344</v>
       </c>
-      <c r="R13">
-        <v>168.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44579</v>
       </c>
@@ -1377,11 +1337,8 @@
       <c r="Q14">
         <v>344.06</v>
       </c>
-      <c r="R14">
-        <v>168.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44580</v>
       </c>
@@ -1433,11 +1390,8 @@
       <c r="Q15">
         <v>344.56</v>
       </c>
-      <c r="R15">
-        <v>168.89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44581</v>
       </c>
@@ -1489,11 +1443,8 @@
       <c r="Q16">
         <v>342.93</v>
       </c>
-      <c r="R16">
-        <v>168.22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44582</v>
       </c>
@@ -1545,11 +1496,8 @@
       <c r="Q17">
         <v>342.28</v>
       </c>
-      <c r="R17">
-        <v>169.02</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44585</v>
       </c>
@@ -1601,11 +1549,8 @@
       <c r="Q18">
         <v>336.97</v>
       </c>
-      <c r="R18">
-        <v>167.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44586</v>
       </c>
@@ -1657,11 +1602,8 @@
       <c r="Q19">
         <v>336.78</v>
       </c>
-      <c r="R19">
-        <v>168.63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44587</v>
       </c>
@@ -1713,11 +1655,8 @@
       <c r="Q20">
         <v>336.33</v>
       </c>
-      <c r="R20">
-        <v>167.99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44588</v>
       </c>
@@ -1769,11 +1708,8 @@
       <c r="Q21">
         <v>335.37</v>
       </c>
-      <c r="R21">
-        <v>167.78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44589</v>
       </c>
@@ -1825,11 +1761,8 @@
       <c r="Q22">
         <v>335.16</v>
       </c>
-      <c r="R22">
-        <v>167.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44592</v>
       </c>
@@ -1881,11 +1814,8 @@
       <c r="Q23">
         <v>335.19</v>
       </c>
-      <c r="R23">
-        <v>167.58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44593</v>
       </c>
@@ -1937,11 +1867,8 @@
       <c r="Q24">
         <v>335.02</v>
       </c>
-      <c r="R24">
-        <v>168.11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>44594</v>
       </c>
@@ -1993,11 +1920,8 @@
       <c r="Q25">
         <v>334.88</v>
       </c>
-      <c r="R25">
-        <v>168.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44595</v>
       </c>
@@ -2049,11 +1973,8 @@
       <c r="Q26">
         <v>334.57</v>
       </c>
-      <c r="R26">
-        <v>169.55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44596</v>
       </c>
@@ -2105,11 +2026,8 @@
       <c r="Q27">
         <v>334.95</v>
       </c>
-      <c r="R27">
-        <v>170.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44599</v>
       </c>
@@ -2161,11 +2079,8 @@
       <c r="Q28">
         <v>335.25</v>
       </c>
-      <c r="R28">
-        <v>170.08</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>44600</v>
       </c>
@@ -2217,11 +2132,8 @@
       <c r="Q29">
         <v>335.29</v>
       </c>
-      <c r="R29">
-        <v>170.24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44601</v>
       </c>
@@ -2273,11 +2185,8 @@
       <c r="Q30">
         <v>335.12</v>
       </c>
-      <c r="R30">
-        <v>169.75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>44602</v>
       </c>
@@ -2329,11 +2238,8 @@
       <c r="Q31">
         <v>333.89</v>
       </c>
-      <c r="R31">
-        <v>169.37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44603</v>
       </c>
@@ -2385,11 +2291,8 @@
       <c r="Q32">
         <v>332.95</v>
       </c>
-      <c r="R32">
-        <v>169.66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>44606</v>
       </c>
@@ -2441,11 +2344,8 @@
       <c r="Q33">
         <v>334.73</v>
       </c>
-      <c r="R33">
-        <v>169.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>44607</v>
       </c>
@@ -2497,11 +2397,8 @@
       <c r="Q34">
         <v>334.79</v>
       </c>
-      <c r="R34">
-        <v>169.34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>44608</v>
       </c>
@@ -2553,11 +2450,8 @@
       <c r="Q35">
         <v>335.14</v>
       </c>
-      <c r="R35">
-        <v>169.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>44609</v>
       </c>
@@ -2609,11 +2503,8 @@
       <c r="Q36">
         <v>333.61</v>
       </c>
-      <c r="R36">
-        <v>169.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>44610</v>
       </c>
@@ -2665,11 +2556,8 @@
       <c r="Q37">
         <v>334.47</v>
       </c>
-      <c r="R37">
-        <v>169.57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>44613</v>
       </c>
@@ -2721,11 +2609,8 @@
       <c r="Q38">
         <v>334.47</v>
       </c>
-      <c r="R38">
-        <v>169.57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>44614</v>
       </c>
@@ -2777,11 +2662,8 @@
       <c r="Q39">
         <v>335.34</v>
       </c>
-      <c r="R39">
-        <v>169.46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>44615</v>
       </c>
@@ -2833,11 +2715,8 @@
       <c r="Q40">
         <v>335.7</v>
       </c>
-      <c r="R40">
-        <v>169.49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>44616</v>
       </c>
@@ -2889,11 +2768,8 @@
       <c r="Q41">
         <v>333.65</v>
       </c>
-      <c r="R41">
-        <v>169.62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>44617</v>
       </c>
@@ -2945,11 +2821,8 @@
       <c r="Q42">
         <v>333.72</v>
       </c>
-      <c r="R42">
-        <v>168.76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>44620</v>
       </c>
@@ -3001,11 +2874,8 @@
       <c r="Q43">
         <v>333.6</v>
       </c>
-      <c r="R43">
-        <v>169.08</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>44621</v>
       </c>
@@ -3057,11 +2927,8 @@
       <c r="Q44">
         <v>334.46</v>
       </c>
-      <c r="R44">
-        <v>169.24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44622</v>
       </c>
@@ -3113,11 +2980,8 @@
       <c r="Q45">
         <v>334.56</v>
       </c>
-      <c r="R45">
-        <v>168.87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44623</v>
       </c>
@@ -3169,11 +3033,8 @@
       <c r="Q46">
         <v>334.48</v>
       </c>
-      <c r="R46">
-        <v>168.96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>44624</v>
       </c>
@@ -3225,11 +3086,8 @@
       <c r="Q47">
         <v>334.44</v>
       </c>
-      <c r="R47">
-        <v>169.59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>44627</v>
       </c>
@@ -3281,11 +3139,8 @@
       <c r="Q48">
         <v>335.25</v>
       </c>
-      <c r="R48">
-        <v>170.11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>44628</v>
       </c>
@@ -3337,11 +3192,8 @@
       <c r="Q49">
         <v>334.99</v>
       </c>
-      <c r="R49">
-        <v>169.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>44629</v>
       </c>
@@ -3393,11 +3245,8 @@
       <c r="Q50">
         <v>334.52</v>
       </c>
-      <c r="R50">
-        <v>169.43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>44630</v>
       </c>
@@ -3449,11 +3298,8 @@
       <c r="Q51">
         <v>334.43</v>
       </c>
-      <c r="R51">
-        <v>169.63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>44631</v>
       </c>
@@ -3505,11 +3351,8 @@
       <c r="Q52">
         <v>334.54</v>
       </c>
-      <c r="R52">
-        <v>169.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>44634</v>
       </c>
@@ -3561,11 +3404,8 @@
       <c r="Q53">
         <v>335.28</v>
       </c>
-      <c r="R53">
-        <v>169.74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>44635</v>
       </c>
@@ -3617,11 +3457,8 @@
       <c r="Q54">
         <v>335.41</v>
       </c>
-      <c r="R54">
-        <v>169.67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>44636</v>
       </c>
@@ -3673,11 +3510,8 @@
       <c r="Q55">
         <v>334.35</v>
       </c>
-      <c r="R55">
-        <v>169.36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44637</v>
       </c>
@@ -3729,11 +3563,8 @@
       <c r="Q56">
         <v>334.36</v>
       </c>
-      <c r="R56">
-        <v>168.89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44638</v>
       </c>
@@ -3785,11 +3616,8 @@
       <c r="Q57">
         <v>334.57</v>
       </c>
-      <c r="R57">
-        <v>169.05</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44641</v>
       </c>
@@ -3841,11 +3669,8 @@
       <c r="Q58">
         <v>335.14</v>
       </c>
-      <c r="R58">
-        <v>169.12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44642</v>
       </c>
@@ -3897,11 +3722,8 @@
       <c r="Q59">
         <v>335.13</v>
       </c>
-      <c r="R59">
-        <v>168.97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44643</v>
       </c>
@@ -3953,11 +3775,8 @@
       <c r="Q60">
         <v>335.09</v>
       </c>
-      <c r="R60">
-        <v>169.26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44644</v>
       </c>
@@ -4009,11 +3828,8 @@
       <c r="Q61">
         <v>334.95</v>
       </c>
-      <c r="R61">
-        <v>169.46</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44645</v>
       </c>
@@ -4065,11 +3881,8 @@
       <c r="Q62">
         <v>335.35</v>
       </c>
-      <c r="R62">
-        <v>169.54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44648</v>
       </c>
@@ -4121,11 +3934,8 @@
       <c r="Q63">
         <v>335.43</v>
       </c>
-      <c r="R63">
-        <v>169.76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44649</v>
       </c>
@@ -4177,11 +3987,8 @@
       <c r="Q64">
         <v>335.16</v>
       </c>
-      <c r="R64">
-        <v>169.21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44650</v>
       </c>
@@ -4233,11 +4040,8 @@
       <c r="Q65">
         <v>335.28</v>
       </c>
-      <c r="R65">
-        <v>169.39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44651</v>
       </c>
@@ -4288,9 +4092,6 @@
       </c>
       <c r="Q66">
         <v>334.28</v>
-      </c>
-      <c r="R66">
-        <v>169.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ups_data for June 2022
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\RMP\EquityHedging\data\update_strats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E0939DA-E5C9-4493-9B2A-5718BCB7E4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -25,8 +24,9 @@
     <definedName name="SpreadsheetBuilder_2" hidden="1">#REF!</definedName>
     <definedName name="SpreadsheetBuilder_3" localSheetId="3" hidden="1">data_original!$A$1:$Q$1</definedName>
     <definedName name="SpreadsheetBuilder_3" hidden="1">data!$A$1:$Q$1</definedName>
+    <definedName name="SpreadsheetBuilder_4" hidden="1">bbg!$A$1:$R$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,102 +177,84 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...2498000376</v>
         <stp/>
-        <stp>BDH|14373309094453461515</stp>
+        <stp>BDH|13443209491875865478</stp>
+        <tr r="O7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...4292474235</v>
+        <stp/>
+        <stp>BDH|17104415084249048216</stp>
+        <tr r="C7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3114597649</v>
+        <stp/>
+        <stp>BDH|10780736232050436488</stp>
+        <tr r="H7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3312458933</v>
+        <stp/>
+        <stp>BDH|11392435143047097029</stp>
+        <tr r="J7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3684680868</v>
+        <stp/>
+        <stp>BDH|13681390364586674687</stp>
+        <tr r="R7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3902279735</v>
+        <stp/>
+        <stp>BDH|12813523539692123174</stp>
         <tr r="N7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...2648455992</v>
         <stp/>
-        <stp>BDH|15254198816498138559</stp>
-        <tr r="K7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12376458535329946451</stp>
+        <stp>BDH|10651658260607967001</stp>
         <tr r="E7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...4262317047</v>
         <stp/>
-        <stp>BDH|14047895025460654716</stp>
-        <tr r="I7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15219073193266403418</stp>
-        <tr r="O7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17676840938570904020</stp>
-        <tr r="D7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17737690590601603895</stp>
-        <tr r="P7" s="4"/>
+        <stp>BDH|16172402952033261032</stp>
+        <tr r="F7" s="4"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...4166306348</v>
         <stp/>
-        <stp>BDH|4440947643953867604</stp>
-        <tr r="J7" s="4"/>
+        <stp>BDH|7372156945517956837</stp>
+        <tr r="I7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...2793532776</v>
         <stp/>
-        <stp>BDH|8374361155286374440</stp>
-        <tr r="H7" s="4"/>
+        <stp>BDH|4044657110195260995</stp>
+        <tr r="K7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3867305555</v>
         <stp/>
-        <stp>BDH|8741188097968377687</stp>
-        <tr r="R7" s="4"/>
+        <stp>BDH|7247267998221805998</stp>
+        <tr r="P7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...2967649377</v>
         <stp/>
-        <stp>BDH|7767975377752466408</stp>
-        <tr r="C7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6781921016611909505</stp>
-        <tr r="F7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|9843400890588627834</stp>
-        <tr r="L7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|7202116120449006907</stp>
-        <tr r="A7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|9968902354943736400</stp>
+        <stp>BDH|5650835060327148944</stp>
         <tr r="M7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3889401973</v>
         <stp/>
-        <stp>BDH|6868970648471322859</stp>
-        <tr r="Q7" s="4"/>
+        <stp>BDH|7940218944212635318</stp>
+        <tr r="A7" s="4"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -415,10 +397,28 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...1056016836</v>
         <stp/>
-        <stp>BDH|906156193663958325</stp>
+        <stp>BDH|842508002716740427</stp>
+        <tr r="D7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...1414537409</v>
+        <stp/>
+        <stp>BDH|872442251777243102</stp>
         <tr r="G7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...4214137878</v>
+        <stp/>
+        <stp>BDH|243377346286374749</stp>
+        <tr r="L7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3080481446</v>
+        <stp/>
+        <stp>BDH|777656755506079947</stp>
+        <tr r="Q7" s="4"/>
       </tp>
     </main>
   </volType>
@@ -687,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="R66" sqref="R66:R109"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:R132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5800,7 +5800,7 @@
         <v>331.91</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44694</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>332.03</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44697</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>332.41</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44698</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>332.41</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44699</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44700</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44701</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>332.67</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44704</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>333.18</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44705</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>333.17</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44706</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>333.37</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44707</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>333.32</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44708</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44711</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44712</v>
       </c>
@@ -6487,6 +6487,1294 @@
       </c>
       <c r="Q109">
         <v>333.63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B110">
+        <v>8648.2839999999997</v>
+      </c>
+      <c r="C110">
+        <v>8468.5300000000007</v>
+      </c>
+      <c r="D110">
+        <v>336.59</v>
+      </c>
+      <c r="E110">
+        <v>4221.5200000000004</v>
+      </c>
+      <c r="F110">
+        <v>158.27000000000001</v>
+      </c>
+      <c r="G110">
+        <v>114.67310000000001</v>
+      </c>
+      <c r="H110">
+        <v>167.5</v>
+      </c>
+      <c r="I110">
+        <v>93.948700000000002</v>
+      </c>
+      <c r="J110">
+        <v>95.638400000000004</v>
+      </c>
+      <c r="K110">
+        <v>128.96019999999999</v>
+      </c>
+      <c r="L110">
+        <v>880.76</v>
+      </c>
+      <c r="M110">
+        <v>1169.79</v>
+      </c>
+      <c r="N110">
+        <v>293.82600000000002</v>
+      </c>
+      <c r="O110">
+        <v>280.49</v>
+      </c>
+      <c r="P110">
+        <v>355.45</v>
+      </c>
+      <c r="Q110">
+        <v>333.44</v>
+      </c>
+      <c r="R110">
+        <v>171.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B111">
+        <v>8809.1790000000001</v>
+      </c>
+      <c r="C111">
+        <v>8550.3799999999992</v>
+      </c>
+      <c r="D111">
+        <v>341.08</v>
+      </c>
+      <c r="E111">
+        <v>4222.55</v>
+      </c>
+      <c r="F111">
+        <v>158.16</v>
+      </c>
+      <c r="G111">
+        <v>115.17359999999999</v>
+      </c>
+      <c r="H111">
+        <v>168.74</v>
+      </c>
+      <c r="I111">
+        <v>93.763599999999997</v>
+      </c>
+      <c r="J111">
+        <v>95.5458</v>
+      </c>
+      <c r="K111">
+        <v>128.86750000000001</v>
+      </c>
+      <c r="L111">
+        <v>874.38</v>
+      </c>
+      <c r="M111">
+        <v>1169.43</v>
+      </c>
+      <c r="N111">
+        <v>292.9896</v>
+      </c>
+      <c r="O111">
+        <v>280.70999999999998</v>
+      </c>
+      <c r="P111">
+        <v>355.78</v>
+      </c>
+      <c r="Q111">
+        <v>333.63</v>
+      </c>
+      <c r="R111">
+        <v>171.17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B112">
+        <v>8665.8009999999995</v>
+      </c>
+      <c r="C112">
+        <v>8524.5400000000009</v>
+      </c>
+      <c r="D112">
+        <v>337.31</v>
+      </c>
+      <c r="E112">
+        <v>4209</v>
+      </c>
+      <c r="F112">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="G112">
+        <v>114.6434</v>
+      </c>
+      <c r="H112">
+        <v>167.83</v>
+      </c>
+      <c r="I112">
+        <v>93.801100000000005</v>
+      </c>
+      <c r="J112">
+        <v>95.553799999999995</v>
+      </c>
+      <c r="K112">
+        <v>128.89189999999999</v>
+      </c>
+      <c r="L112">
+        <v>880.41</v>
+      </c>
+      <c r="M112">
+        <v>1171.57</v>
+      </c>
+      <c r="N112">
+        <v>292.38049999999998</v>
+      </c>
+      <c r="O112">
+        <v>280.87</v>
+      </c>
+      <c r="P112">
+        <v>355.98</v>
+      </c>
+      <c r="Q112">
+        <v>333.82</v>
+      </c>
+      <c r="R112">
+        <v>171.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B113">
+        <v>8693.0570000000007</v>
+      </c>
+      <c r="C113">
+        <v>8647.91</v>
+      </c>
+      <c r="D113">
+        <v>338.87</v>
+      </c>
+      <c r="E113">
+        <v>4159.0600000000004</v>
+      </c>
+      <c r="F113">
+        <v>154.12</v>
+      </c>
+      <c r="G113">
+        <v>114.5215</v>
+      </c>
+      <c r="H113">
+        <v>168.06</v>
+      </c>
+      <c r="I113">
+        <v>93.754999999999995</v>
+      </c>
+      <c r="J113">
+        <v>95.502300000000005</v>
+      </c>
+      <c r="K113">
+        <v>128.86089999999999</v>
+      </c>
+      <c r="L113">
+        <v>879.61</v>
+      </c>
+      <c r="M113">
+        <v>1169.26</v>
+      </c>
+      <c r="N113">
+        <v>292.55739999999997</v>
+      </c>
+      <c r="O113">
+        <v>280.56</v>
+      </c>
+      <c r="P113">
+        <v>355.64</v>
+      </c>
+      <c r="Q113">
+        <v>333.57</v>
+      </c>
+      <c r="R113">
+        <v>171.44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B114">
+        <v>8776.0889999999999</v>
+      </c>
+      <c r="C114">
+        <v>8576.5400000000009</v>
+      </c>
+      <c r="D114">
+        <v>340.17</v>
+      </c>
+      <c r="E114">
+        <v>4189.1099999999997</v>
+      </c>
+      <c r="F114">
+        <v>156.15</v>
+      </c>
+      <c r="G114">
+        <v>114.7586</v>
+      </c>
+      <c r="H114">
+        <v>168.58</v>
+      </c>
+      <c r="I114">
+        <v>93.699600000000004</v>
+      </c>
+      <c r="J114">
+        <v>95.497900000000001</v>
+      </c>
+      <c r="K114">
+        <v>128.83879999999999</v>
+      </c>
+      <c r="L114">
+        <v>876.67</v>
+      </c>
+      <c r="M114">
+        <v>1166.43</v>
+      </c>
+      <c r="N114">
+        <v>292.2568</v>
+      </c>
+      <c r="O114">
+        <v>280.72000000000003</v>
+      </c>
+      <c r="P114">
+        <v>355.72</v>
+      </c>
+      <c r="Q114">
+        <v>333.68</v>
+      </c>
+      <c r="R114">
+        <v>171.12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B115">
+        <v>8681.6839999999993</v>
+      </c>
+      <c r="C115">
+        <v>8536.41</v>
+      </c>
+      <c r="D115">
+        <v>338.28</v>
+      </c>
+      <c r="E115">
+        <v>4163.7700000000004</v>
+      </c>
+      <c r="F115">
+        <v>154.5</v>
+      </c>
+      <c r="G115">
+        <v>114.1202</v>
+      </c>
+      <c r="H115">
+        <v>168.04</v>
+      </c>
+      <c r="I115">
+        <v>93.687200000000004</v>
+      </c>
+      <c r="J115">
+        <v>95.4452</v>
+      </c>
+      <c r="K115">
+        <v>128.82140000000001</v>
+      </c>
+      <c r="L115">
+        <v>880.71</v>
+      </c>
+      <c r="M115">
+        <v>1165.82</v>
+      </c>
+      <c r="N115">
+        <v>292.07150000000001</v>
+      </c>
+      <c r="O115">
+        <v>280.81</v>
+      </c>
+      <c r="P115">
+        <v>355.86</v>
+      </c>
+      <c r="Q115">
+        <v>333.78</v>
+      </c>
+      <c r="R115">
+        <v>170.97</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B116">
+        <v>8475.9120000000003</v>
+      </c>
+      <c r="C116">
+        <v>8391.15</v>
+      </c>
+      <c r="D116">
+        <v>331.46</v>
+      </c>
+      <c r="E116">
+        <v>4155.17</v>
+      </c>
+      <c r="F116">
+        <v>155.22999999999999</v>
+      </c>
+      <c r="G116">
+        <v>113.5078</v>
+      </c>
+      <c r="H116">
+        <v>166.16</v>
+      </c>
+      <c r="I116">
+        <v>93.726100000000002</v>
+      </c>
+      <c r="J116">
+        <v>95.442700000000002</v>
+      </c>
+      <c r="K116">
+        <v>128.83369999999999</v>
+      </c>
+      <c r="L116">
+        <v>888</v>
+      </c>
+      <c r="M116">
+        <v>1163.27</v>
+      </c>
+      <c r="N116">
+        <v>292.18700000000001</v>
+      </c>
+      <c r="O116">
+        <v>279.95999999999998</v>
+      </c>
+      <c r="P116">
+        <v>354.69</v>
+      </c>
+      <c r="Q116">
+        <v>331.73</v>
+      </c>
+      <c r="R116">
+        <v>170.95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B117">
+        <v>8229.4259999999995</v>
+      </c>
+      <c r="C117">
+        <v>8108.95</v>
+      </c>
+      <c r="D117">
+        <v>322.39</v>
+      </c>
+      <c r="E117">
+        <v>4103.08</v>
+      </c>
+      <c r="F117">
+        <v>154.51</v>
+      </c>
+      <c r="G117">
+        <v>112.6748</v>
+      </c>
+      <c r="H117">
+        <v>163.11000000000001</v>
+      </c>
+      <c r="I117">
+        <v>93.967500000000001</v>
+      </c>
+      <c r="J117">
+        <v>95.713200000000001</v>
+      </c>
+      <c r="K117">
+        <v>128.9804</v>
+      </c>
+      <c r="L117">
+        <v>896.63</v>
+      </c>
+      <c r="M117">
+        <v>1163.08</v>
+      </c>
+      <c r="N117">
+        <v>291.24810000000002</v>
+      </c>
+      <c r="O117">
+        <v>279.89999999999998</v>
+      </c>
+      <c r="P117">
+        <v>354.12</v>
+      </c>
+      <c r="Q117">
+        <v>330.55</v>
+      </c>
+      <c r="R117">
+        <v>170.76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B118">
+        <v>7910.4279999999999</v>
+      </c>
+      <c r="C118">
+        <v>7891.09</v>
+      </c>
+      <c r="D118">
+        <v>310.61</v>
+      </c>
+      <c r="E118">
+        <v>3971.49</v>
+      </c>
+      <c r="F118">
+        <v>148.51</v>
+      </c>
+      <c r="G118">
+        <v>112.6353</v>
+      </c>
+      <c r="H118">
+        <v>158.22999999999999</v>
+      </c>
+      <c r="I118">
+        <v>94.820599999999999</v>
+      </c>
+      <c r="J118">
+        <v>96.454300000000003</v>
+      </c>
+      <c r="K118">
+        <v>129.51150000000001</v>
+      </c>
+      <c r="L118">
+        <v>902.34</v>
+      </c>
+      <c r="M118">
+        <v>1155.43</v>
+      </c>
+      <c r="N118">
+        <v>287.24950000000001</v>
+      </c>
+      <c r="O118">
+        <v>277.58999999999997</v>
+      </c>
+      <c r="P118">
+        <v>354.05</v>
+      </c>
+      <c r="Q118">
+        <v>328.14</v>
+      </c>
+      <c r="R118">
+        <v>171.27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B119">
+        <v>7883.3410000000003</v>
+      </c>
+      <c r="C119">
+        <v>7829.55</v>
+      </c>
+      <c r="D119">
+        <v>308.64999999999998</v>
+      </c>
+      <c r="E119">
+        <v>3934.82</v>
+      </c>
+      <c r="F119">
+        <v>146.13</v>
+      </c>
+      <c r="G119">
+        <v>111.511</v>
+      </c>
+      <c r="H119">
+        <v>157.59</v>
+      </c>
+      <c r="I119">
+        <v>94.619900000000001</v>
+      </c>
+      <c r="J119">
+        <v>96.593000000000004</v>
+      </c>
+      <c r="K119">
+        <v>129.4881</v>
+      </c>
+      <c r="L119">
+        <v>904.89</v>
+      </c>
+      <c r="M119">
+        <v>1155.54</v>
+      </c>
+      <c r="N119">
+        <v>287.84039999999999</v>
+      </c>
+      <c r="O119">
+        <v>278.66000000000003</v>
+      </c>
+      <c r="P119">
+        <v>354.4</v>
+      </c>
+      <c r="Q119">
+        <v>330.22</v>
+      </c>
+      <c r="R119">
+        <v>170.85</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B120">
+        <v>7998.6189999999997</v>
+      </c>
+      <c r="C120">
+        <v>7958.29</v>
+      </c>
+      <c r="D120">
+        <v>312.06</v>
+      </c>
+      <c r="E120">
+        <v>4009.71</v>
+      </c>
+      <c r="F120">
+        <v>149.38</v>
+      </c>
+      <c r="G120">
+        <v>111.1835</v>
+      </c>
+      <c r="H120">
+        <v>159.43</v>
+      </c>
+      <c r="I120">
+        <v>93.5017</v>
+      </c>
+      <c r="J120">
+        <v>95.749600000000001</v>
+      </c>
+      <c r="K120">
+        <v>128.69110000000001</v>
+      </c>
+      <c r="L120">
+        <v>902.75</v>
+      </c>
+      <c r="M120">
+        <v>1155.08</v>
+      </c>
+      <c r="N120">
+        <v>287.88510000000002</v>
+      </c>
+      <c r="O120">
+        <v>279.43</v>
+      </c>
+      <c r="P120">
+        <v>355.16</v>
+      </c>
+      <c r="Q120">
+        <v>331.32</v>
+      </c>
+      <c r="R120">
+        <v>170.18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B121">
+        <v>7739.3879999999999</v>
+      </c>
+      <c r="C121">
+        <v>7723.05</v>
+      </c>
+      <c r="D121">
+        <v>304.55</v>
+      </c>
+      <c r="E121">
+        <v>4008.65</v>
+      </c>
+      <c r="F121">
+        <v>150.53</v>
+      </c>
+      <c r="G121">
+        <v>111.1417</v>
+      </c>
+      <c r="H121">
+        <v>154.57</v>
+      </c>
+      <c r="I121">
+        <v>94.153099999999995</v>
+      </c>
+      <c r="J121">
+        <v>96.234099999999998</v>
+      </c>
+      <c r="K121">
+        <v>129.26</v>
+      </c>
+      <c r="L121">
+        <v>907.41</v>
+      </c>
+      <c r="M121">
+        <v>1154.82</v>
+      </c>
+      <c r="N121">
+        <v>290.25220000000002</v>
+      </c>
+      <c r="O121">
+        <v>279.32</v>
+      </c>
+      <c r="P121">
+        <v>354.68</v>
+      </c>
+      <c r="Q121">
+        <v>329.89</v>
+      </c>
+      <c r="R121">
+        <v>170.73</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B122">
+        <v>7756.5950000000003</v>
+      </c>
+      <c r="C122">
+        <v>7746.82</v>
+      </c>
+      <c r="D122">
+        <v>303.92</v>
+      </c>
+      <c r="E122">
+        <v>4024.97</v>
+      </c>
+      <c r="F122">
+        <v>151.54</v>
+      </c>
+      <c r="G122">
+        <v>110.34229999999999</v>
+      </c>
+      <c r="H122">
+        <v>154.12</v>
+      </c>
+      <c r="I122">
+        <v>93.622399999999999</v>
+      </c>
+      <c r="J122">
+        <v>95.996899999999997</v>
+      </c>
+      <c r="K122">
+        <v>128.7765</v>
+      </c>
+      <c r="L122">
+        <v>908.48</v>
+      </c>
+      <c r="M122">
+        <v>1152.6199999999999</v>
+      </c>
+      <c r="N122">
+        <v>291.83569999999997</v>
+      </c>
+      <c r="O122">
+        <v>279.94</v>
+      </c>
+      <c r="P122">
+        <v>355.87</v>
+      </c>
+      <c r="Q122">
+        <v>331.71</v>
+      </c>
+      <c r="R122">
+        <v>170.12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>44732</v>
+      </c>
+      <c r="B123">
+        <v>7756.5950000000003</v>
+      </c>
+      <c r="C123">
+        <v>7817.5</v>
+      </c>
+      <c r="D123">
+        <v>304.77</v>
+      </c>
+      <c r="E123">
+        <v>4024.97</v>
+      </c>
+      <c r="F123">
+        <v>151.54</v>
+      </c>
+      <c r="G123">
+        <v>110.34229999999999</v>
+      </c>
+      <c r="H123">
+        <v>154.12</v>
+      </c>
+      <c r="I123">
+        <v>93.622399999999999</v>
+      </c>
+      <c r="J123">
+        <v>95.996899999999997</v>
+      </c>
+      <c r="K123">
+        <v>128.7765</v>
+      </c>
+      <c r="L123">
+        <v>908.48</v>
+      </c>
+      <c r="M123">
+        <v>1152.6199999999999</v>
+      </c>
+      <c r="N123">
+        <v>291.83569999999997</v>
+      </c>
+      <c r="O123">
+        <v>279.94</v>
+      </c>
+      <c r="P123">
+        <v>355.87</v>
+      </c>
+      <c r="Q123">
+        <v>331.71</v>
+      </c>
+      <c r="R123">
+        <v>170.12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>44733</v>
+      </c>
+      <c r="B124">
+        <v>7946.8860000000004</v>
+      </c>
+      <c r="C124">
+        <v>7875.87</v>
+      </c>
+      <c r="D124">
+        <v>310.60000000000002</v>
+      </c>
+      <c r="E124">
+        <v>3978.55</v>
+      </c>
+      <c r="F124">
+        <v>147.91999999999999</v>
+      </c>
+      <c r="G124">
+        <v>110.9615</v>
+      </c>
+      <c r="H124">
+        <v>158.63999999999999</v>
+      </c>
+      <c r="I124">
+        <v>93.200299999999999</v>
+      </c>
+      <c r="J124">
+        <v>95.279600000000002</v>
+      </c>
+      <c r="K124">
+        <v>128.37100000000001</v>
+      </c>
+      <c r="L124">
+        <v>903.68</v>
+      </c>
+      <c r="M124">
+        <v>1150.4100000000001</v>
+      </c>
+      <c r="N124">
+        <v>290.11020000000002</v>
+      </c>
+      <c r="O124">
+        <v>279.94</v>
+      </c>
+      <c r="P124">
+        <v>355.35</v>
+      </c>
+      <c r="Q124">
+        <v>331.44</v>
+      </c>
+      <c r="R124">
+        <v>169.56</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>44734</v>
+      </c>
+      <c r="B125">
+        <v>7936.6729999999998</v>
+      </c>
+      <c r="C125">
+        <v>7809.68</v>
+      </c>
+      <c r="D125">
+        <v>309.10000000000002</v>
+      </c>
+      <c r="E125">
+        <v>4028.23</v>
+      </c>
+      <c r="F125">
+        <v>153.07</v>
+      </c>
+      <c r="G125">
+        <v>110.6224</v>
+      </c>
+      <c r="H125">
+        <v>157.65</v>
+      </c>
+      <c r="I125">
+        <v>93.122900000000001</v>
+      </c>
+      <c r="J125">
+        <v>95.2881</v>
+      </c>
+      <c r="K125">
+        <v>128.35980000000001</v>
+      </c>
+      <c r="L125">
+        <v>905.27</v>
+      </c>
+      <c r="M125">
+        <v>1151.96</v>
+      </c>
+      <c r="N125">
+        <v>287.1431</v>
+      </c>
+      <c r="O125">
+        <v>280.23</v>
+      </c>
+      <c r="P125">
+        <v>355.7</v>
+      </c>
+      <c r="Q125">
+        <v>331.79</v>
+      </c>
+      <c r="R125">
+        <v>170.09</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>44735</v>
+      </c>
+      <c r="B126">
+        <v>8012.6750000000002</v>
+      </c>
+      <c r="C126">
+        <v>7745.78</v>
+      </c>
+      <c r="D126">
+        <v>310.47000000000003</v>
+      </c>
+      <c r="E126">
+        <v>4050.48</v>
+      </c>
+      <c r="F126">
+        <v>154.78</v>
+      </c>
+      <c r="G126">
+        <v>110.97799999999999</v>
+      </c>
+      <c r="H126">
+        <v>159.47</v>
+      </c>
+      <c r="I126">
+        <v>93.082899999999995</v>
+      </c>
+      <c r="J126">
+        <v>95.198499999999996</v>
+      </c>
+      <c r="K126">
+        <v>128.2911</v>
+      </c>
+      <c r="L126">
+        <v>903</v>
+      </c>
+      <c r="M126">
+        <v>1151.94</v>
+      </c>
+      <c r="N126">
+        <v>286.12720000000002</v>
+      </c>
+      <c r="O126">
+        <v>280.5</v>
+      </c>
+      <c r="P126">
+        <v>356.06</v>
+      </c>
+      <c r="Q126">
+        <v>331.75</v>
+      </c>
+      <c r="R126">
+        <v>169.88</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>44736</v>
+      </c>
+      <c r="B127">
+        <v>8257.723</v>
+      </c>
+      <c r="C127">
+        <v>7964.15</v>
+      </c>
+      <c r="D127">
+        <v>318.63</v>
+      </c>
+      <c r="E127">
+        <v>4031.65</v>
+      </c>
+      <c r="F127">
+        <v>151.78</v>
+      </c>
+      <c r="G127">
+        <v>112.5175</v>
+      </c>
+      <c r="H127">
+        <v>164.04</v>
+      </c>
+      <c r="I127">
+        <v>92.758200000000002</v>
+      </c>
+      <c r="J127">
+        <v>94.878500000000003</v>
+      </c>
+      <c r="K127">
+        <v>128.0573</v>
+      </c>
+      <c r="L127">
+        <v>895.01</v>
+      </c>
+      <c r="M127">
+        <v>1147.28</v>
+      </c>
+      <c r="N127">
+        <v>287.80189999999999</v>
+      </c>
+      <c r="O127">
+        <v>280.39</v>
+      </c>
+      <c r="P127">
+        <v>356.08</v>
+      </c>
+      <c r="Q127">
+        <v>331.87</v>
+      </c>
+      <c r="R127">
+        <v>169.35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>44739</v>
+      </c>
+      <c r="B128">
+        <v>8233.4210000000003</v>
+      </c>
+      <c r="C128">
+        <v>7977.03</v>
+      </c>
+      <c r="D128">
+        <v>319.64</v>
+      </c>
+      <c r="E128">
+        <v>4002.53</v>
+      </c>
+      <c r="F128">
+        <v>150.22999999999999</v>
+      </c>
+      <c r="G128">
+        <v>111.9072</v>
+      </c>
+      <c r="H128">
+        <v>163.54</v>
+      </c>
+      <c r="I128">
+        <v>92.659000000000006</v>
+      </c>
+      <c r="J128">
+        <v>94.802199999999999</v>
+      </c>
+      <c r="K128">
+        <v>127.98569999999999</v>
+      </c>
+      <c r="L128">
+        <v>896.96</v>
+      </c>
+      <c r="M128">
+        <v>1148.3399999999999</v>
+      </c>
+      <c r="N128">
+        <v>284.53309999999999</v>
+      </c>
+      <c r="O128">
+        <v>280.75</v>
+      </c>
+      <c r="P128">
+        <v>356.54</v>
+      </c>
+      <c r="Q128">
+        <v>332.18</v>
+      </c>
+      <c r="R128">
+        <v>169.59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44740</v>
+      </c>
+      <c r="B129">
+        <v>8067.558</v>
+      </c>
+      <c r="C129">
+        <v>8000.5</v>
+      </c>
+      <c r="D129">
+        <v>315.55</v>
+      </c>
+      <c r="E129">
+        <v>4001.91</v>
+      </c>
+      <c r="F129">
+        <v>151.11000000000001</v>
+      </c>
+      <c r="G129">
+        <v>111.3095</v>
+      </c>
+      <c r="H129">
+        <v>160.51</v>
+      </c>
+      <c r="I129">
+        <v>92.689599999999999</v>
+      </c>
+      <c r="J129">
+        <v>94.776899999999998</v>
+      </c>
+      <c r="K129">
+        <v>128.0222</v>
+      </c>
+      <c r="L129">
+        <v>902.32</v>
+      </c>
+      <c r="M129">
+        <v>1152.18</v>
+      </c>
+      <c r="N129">
+        <v>285.69220000000001</v>
+      </c>
+      <c r="O129">
+        <v>280.39</v>
+      </c>
+      <c r="P129">
+        <v>355.77</v>
+      </c>
+      <c r="Q129">
+        <v>332.05</v>
+      </c>
+      <c r="R129">
+        <v>169.78</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44741</v>
+      </c>
+      <c r="B130">
+        <v>8062.7160000000003</v>
+      </c>
+      <c r="C130">
+        <v>7921.66</v>
+      </c>
+      <c r="D130">
+        <v>314</v>
+      </c>
+      <c r="E130">
+        <v>4035.07</v>
+      </c>
+      <c r="F130">
+        <v>154.1</v>
+      </c>
+      <c r="G130">
+        <v>111.2119</v>
+      </c>
+      <c r="H130">
+        <v>160.46</v>
+      </c>
+      <c r="I130">
+        <v>92.822100000000006</v>
+      </c>
+      <c r="J130">
+        <v>94.894499999999994</v>
+      </c>
+      <c r="K130">
+        <v>128.09729999999999</v>
+      </c>
+      <c r="L130">
+        <v>902.93</v>
+      </c>
+      <c r="M130">
+        <v>1154.01</v>
+      </c>
+      <c r="N130">
+        <v>285.67520000000002</v>
+      </c>
+      <c r="O130">
+        <v>280.72000000000003</v>
+      </c>
+      <c r="P130">
+        <v>356.26</v>
+      </c>
+      <c r="Q130">
+        <v>332.39</v>
+      </c>
+      <c r="R130">
+        <v>170.05</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B131">
+        <v>7993.4309999999996</v>
+      </c>
+      <c r="C131">
+        <v>7787.65</v>
+      </c>
+      <c r="D131">
+        <v>310.52999999999997</v>
+      </c>
+      <c r="E131">
+        <v>4043.14</v>
+      </c>
+      <c r="F131">
+        <v>155.53</v>
+      </c>
+      <c r="G131">
+        <v>111.0522</v>
+      </c>
+      <c r="H131">
+        <v>158.94</v>
+      </c>
+      <c r="I131">
+        <v>92.837500000000006</v>
+      </c>
+      <c r="J131">
+        <v>95.083399999999997</v>
+      </c>
+      <c r="K131">
+        <v>128.1704</v>
+      </c>
+      <c r="L131">
+        <v>903.49</v>
+      </c>
+      <c r="M131">
+        <v>1155.82</v>
+      </c>
+      <c r="N131">
+        <v>285.72050000000002</v>
+      </c>
+      <c r="O131">
+        <v>280.33</v>
+      </c>
+      <c r="P131">
+        <v>355.74</v>
+      </c>
+      <c r="Q131">
+        <v>331.33</v>
+      </c>
+      <c r="R131">
+        <v>169.57</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B132">
+        <v>8077.8919999999998</v>
+      </c>
+      <c r="C132">
+        <v>7772.86</v>
+      </c>
+      <c r="D132">
+        <v>311.73</v>
+      </c>
+      <c r="E132">
+        <v>4067.56</v>
+      </c>
+      <c r="F132">
+        <v>156.43</v>
+      </c>
+      <c r="G132">
+        <v>111.1767</v>
+      </c>
+      <c r="H132">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="I132">
+        <v>92.722399999999993</v>
+      </c>
+      <c r="J132">
+        <v>94.889799999999994</v>
+      </c>
+      <c r="K132">
+        <v>128.06899999999999</v>
+      </c>
+      <c r="L132">
+        <v>902.1</v>
+      </c>
+      <c r="M132">
+        <v>1155.33</v>
+      </c>
+      <c r="N132">
+        <v>286.02019999999999</v>
+      </c>
+      <c r="O132">
+        <v>280.37</v>
+      </c>
+      <c r="P132">
+        <v>356.08</v>
+      </c>
+      <c r="Q132">
+        <v>332.06</v>
+      </c>
+      <c r="R132">
+        <v>169.94</v>
       </c>
     </row>
   </sheetData>
@@ -6495,10 +7783,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3611"/>
   <sheetViews>
-    <sheetView topLeftCell="A3573" workbookViewId="0">
+    <sheetView topLeftCell="A3603" workbookViewId="0">
       <selection activeCell="C3611" sqref="C3611"/>
     </sheetView>
   </sheetViews>
@@ -57067,11 +58355,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R289"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R283"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:R137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57095,7 +58383,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1">
@@ -57103,14 +58391,18 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>44712</v>
-      </c>
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -57164,6 +58456,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" t="str">
         <f>_xll.BFieldInfo(B$6)</f>
         <v>Last Price</v>
@@ -57234,7 +58527,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -57291,74 +58584,74 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=108")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=131")</f>
         <v>44561</v>
       </c>
       <c r="B7">
         <v>9986.6980000000003</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>9491.1</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>389.04</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>5233.6899999999996</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>214.08</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>122.8967</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>175.14</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>98.672499999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>101.2684</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>135.21369999999999</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>835.24</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>1088</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>297.6395</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>287.23</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>368.34</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>345.76</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
         <v>169.35</v>
       </c>
     </row>
@@ -63355,93 +64648,1312 @@
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
+      <c r="A115" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B115">
+        <v>8648.2839999999997</v>
+      </c>
+      <c r="C115">
+        <v>8468.5300000000007</v>
+      </c>
+      <c r="D115">
+        <v>336.59</v>
+      </c>
+      <c r="E115">
+        <v>4221.5200000000004</v>
+      </c>
+      <c r="F115">
+        <v>158.27000000000001</v>
+      </c>
+      <c r="G115">
+        <v>114.67310000000001</v>
+      </c>
+      <c r="H115">
+        <v>167.5</v>
+      </c>
+      <c r="I115">
+        <v>93.948700000000002</v>
+      </c>
+      <c r="J115">
+        <v>95.638400000000004</v>
+      </c>
+      <c r="K115">
+        <v>128.96019999999999</v>
+      </c>
+      <c r="L115">
+        <v>880.76</v>
+      </c>
+      <c r="M115">
+        <v>1169.79</v>
+      </c>
+      <c r="N115">
+        <v>293.82600000000002</v>
+      </c>
+      <c r="O115">
+        <v>280.49</v>
+      </c>
+      <c r="P115">
+        <v>355.45</v>
+      </c>
+      <c r="Q115">
+        <v>333.44</v>
+      </c>
+      <c r="R115">
+        <v>171.3</v>
+      </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+      <c r="A116" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B116">
+        <v>8809.1790000000001</v>
+      </c>
+      <c r="C116">
+        <v>8550.3799999999992</v>
+      </c>
+      <c r="D116">
+        <v>341.08</v>
+      </c>
+      <c r="E116">
+        <v>4222.55</v>
+      </c>
+      <c r="F116">
+        <v>158.16</v>
+      </c>
+      <c r="G116">
+        <v>115.17359999999999</v>
+      </c>
+      <c r="H116">
+        <v>168.74</v>
+      </c>
+      <c r="I116">
+        <v>93.763599999999997</v>
+      </c>
+      <c r="J116">
+        <v>95.5458</v>
+      </c>
+      <c r="K116">
+        <v>128.86750000000001</v>
+      </c>
+      <c r="L116">
+        <v>874.38</v>
+      </c>
+      <c r="M116">
+        <v>1169.43</v>
+      </c>
+      <c r="N116">
+        <v>292.9896</v>
+      </c>
+      <c r="O116">
+        <v>280.70999999999998</v>
+      </c>
+      <c r="P116">
+        <v>355.78</v>
+      </c>
+      <c r="Q116">
+        <v>333.63</v>
+      </c>
+      <c r="R116">
+        <v>171.17</v>
+      </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+      <c r="A117" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B117">
+        <v>8665.8009999999995</v>
+      </c>
+      <c r="C117">
+        <v>8524.5400000000009</v>
+      </c>
+      <c r="D117">
+        <v>337.31</v>
+      </c>
+      <c r="E117">
+        <v>4209</v>
+      </c>
+      <c r="F117">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="G117">
+        <v>114.6434</v>
+      </c>
+      <c r="H117">
+        <v>167.83</v>
+      </c>
+      <c r="I117">
+        <v>93.801100000000005</v>
+      </c>
+      <c r="J117">
+        <v>95.553799999999995</v>
+      </c>
+      <c r="K117">
+        <v>128.89189999999999</v>
+      </c>
+      <c r="L117">
+        <v>880.41</v>
+      </c>
+      <c r="M117">
+        <v>1171.57</v>
+      </c>
+      <c r="N117">
+        <v>292.38049999999998</v>
+      </c>
+      <c r="O117">
+        <v>280.87</v>
+      </c>
+      <c r="P117">
+        <v>355.98</v>
+      </c>
+      <c r="Q117">
+        <v>333.82</v>
+      </c>
+      <c r="R117">
+        <v>171.6</v>
+      </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+      <c r="A118" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B118">
+        <v>8693.0570000000007</v>
+      </c>
+      <c r="C118">
+        <v>8647.91</v>
+      </c>
+      <c r="D118">
+        <v>338.87</v>
+      </c>
+      <c r="E118">
+        <v>4159.0600000000004</v>
+      </c>
+      <c r="F118">
+        <v>154.12</v>
+      </c>
+      <c r="G118">
+        <v>114.5215</v>
+      </c>
+      <c r="H118">
+        <v>168.06</v>
+      </c>
+      <c r="I118">
+        <v>93.754999999999995</v>
+      </c>
+      <c r="J118">
+        <v>95.502300000000005</v>
+      </c>
+      <c r="K118">
+        <v>128.86089999999999</v>
+      </c>
+      <c r="L118">
+        <v>879.61</v>
+      </c>
+      <c r="M118">
+        <v>1169.26</v>
+      </c>
+      <c r="N118">
+        <v>292.55739999999997</v>
+      </c>
+      <c r="O118">
+        <v>280.56</v>
+      </c>
+      <c r="P118">
+        <v>355.64</v>
+      </c>
+      <c r="Q118">
+        <v>333.57</v>
+      </c>
+      <c r="R118">
+        <v>171.44</v>
+      </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B119">
+        <v>8776.0889999999999</v>
+      </c>
+      <c r="C119">
+        <v>8576.5400000000009</v>
+      </c>
+      <c r="D119">
+        <v>340.17</v>
+      </c>
+      <c r="E119">
+        <v>4189.1099999999997</v>
+      </c>
+      <c r="F119">
+        <v>156.15</v>
+      </c>
+      <c r="G119">
+        <v>114.7586</v>
+      </c>
+      <c r="H119">
+        <v>168.58</v>
+      </c>
+      <c r="I119">
+        <v>93.699600000000004</v>
+      </c>
+      <c r="J119">
+        <v>95.497900000000001</v>
+      </c>
+      <c r="K119">
+        <v>128.83879999999999</v>
+      </c>
+      <c r="L119">
+        <v>876.67</v>
+      </c>
+      <c r="M119">
+        <v>1166.43</v>
+      </c>
+      <c r="N119">
+        <v>292.2568</v>
+      </c>
+      <c r="O119">
+        <v>280.72000000000003</v>
+      </c>
+      <c r="P119">
+        <v>355.72</v>
+      </c>
+      <c r="Q119">
+        <v>333.68</v>
+      </c>
+      <c r="R119">
+        <v>171.12</v>
+      </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
+      <c r="A120" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B120">
+        <v>8681.6839999999993</v>
+      </c>
+      <c r="C120">
+        <v>8536.41</v>
+      </c>
+      <c r="D120">
+        <v>338.28</v>
+      </c>
+      <c r="E120">
+        <v>4163.7700000000004</v>
+      </c>
+      <c r="F120">
+        <v>154.5</v>
+      </c>
+      <c r="G120">
+        <v>114.1202</v>
+      </c>
+      <c r="H120">
+        <v>168.04</v>
+      </c>
+      <c r="I120">
+        <v>93.687200000000004</v>
+      </c>
+      <c r="J120">
+        <v>95.4452</v>
+      </c>
+      <c r="K120">
+        <v>128.82140000000001</v>
+      </c>
+      <c r="L120">
+        <v>880.71</v>
+      </c>
+      <c r="M120">
+        <v>1165.82</v>
+      </c>
+      <c r="N120">
+        <v>292.07150000000001</v>
+      </c>
+      <c r="O120">
+        <v>280.81</v>
+      </c>
+      <c r="P120">
+        <v>355.86</v>
+      </c>
+      <c r="Q120">
+        <v>333.78</v>
+      </c>
+      <c r="R120">
+        <v>170.97</v>
+      </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
+      <c r="A121" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B121">
+        <v>8475.9120000000003</v>
+      </c>
+      <c r="C121">
+        <v>8391.15</v>
+      </c>
+      <c r="D121">
+        <v>331.46</v>
+      </c>
+      <c r="E121">
+        <v>4155.17</v>
+      </c>
+      <c r="F121">
+        <v>155.22999999999999</v>
+      </c>
+      <c r="G121">
+        <v>113.5078</v>
+      </c>
+      <c r="H121">
+        <v>166.16</v>
+      </c>
+      <c r="I121">
+        <v>93.726100000000002</v>
+      </c>
+      <c r="J121">
+        <v>95.442700000000002</v>
+      </c>
+      <c r="K121">
+        <v>128.83369999999999</v>
+      </c>
+      <c r="L121">
+        <v>888</v>
+      </c>
+      <c r="M121">
+        <v>1163.27</v>
+      </c>
+      <c r="N121">
+        <v>292.18700000000001</v>
+      </c>
+      <c r="O121">
+        <v>279.95999999999998</v>
+      </c>
+      <c r="P121">
+        <v>354.69</v>
+      </c>
+      <c r="Q121">
+        <v>331.73</v>
+      </c>
+      <c r="R121">
+        <v>170.95</v>
+      </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B122">
+        <v>8229.4259999999995</v>
+      </c>
+      <c r="C122">
+        <v>8108.95</v>
+      </c>
+      <c r="D122">
+        <v>322.39</v>
+      </c>
+      <c r="E122">
+        <v>4103.08</v>
+      </c>
+      <c r="F122">
+        <v>154.51</v>
+      </c>
+      <c r="G122">
+        <v>112.6748</v>
+      </c>
+      <c r="H122">
+        <v>163.11000000000001</v>
+      </c>
+      <c r="I122">
+        <v>93.967500000000001</v>
+      </c>
+      <c r="J122">
+        <v>95.713200000000001</v>
+      </c>
+      <c r="K122">
+        <v>128.9804</v>
+      </c>
+      <c r="L122">
+        <v>896.63</v>
+      </c>
+      <c r="M122">
+        <v>1163.08</v>
+      </c>
+      <c r="N122">
+        <v>291.24810000000002</v>
+      </c>
+      <c r="O122">
+        <v>279.89999999999998</v>
+      </c>
+      <c r="P122">
+        <v>354.12</v>
+      </c>
+      <c r="Q122">
+        <v>330.55</v>
+      </c>
+      <c r="R122">
+        <v>170.76</v>
+      </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B123">
+        <v>7910.4279999999999</v>
+      </c>
+      <c r="C123">
+        <v>7891.09</v>
+      </c>
+      <c r="D123">
+        <v>310.61</v>
+      </c>
+      <c r="E123">
+        <v>3971.49</v>
+      </c>
+      <c r="F123">
+        <v>148.51</v>
+      </c>
+      <c r="G123">
+        <v>112.6353</v>
+      </c>
+      <c r="H123">
+        <v>158.22999999999999</v>
+      </c>
+      <c r="I123">
+        <v>94.820599999999999</v>
+      </c>
+      <c r="J123">
+        <v>96.454300000000003</v>
+      </c>
+      <c r="K123">
+        <v>129.51150000000001</v>
+      </c>
+      <c r="L123">
+        <v>902.34</v>
+      </c>
+      <c r="M123">
+        <v>1155.43</v>
+      </c>
+      <c r="N123">
+        <v>287.24950000000001</v>
+      </c>
+      <c r="O123">
+        <v>277.58999999999997</v>
+      </c>
+      <c r="P123">
+        <v>354.05</v>
+      </c>
+      <c r="Q123">
+        <v>328.14</v>
+      </c>
+      <c r="R123">
+        <v>171.27</v>
+      </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B124">
+        <v>7883.3410000000003</v>
+      </c>
+      <c r="C124">
+        <v>7829.55</v>
+      </c>
+      <c r="D124">
+        <v>308.64999999999998</v>
+      </c>
+      <c r="E124">
+        <v>3934.82</v>
+      </c>
+      <c r="F124">
+        <v>146.13</v>
+      </c>
+      <c r="G124">
+        <v>111.511</v>
+      </c>
+      <c r="H124">
+        <v>157.59</v>
+      </c>
+      <c r="I124">
+        <v>94.619900000000001</v>
+      </c>
+      <c r="J124">
+        <v>96.593000000000004</v>
+      </c>
+      <c r="K124">
+        <v>129.4881</v>
+      </c>
+      <c r="L124">
+        <v>904.89</v>
+      </c>
+      <c r="M124">
+        <v>1155.54</v>
+      </c>
+      <c r="N124">
+        <v>287.84039999999999</v>
+      </c>
+      <c r="O124">
+        <v>278.66000000000003</v>
+      </c>
+      <c r="P124">
+        <v>354.4</v>
+      </c>
+      <c r="Q124">
+        <v>330.22</v>
+      </c>
+      <c r="R124">
+        <v>170.85</v>
+      </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
+      <c r="A125" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B125">
+        <v>7998.6189999999997</v>
+      </c>
+      <c r="C125">
+        <v>7958.29</v>
+      </c>
+      <c r="D125">
+        <v>312.06</v>
+      </c>
+      <c r="E125">
+        <v>4009.71</v>
+      </c>
+      <c r="F125">
+        <v>149.38</v>
+      </c>
+      <c r="G125">
+        <v>111.1835</v>
+      </c>
+      <c r="H125">
+        <v>159.43</v>
+      </c>
+      <c r="I125">
+        <v>93.5017</v>
+      </c>
+      <c r="J125">
+        <v>95.749600000000001</v>
+      </c>
+      <c r="K125">
+        <v>128.69110000000001</v>
+      </c>
+      <c r="L125">
+        <v>902.75</v>
+      </c>
+      <c r="M125">
+        <v>1155.08</v>
+      </c>
+      <c r="N125">
+        <v>287.88510000000002</v>
+      </c>
+      <c r="O125">
+        <v>279.43</v>
+      </c>
+      <c r="P125">
+        <v>355.16</v>
+      </c>
+      <c r="Q125">
+        <v>331.32</v>
+      </c>
+      <c r="R125">
+        <v>170.18</v>
+      </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
+      <c r="A126" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B126">
+        <v>7739.3879999999999</v>
+      </c>
+      <c r="C126">
+        <v>7723.05</v>
+      </c>
+      <c r="D126">
+        <v>304.55</v>
+      </c>
+      <c r="E126">
+        <v>4008.65</v>
+      </c>
+      <c r="F126">
+        <v>150.53</v>
+      </c>
+      <c r="G126">
+        <v>111.1417</v>
+      </c>
+      <c r="H126">
+        <v>154.57</v>
+      </c>
+      <c r="I126">
+        <v>94.153099999999995</v>
+      </c>
+      <c r="J126">
+        <v>96.234099999999998</v>
+      </c>
+      <c r="K126">
+        <v>129.26</v>
+      </c>
+      <c r="L126">
+        <v>907.41</v>
+      </c>
+      <c r="M126">
+        <v>1154.82</v>
+      </c>
+      <c r="N126">
+        <v>290.25220000000002</v>
+      </c>
+      <c r="O126">
+        <v>279.32</v>
+      </c>
+      <c r="P126">
+        <v>354.68</v>
+      </c>
+      <c r="Q126">
+        <v>329.89</v>
+      </c>
+      <c r="R126">
+        <v>170.73</v>
+      </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
+      <c r="A127" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B127">
+        <v>7756.5950000000003</v>
+      </c>
+      <c r="C127">
+        <v>7746.82</v>
+      </c>
+      <c r="D127">
+        <v>303.92</v>
+      </c>
+      <c r="E127">
+        <v>4024.97</v>
+      </c>
+      <c r="F127">
+        <v>151.54</v>
+      </c>
+      <c r="G127">
+        <v>110.34229999999999</v>
+      </c>
+      <c r="H127">
+        <v>154.12</v>
+      </c>
+      <c r="I127">
+        <v>93.622399999999999</v>
+      </c>
+      <c r="J127">
+        <v>95.996899999999997</v>
+      </c>
+      <c r="K127">
+        <v>128.7765</v>
+      </c>
+      <c r="L127">
+        <v>908.48</v>
+      </c>
+      <c r="M127">
+        <v>1152.6199999999999</v>
+      </c>
+      <c r="N127">
+        <v>291.83569999999997</v>
+      </c>
+      <c r="O127">
+        <v>279.94</v>
+      </c>
+      <c r="P127">
+        <v>355.87</v>
+      </c>
+      <c r="Q127">
+        <v>331.71</v>
+      </c>
+      <c r="R127">
+        <v>170.12</v>
+      </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>44732</v>
+      </c>
+      <c r="B128">
+        <v>7756.5950000000003</v>
+      </c>
+      <c r="C128">
+        <v>7817.5</v>
+      </c>
+      <c r="D128">
+        <v>304.77</v>
+      </c>
+      <c r="E128">
+        <v>4024.97</v>
+      </c>
+      <c r="F128">
+        <v>151.54</v>
+      </c>
+      <c r="G128">
+        <v>110.34229999999999</v>
+      </c>
+      <c r="H128">
+        <v>154.12</v>
+      </c>
+      <c r="I128">
+        <v>93.622399999999999</v>
+      </c>
+      <c r="J128">
+        <v>95.996899999999997</v>
+      </c>
+      <c r="K128">
+        <v>128.7765</v>
+      </c>
+      <c r="L128">
+        <v>908.48</v>
+      </c>
+      <c r="M128">
+        <v>1152.6199999999999</v>
+      </c>
+      <c r="N128">
+        <v>291.83569999999997</v>
+      </c>
+      <c r="O128">
+        <v>279.94</v>
+      </c>
+      <c r="P128">
+        <v>355.87</v>
+      </c>
+      <c r="Q128">
+        <v>331.71</v>
+      </c>
+      <c r="R128">
+        <v>170.12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44733</v>
+      </c>
+      <c r="B129">
+        <v>7946.8860000000004</v>
+      </c>
+      <c r="C129">
+        <v>7875.87</v>
+      </c>
+      <c r="D129">
+        <v>310.60000000000002</v>
+      </c>
+      <c r="E129">
+        <v>3978.55</v>
+      </c>
+      <c r="F129">
+        <v>147.91999999999999</v>
+      </c>
+      <c r="G129">
+        <v>110.9615</v>
+      </c>
+      <c r="H129">
+        <v>158.63999999999999</v>
+      </c>
+      <c r="I129">
+        <v>93.200299999999999</v>
+      </c>
+      <c r="J129">
+        <v>95.279600000000002</v>
+      </c>
+      <c r="K129">
+        <v>128.37100000000001</v>
+      </c>
+      <c r="L129">
+        <v>903.68</v>
+      </c>
+      <c r="M129">
+        <v>1150.4100000000001</v>
+      </c>
+      <c r="N129">
+        <v>290.11020000000002</v>
+      </c>
+      <c r="O129">
+        <v>279.94</v>
+      </c>
+      <c r="P129">
+        <v>355.35</v>
+      </c>
+      <c r="Q129">
+        <v>331.44</v>
+      </c>
+      <c r="R129">
+        <v>169.56</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44734</v>
+      </c>
+      <c r="B130">
+        <v>7936.6729999999998</v>
+      </c>
+      <c r="C130">
+        <v>7809.68</v>
+      </c>
+      <c r="D130">
+        <v>309.10000000000002</v>
+      </c>
+      <c r="E130">
+        <v>4028.23</v>
+      </c>
+      <c r="F130">
+        <v>153.07</v>
+      </c>
+      <c r="G130">
+        <v>110.6224</v>
+      </c>
+      <c r="H130">
+        <v>157.65</v>
+      </c>
+      <c r="I130">
+        <v>93.122900000000001</v>
+      </c>
+      <c r="J130">
+        <v>95.2881</v>
+      </c>
+      <c r="K130">
+        <v>128.35980000000001</v>
+      </c>
+      <c r="L130">
+        <v>905.27</v>
+      </c>
+      <c r="M130">
+        <v>1151.96</v>
+      </c>
+      <c r="N130">
+        <v>287.1431</v>
+      </c>
+      <c r="O130">
+        <v>280.23</v>
+      </c>
+      <c r="P130">
+        <v>355.7</v>
+      </c>
+      <c r="Q130">
+        <v>331.79</v>
+      </c>
+      <c r="R130">
+        <v>170.09</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44735</v>
+      </c>
+      <c r="B131">
+        <v>8012.6750000000002</v>
+      </c>
+      <c r="C131">
+        <v>7745.78</v>
+      </c>
+      <c r="D131">
+        <v>310.47000000000003</v>
+      </c>
+      <c r="E131">
+        <v>4050.48</v>
+      </c>
+      <c r="F131">
+        <v>154.78</v>
+      </c>
+      <c r="G131">
+        <v>110.97799999999999</v>
+      </c>
+      <c r="H131">
+        <v>159.47</v>
+      </c>
+      <c r="I131">
+        <v>93.082899999999995</v>
+      </c>
+      <c r="J131">
+        <v>95.198499999999996</v>
+      </c>
+      <c r="K131">
+        <v>128.2911</v>
+      </c>
+      <c r="L131">
+        <v>903</v>
+      </c>
+      <c r="M131">
+        <v>1151.94</v>
+      </c>
+      <c r="N131">
+        <v>286.12720000000002</v>
+      </c>
+      <c r="O131">
+        <v>280.5</v>
+      </c>
+      <c r="P131">
+        <v>356.06</v>
+      </c>
+      <c r="Q131">
+        <v>331.75</v>
+      </c>
+      <c r="R131">
+        <v>169.88</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44736</v>
+      </c>
+      <c r="B132">
+        <v>8257.723</v>
+      </c>
+      <c r="C132">
+        <v>7964.15</v>
+      </c>
+      <c r="D132">
+        <v>318.63</v>
+      </c>
+      <c r="E132">
+        <v>4031.65</v>
+      </c>
+      <c r="F132">
+        <v>151.78</v>
+      </c>
+      <c r="G132">
+        <v>112.5175</v>
+      </c>
+      <c r="H132">
+        <v>164.04</v>
+      </c>
+      <c r="I132">
+        <v>92.758200000000002</v>
+      </c>
+      <c r="J132">
+        <v>94.878500000000003</v>
+      </c>
+      <c r="K132">
+        <v>128.0573</v>
+      </c>
+      <c r="L132">
+        <v>895.01</v>
+      </c>
+      <c r="M132">
+        <v>1147.28</v>
+      </c>
+      <c r="N132">
+        <v>287.80189999999999</v>
+      </c>
+      <c r="O132">
+        <v>280.39</v>
+      </c>
+      <c r="P132">
+        <v>356.08</v>
+      </c>
+      <c r="Q132">
+        <v>331.87</v>
+      </c>
+      <c r="R132">
+        <v>169.35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>44739</v>
+      </c>
+      <c r="B133">
+        <v>8233.4210000000003</v>
+      </c>
+      <c r="C133">
+        <v>7977.03</v>
+      </c>
+      <c r="D133">
+        <v>319.64</v>
+      </c>
+      <c r="E133">
+        <v>4002.53</v>
+      </c>
+      <c r="F133">
+        <v>150.22999999999999</v>
+      </c>
+      <c r="G133">
+        <v>111.9072</v>
+      </c>
+      <c r="H133">
+        <v>163.54</v>
+      </c>
+      <c r="I133">
+        <v>92.659000000000006</v>
+      </c>
+      <c r="J133">
+        <v>94.802199999999999</v>
+      </c>
+      <c r="K133">
+        <v>127.98569999999999</v>
+      </c>
+      <c r="L133">
+        <v>896.96</v>
+      </c>
+      <c r="M133">
+        <v>1148.3399999999999</v>
+      </c>
+      <c r="N133">
+        <v>284.53309999999999</v>
+      </c>
+      <c r="O133">
+        <v>280.75</v>
+      </c>
+      <c r="P133">
+        <v>356.54</v>
+      </c>
+      <c r="Q133">
+        <v>332.18</v>
+      </c>
+      <c r="R133">
+        <v>169.59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>44740</v>
+      </c>
+      <c r="B134">
+        <v>8067.558</v>
+      </c>
+      <c r="C134">
+        <v>8000.5</v>
+      </c>
+      <c r="D134">
+        <v>315.55</v>
+      </c>
+      <c r="E134">
+        <v>4001.91</v>
+      </c>
+      <c r="F134">
+        <v>151.11000000000001</v>
+      </c>
+      <c r="G134">
+        <v>111.3095</v>
+      </c>
+      <c r="H134">
+        <v>160.51</v>
+      </c>
+      <c r="I134">
+        <v>92.689599999999999</v>
+      </c>
+      <c r="J134">
+        <v>94.776899999999998</v>
+      </c>
+      <c r="K134">
+        <v>128.0222</v>
+      </c>
+      <c r="L134">
+        <v>902.32</v>
+      </c>
+      <c r="M134">
+        <v>1152.18</v>
+      </c>
+      <c r="N134">
+        <v>285.69220000000001</v>
+      </c>
+      <c r="O134">
+        <v>280.39</v>
+      </c>
+      <c r="P134">
+        <v>355.77</v>
+      </c>
+      <c r="Q134">
+        <v>332.05</v>
+      </c>
+      <c r="R134">
+        <v>169.78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>44741</v>
+      </c>
+      <c r="B135">
+        <v>8062.7160000000003</v>
+      </c>
+      <c r="C135">
+        <v>7921.66</v>
+      </c>
+      <c r="D135">
+        <v>314</v>
+      </c>
+      <c r="E135">
+        <v>4035.07</v>
+      </c>
+      <c r="F135">
+        <v>154.1</v>
+      </c>
+      <c r="G135">
+        <v>111.2119</v>
+      </c>
+      <c r="H135">
+        <v>160.46</v>
+      </c>
+      <c r="I135">
+        <v>92.822100000000006</v>
+      </c>
+      <c r="J135">
+        <v>94.894499999999994</v>
+      </c>
+      <c r="K135">
+        <v>128.09729999999999</v>
+      </c>
+      <c r="L135">
+        <v>902.93</v>
+      </c>
+      <c r="M135">
+        <v>1154.01</v>
+      </c>
+      <c r="N135">
+        <v>285.67520000000002</v>
+      </c>
+      <c r="O135">
+        <v>280.72000000000003</v>
+      </c>
+      <c r="P135">
+        <v>356.26</v>
+      </c>
+      <c r="Q135">
+        <v>332.39</v>
+      </c>
+      <c r="R135">
+        <v>170.05</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B136">
+        <v>7993.4309999999996</v>
+      </c>
+      <c r="C136">
+        <v>7787.65</v>
+      </c>
+      <c r="D136">
+        <v>310.52999999999997</v>
+      </c>
+      <c r="E136">
+        <v>4043.14</v>
+      </c>
+      <c r="F136">
+        <v>155.53</v>
+      </c>
+      <c r="G136">
+        <v>111.0522</v>
+      </c>
+      <c r="H136">
+        <v>158.94</v>
+      </c>
+      <c r="I136">
+        <v>92.837500000000006</v>
+      </c>
+      <c r="J136">
+        <v>95.083399999999997</v>
+      </c>
+      <c r="K136">
+        <v>128.1704</v>
+      </c>
+      <c r="L136">
+        <v>903.49</v>
+      </c>
+      <c r="M136">
+        <v>1155.82</v>
+      </c>
+      <c r="N136">
+        <v>285.72050000000002</v>
+      </c>
+      <c r="O136">
+        <v>280.33</v>
+      </c>
+      <c r="P136">
+        <v>355.74</v>
+      </c>
+      <c r="Q136">
+        <v>331.33</v>
+      </c>
+      <c r="R136">
+        <v>169.57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B137">
+        <v>8077.8919999999998</v>
+      </c>
+      <c r="C137">
+        <v>7772.86</v>
+      </c>
+      <c r="D137">
+        <v>311.73</v>
+      </c>
+      <c r="E137">
+        <v>4067.56</v>
+      </c>
+      <c r="F137">
+        <v>156.43</v>
+      </c>
+      <c r="G137">
+        <v>111.1767</v>
+      </c>
+      <c r="H137">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="I137">
+        <v>92.722399999999993</v>
+      </c>
+      <c r="J137">
+        <v>94.889799999999994</v>
+      </c>
+      <c r="K137">
+        <v>128.06899999999999</v>
+      </c>
+      <c r="L137">
+        <v>902.1</v>
+      </c>
+      <c r="M137">
+        <v>1155.33</v>
+      </c>
+      <c r="N137">
+        <v>286.02019999999999</v>
+      </c>
+      <c r="O137">
+        <v>280.37</v>
+      </c>
+      <c r="P137">
+        <v>356.08</v>
+      </c>
+      <c r="Q137">
+        <v>332.06</v>
+      </c>
+      <c r="R137">
+        <v>169.94</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
@@ -63860,24 +66372,6 @@
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="1"/>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="1"/>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="1"/>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="1"/>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -63885,11 +66379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "update ups_data for June 2022"
This reverts commit bd22ee26306f849ce1925b4062f333a985a0f19b.
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\RMP\EquityHedging\data\update_strats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E0939DA-E5C9-4493-9B2A-5718BCB7E4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -24,9 +25,8 @@
     <definedName name="SpreadsheetBuilder_2" hidden="1">#REF!</definedName>
     <definedName name="SpreadsheetBuilder_3" localSheetId="3" hidden="1">data_original!$A$1:$Q$1</definedName>
     <definedName name="SpreadsheetBuilder_3" hidden="1">data!$A$1:$Q$1</definedName>
-    <definedName name="SpreadsheetBuilder_4" hidden="1">bbg!$A$1:$R$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,84 +177,102 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...2498000376</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13443209491875865478</stp>
+        <stp>BDH|14373309094453461515</stp>
+        <tr r="N7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15254198816498138559</stp>
+        <tr r="K7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12376458535329946451</stp>
+        <tr r="E7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14047895025460654716</stp>
+        <tr r="I7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15219073193266403418</stp>
         <tr r="O7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292474235</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17104415084249048216</stp>
-        <tr r="C7" s="4"/>
+        <stp>BDH|17676840938570904020</stp>
+        <tr r="D7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3114597649</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10780736232050436488</stp>
-        <tr r="H7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3312458933</v>
-        <stp/>
-        <stp>BDH|11392435143047097029</stp>
-        <tr r="J7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3684680868</v>
-        <stp/>
-        <stp>BDH|13681390364586674687</stp>
-        <tr r="R7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3902279735</v>
-        <stp/>
-        <stp>BDH|12813523539692123174</stp>
-        <tr r="N7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...2648455992</v>
-        <stp/>
-        <stp>BDH|10651658260607967001</stp>
-        <tr r="E7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4262317047</v>
-        <stp/>
-        <stp>BDH|16172402952033261032</stp>
-        <tr r="F7" s="4"/>
+        <stp>BDH|17737690590601603895</stp>
+        <tr r="P7" s="4"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4166306348</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7372156945517956837</stp>
-        <tr r="I7" s="4"/>
+        <stp>BDH|4440947643953867604</stp>
+        <tr r="J7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2793532776</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4044657110195260995</stp>
-        <tr r="K7" s="4"/>
+        <stp>BDH|8374361155286374440</stp>
+        <tr r="H7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3867305555</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7247267998221805998</stp>
-        <tr r="P7" s="4"/>
+        <stp>BDH|8741188097968377687</stp>
+        <tr r="R7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2967649377</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5650835060327148944</stp>
+        <stp>BDH|7767975377752466408</stp>
+        <tr r="C7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|6781921016611909505</stp>
+        <tr r="F7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9843400890588627834</stp>
+        <tr r="L7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7202116120449006907</stp>
+        <tr r="A7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9968902354943736400</stp>
         <tr r="M7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3889401973</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7940218944212635318</stp>
-        <tr r="A7" s="4"/>
+        <stp>BDH|6868970648471322859</stp>
+        <tr r="Q7" s="4"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -397,28 +415,10 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...1056016836</v>
+        <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|842508002716740427</stp>
-        <tr r="D7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...1414537409</v>
-        <stp/>
-        <stp>BDH|872442251777243102</stp>
+        <stp>BDH|906156193663958325</stp>
         <tr r="G7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4214137878</v>
-        <stp/>
-        <stp>BDH|243377346286374749</stp>
-        <tr r="L7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3080481446</v>
-        <stp/>
-        <stp>BDH|777656755506079947</stp>
-        <tr r="Q7" s="4"/>
       </tp>
     </main>
   </volType>
@@ -687,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:R132"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66:R109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5800,7 +5800,7 @@
         <v>331.91</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44694</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>332.03</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44697</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>332.41</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44698</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>332.41</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44699</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44700</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44701</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>332.67</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44704</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>333.18</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44705</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>333.17</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44706</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>333.37</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44707</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>333.32</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44708</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44711</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>333.58</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44712</v>
       </c>
@@ -6487,1294 +6487,6 @@
       </c>
       <c r="Q109">
         <v>333.63</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>44713</v>
-      </c>
-      <c r="B110">
-        <v>8648.2839999999997</v>
-      </c>
-      <c r="C110">
-        <v>8468.5300000000007</v>
-      </c>
-      <c r="D110">
-        <v>336.59</v>
-      </c>
-      <c r="E110">
-        <v>4221.5200000000004</v>
-      </c>
-      <c r="F110">
-        <v>158.27000000000001</v>
-      </c>
-      <c r="G110">
-        <v>114.67310000000001</v>
-      </c>
-      <c r="H110">
-        <v>167.5</v>
-      </c>
-      <c r="I110">
-        <v>93.948700000000002</v>
-      </c>
-      <c r="J110">
-        <v>95.638400000000004</v>
-      </c>
-      <c r="K110">
-        <v>128.96019999999999</v>
-      </c>
-      <c r="L110">
-        <v>880.76</v>
-      </c>
-      <c r="M110">
-        <v>1169.79</v>
-      </c>
-      <c r="N110">
-        <v>293.82600000000002</v>
-      </c>
-      <c r="O110">
-        <v>280.49</v>
-      </c>
-      <c r="P110">
-        <v>355.45</v>
-      </c>
-      <c r="Q110">
-        <v>333.44</v>
-      </c>
-      <c r="R110">
-        <v>171.3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>44714</v>
-      </c>
-      <c r="B111">
-        <v>8809.1790000000001</v>
-      </c>
-      <c r="C111">
-        <v>8550.3799999999992</v>
-      </c>
-      <c r="D111">
-        <v>341.08</v>
-      </c>
-      <c r="E111">
-        <v>4222.55</v>
-      </c>
-      <c r="F111">
-        <v>158.16</v>
-      </c>
-      <c r="G111">
-        <v>115.17359999999999</v>
-      </c>
-      <c r="H111">
-        <v>168.74</v>
-      </c>
-      <c r="I111">
-        <v>93.763599999999997</v>
-      </c>
-      <c r="J111">
-        <v>95.5458</v>
-      </c>
-      <c r="K111">
-        <v>128.86750000000001</v>
-      </c>
-      <c r="L111">
-        <v>874.38</v>
-      </c>
-      <c r="M111">
-        <v>1169.43</v>
-      </c>
-      <c r="N111">
-        <v>292.9896</v>
-      </c>
-      <c r="O111">
-        <v>280.70999999999998</v>
-      </c>
-      <c r="P111">
-        <v>355.78</v>
-      </c>
-      <c r="Q111">
-        <v>333.63</v>
-      </c>
-      <c r="R111">
-        <v>171.17</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>44715</v>
-      </c>
-      <c r="B112">
-        <v>8665.8009999999995</v>
-      </c>
-      <c r="C112">
-        <v>8524.5400000000009</v>
-      </c>
-      <c r="D112">
-        <v>337.31</v>
-      </c>
-      <c r="E112">
-        <v>4209</v>
-      </c>
-      <c r="F112">
-        <v>157.80000000000001</v>
-      </c>
-      <c r="G112">
-        <v>114.6434</v>
-      </c>
-      <c r="H112">
-        <v>167.83</v>
-      </c>
-      <c r="I112">
-        <v>93.801100000000005</v>
-      </c>
-      <c r="J112">
-        <v>95.553799999999995</v>
-      </c>
-      <c r="K112">
-        <v>128.89189999999999</v>
-      </c>
-      <c r="L112">
-        <v>880.41</v>
-      </c>
-      <c r="M112">
-        <v>1171.57</v>
-      </c>
-      <c r="N112">
-        <v>292.38049999999998</v>
-      </c>
-      <c r="O112">
-        <v>280.87</v>
-      </c>
-      <c r="P112">
-        <v>355.98</v>
-      </c>
-      <c r="Q112">
-        <v>333.82</v>
-      </c>
-      <c r="R112">
-        <v>171.6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>44718</v>
-      </c>
-      <c r="B113">
-        <v>8693.0570000000007</v>
-      </c>
-      <c r="C113">
-        <v>8647.91</v>
-      </c>
-      <c r="D113">
-        <v>338.87</v>
-      </c>
-      <c r="E113">
-        <v>4159.0600000000004</v>
-      </c>
-      <c r="F113">
-        <v>154.12</v>
-      </c>
-      <c r="G113">
-        <v>114.5215</v>
-      </c>
-      <c r="H113">
-        <v>168.06</v>
-      </c>
-      <c r="I113">
-        <v>93.754999999999995</v>
-      </c>
-      <c r="J113">
-        <v>95.502300000000005</v>
-      </c>
-      <c r="K113">
-        <v>128.86089999999999</v>
-      </c>
-      <c r="L113">
-        <v>879.61</v>
-      </c>
-      <c r="M113">
-        <v>1169.26</v>
-      </c>
-      <c r="N113">
-        <v>292.55739999999997</v>
-      </c>
-      <c r="O113">
-        <v>280.56</v>
-      </c>
-      <c r="P113">
-        <v>355.64</v>
-      </c>
-      <c r="Q113">
-        <v>333.57</v>
-      </c>
-      <c r="R113">
-        <v>171.44</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>44719</v>
-      </c>
-      <c r="B114">
-        <v>8776.0889999999999</v>
-      </c>
-      <c r="C114">
-        <v>8576.5400000000009</v>
-      </c>
-      <c r="D114">
-        <v>340.17</v>
-      </c>
-      <c r="E114">
-        <v>4189.1099999999997</v>
-      </c>
-      <c r="F114">
-        <v>156.15</v>
-      </c>
-      <c r="G114">
-        <v>114.7586</v>
-      </c>
-      <c r="H114">
-        <v>168.58</v>
-      </c>
-      <c r="I114">
-        <v>93.699600000000004</v>
-      </c>
-      <c r="J114">
-        <v>95.497900000000001</v>
-      </c>
-      <c r="K114">
-        <v>128.83879999999999</v>
-      </c>
-      <c r="L114">
-        <v>876.67</v>
-      </c>
-      <c r="M114">
-        <v>1166.43</v>
-      </c>
-      <c r="N114">
-        <v>292.2568</v>
-      </c>
-      <c r="O114">
-        <v>280.72000000000003</v>
-      </c>
-      <c r="P114">
-        <v>355.72</v>
-      </c>
-      <c r="Q114">
-        <v>333.68</v>
-      </c>
-      <c r="R114">
-        <v>171.12</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>44720</v>
-      </c>
-      <c r="B115">
-        <v>8681.6839999999993</v>
-      </c>
-      <c r="C115">
-        <v>8536.41</v>
-      </c>
-      <c r="D115">
-        <v>338.28</v>
-      </c>
-      <c r="E115">
-        <v>4163.7700000000004</v>
-      </c>
-      <c r="F115">
-        <v>154.5</v>
-      </c>
-      <c r="G115">
-        <v>114.1202</v>
-      </c>
-      <c r="H115">
-        <v>168.04</v>
-      </c>
-      <c r="I115">
-        <v>93.687200000000004</v>
-      </c>
-      <c r="J115">
-        <v>95.4452</v>
-      </c>
-      <c r="K115">
-        <v>128.82140000000001</v>
-      </c>
-      <c r="L115">
-        <v>880.71</v>
-      </c>
-      <c r="M115">
-        <v>1165.82</v>
-      </c>
-      <c r="N115">
-        <v>292.07150000000001</v>
-      </c>
-      <c r="O115">
-        <v>280.81</v>
-      </c>
-      <c r="P115">
-        <v>355.86</v>
-      </c>
-      <c r="Q115">
-        <v>333.78</v>
-      </c>
-      <c r="R115">
-        <v>170.97</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>44721</v>
-      </c>
-      <c r="B116">
-        <v>8475.9120000000003</v>
-      </c>
-      <c r="C116">
-        <v>8391.15</v>
-      </c>
-      <c r="D116">
-        <v>331.46</v>
-      </c>
-      <c r="E116">
-        <v>4155.17</v>
-      </c>
-      <c r="F116">
-        <v>155.22999999999999</v>
-      </c>
-      <c r="G116">
-        <v>113.5078</v>
-      </c>
-      <c r="H116">
-        <v>166.16</v>
-      </c>
-      <c r="I116">
-        <v>93.726100000000002</v>
-      </c>
-      <c r="J116">
-        <v>95.442700000000002</v>
-      </c>
-      <c r="K116">
-        <v>128.83369999999999</v>
-      </c>
-      <c r="L116">
-        <v>888</v>
-      </c>
-      <c r="M116">
-        <v>1163.27</v>
-      </c>
-      <c r="N116">
-        <v>292.18700000000001</v>
-      </c>
-      <c r="O116">
-        <v>279.95999999999998</v>
-      </c>
-      <c r="P116">
-        <v>354.69</v>
-      </c>
-      <c r="Q116">
-        <v>331.73</v>
-      </c>
-      <c r="R116">
-        <v>170.95</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>44722</v>
-      </c>
-      <c r="B117">
-        <v>8229.4259999999995</v>
-      </c>
-      <c r="C117">
-        <v>8108.95</v>
-      </c>
-      <c r="D117">
-        <v>322.39</v>
-      </c>
-      <c r="E117">
-        <v>4103.08</v>
-      </c>
-      <c r="F117">
-        <v>154.51</v>
-      </c>
-      <c r="G117">
-        <v>112.6748</v>
-      </c>
-      <c r="H117">
-        <v>163.11000000000001</v>
-      </c>
-      <c r="I117">
-        <v>93.967500000000001</v>
-      </c>
-      <c r="J117">
-        <v>95.713200000000001</v>
-      </c>
-      <c r="K117">
-        <v>128.9804</v>
-      </c>
-      <c r="L117">
-        <v>896.63</v>
-      </c>
-      <c r="M117">
-        <v>1163.08</v>
-      </c>
-      <c r="N117">
-        <v>291.24810000000002</v>
-      </c>
-      <c r="O117">
-        <v>279.89999999999998</v>
-      </c>
-      <c r="P117">
-        <v>354.12</v>
-      </c>
-      <c r="Q117">
-        <v>330.55</v>
-      </c>
-      <c r="R117">
-        <v>170.76</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>44725</v>
-      </c>
-      <c r="B118">
-        <v>7910.4279999999999</v>
-      </c>
-      <c r="C118">
-        <v>7891.09</v>
-      </c>
-      <c r="D118">
-        <v>310.61</v>
-      </c>
-      <c r="E118">
-        <v>3971.49</v>
-      </c>
-      <c r="F118">
-        <v>148.51</v>
-      </c>
-      <c r="G118">
-        <v>112.6353</v>
-      </c>
-      <c r="H118">
-        <v>158.22999999999999</v>
-      </c>
-      <c r="I118">
-        <v>94.820599999999999</v>
-      </c>
-      <c r="J118">
-        <v>96.454300000000003</v>
-      </c>
-      <c r="K118">
-        <v>129.51150000000001</v>
-      </c>
-      <c r="L118">
-        <v>902.34</v>
-      </c>
-      <c r="M118">
-        <v>1155.43</v>
-      </c>
-      <c r="N118">
-        <v>287.24950000000001</v>
-      </c>
-      <c r="O118">
-        <v>277.58999999999997</v>
-      </c>
-      <c r="P118">
-        <v>354.05</v>
-      </c>
-      <c r="Q118">
-        <v>328.14</v>
-      </c>
-      <c r="R118">
-        <v>171.27</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>44726</v>
-      </c>
-      <c r="B119">
-        <v>7883.3410000000003</v>
-      </c>
-      <c r="C119">
-        <v>7829.55</v>
-      </c>
-      <c r="D119">
-        <v>308.64999999999998</v>
-      </c>
-      <c r="E119">
-        <v>3934.82</v>
-      </c>
-      <c r="F119">
-        <v>146.13</v>
-      </c>
-      <c r="G119">
-        <v>111.511</v>
-      </c>
-      <c r="H119">
-        <v>157.59</v>
-      </c>
-      <c r="I119">
-        <v>94.619900000000001</v>
-      </c>
-      <c r="J119">
-        <v>96.593000000000004</v>
-      </c>
-      <c r="K119">
-        <v>129.4881</v>
-      </c>
-      <c r="L119">
-        <v>904.89</v>
-      </c>
-      <c r="M119">
-        <v>1155.54</v>
-      </c>
-      <c r="N119">
-        <v>287.84039999999999</v>
-      </c>
-      <c r="O119">
-        <v>278.66000000000003</v>
-      </c>
-      <c r="P119">
-        <v>354.4</v>
-      </c>
-      <c r="Q119">
-        <v>330.22</v>
-      </c>
-      <c r="R119">
-        <v>170.85</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>44727</v>
-      </c>
-      <c r="B120">
-        <v>7998.6189999999997</v>
-      </c>
-      <c r="C120">
-        <v>7958.29</v>
-      </c>
-      <c r="D120">
-        <v>312.06</v>
-      </c>
-      <c r="E120">
-        <v>4009.71</v>
-      </c>
-      <c r="F120">
-        <v>149.38</v>
-      </c>
-      <c r="G120">
-        <v>111.1835</v>
-      </c>
-      <c r="H120">
-        <v>159.43</v>
-      </c>
-      <c r="I120">
-        <v>93.5017</v>
-      </c>
-      <c r="J120">
-        <v>95.749600000000001</v>
-      </c>
-      <c r="K120">
-        <v>128.69110000000001</v>
-      </c>
-      <c r="L120">
-        <v>902.75</v>
-      </c>
-      <c r="M120">
-        <v>1155.08</v>
-      </c>
-      <c r="N120">
-        <v>287.88510000000002</v>
-      </c>
-      <c r="O120">
-        <v>279.43</v>
-      </c>
-      <c r="P120">
-        <v>355.16</v>
-      </c>
-      <c r="Q120">
-        <v>331.32</v>
-      </c>
-      <c r="R120">
-        <v>170.18</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>44728</v>
-      </c>
-      <c r="B121">
-        <v>7739.3879999999999</v>
-      </c>
-      <c r="C121">
-        <v>7723.05</v>
-      </c>
-      <c r="D121">
-        <v>304.55</v>
-      </c>
-      <c r="E121">
-        <v>4008.65</v>
-      </c>
-      <c r="F121">
-        <v>150.53</v>
-      </c>
-      <c r="G121">
-        <v>111.1417</v>
-      </c>
-      <c r="H121">
-        <v>154.57</v>
-      </c>
-      <c r="I121">
-        <v>94.153099999999995</v>
-      </c>
-      <c r="J121">
-        <v>96.234099999999998</v>
-      </c>
-      <c r="K121">
-        <v>129.26</v>
-      </c>
-      <c r="L121">
-        <v>907.41</v>
-      </c>
-      <c r="M121">
-        <v>1154.82</v>
-      </c>
-      <c r="N121">
-        <v>290.25220000000002</v>
-      </c>
-      <c r="O121">
-        <v>279.32</v>
-      </c>
-      <c r="P121">
-        <v>354.68</v>
-      </c>
-      <c r="Q121">
-        <v>329.89</v>
-      </c>
-      <c r="R121">
-        <v>170.73</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>44729</v>
-      </c>
-      <c r="B122">
-        <v>7756.5950000000003</v>
-      </c>
-      <c r="C122">
-        <v>7746.82</v>
-      </c>
-      <c r="D122">
-        <v>303.92</v>
-      </c>
-      <c r="E122">
-        <v>4024.97</v>
-      </c>
-      <c r="F122">
-        <v>151.54</v>
-      </c>
-      <c r="G122">
-        <v>110.34229999999999</v>
-      </c>
-      <c r="H122">
-        <v>154.12</v>
-      </c>
-      <c r="I122">
-        <v>93.622399999999999</v>
-      </c>
-      <c r="J122">
-        <v>95.996899999999997</v>
-      </c>
-      <c r="K122">
-        <v>128.7765</v>
-      </c>
-      <c r="L122">
-        <v>908.48</v>
-      </c>
-      <c r="M122">
-        <v>1152.6199999999999</v>
-      </c>
-      <c r="N122">
-        <v>291.83569999999997</v>
-      </c>
-      <c r="O122">
-        <v>279.94</v>
-      </c>
-      <c r="P122">
-        <v>355.87</v>
-      </c>
-      <c r="Q122">
-        <v>331.71</v>
-      </c>
-      <c r="R122">
-        <v>170.12</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>44732</v>
-      </c>
-      <c r="B123">
-        <v>7756.5950000000003</v>
-      </c>
-      <c r="C123">
-        <v>7817.5</v>
-      </c>
-      <c r="D123">
-        <v>304.77</v>
-      </c>
-      <c r="E123">
-        <v>4024.97</v>
-      </c>
-      <c r="F123">
-        <v>151.54</v>
-      </c>
-      <c r="G123">
-        <v>110.34229999999999</v>
-      </c>
-      <c r="H123">
-        <v>154.12</v>
-      </c>
-      <c r="I123">
-        <v>93.622399999999999</v>
-      </c>
-      <c r="J123">
-        <v>95.996899999999997</v>
-      </c>
-      <c r="K123">
-        <v>128.7765</v>
-      </c>
-      <c r="L123">
-        <v>908.48</v>
-      </c>
-      <c r="M123">
-        <v>1152.6199999999999</v>
-      </c>
-      <c r="N123">
-        <v>291.83569999999997</v>
-      </c>
-      <c r="O123">
-        <v>279.94</v>
-      </c>
-      <c r="P123">
-        <v>355.87</v>
-      </c>
-      <c r="Q123">
-        <v>331.71</v>
-      </c>
-      <c r="R123">
-        <v>170.12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>44733</v>
-      </c>
-      <c r="B124">
-        <v>7946.8860000000004</v>
-      </c>
-      <c r="C124">
-        <v>7875.87</v>
-      </c>
-      <c r="D124">
-        <v>310.60000000000002</v>
-      </c>
-      <c r="E124">
-        <v>3978.55</v>
-      </c>
-      <c r="F124">
-        <v>147.91999999999999</v>
-      </c>
-      <c r="G124">
-        <v>110.9615</v>
-      </c>
-      <c r="H124">
-        <v>158.63999999999999</v>
-      </c>
-      <c r="I124">
-        <v>93.200299999999999</v>
-      </c>
-      <c r="J124">
-        <v>95.279600000000002</v>
-      </c>
-      <c r="K124">
-        <v>128.37100000000001</v>
-      </c>
-      <c r="L124">
-        <v>903.68</v>
-      </c>
-      <c r="M124">
-        <v>1150.4100000000001</v>
-      </c>
-      <c r="N124">
-        <v>290.11020000000002</v>
-      </c>
-      <c r="O124">
-        <v>279.94</v>
-      </c>
-      <c r="P124">
-        <v>355.35</v>
-      </c>
-      <c r="Q124">
-        <v>331.44</v>
-      </c>
-      <c r="R124">
-        <v>169.56</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>44734</v>
-      </c>
-      <c r="B125">
-        <v>7936.6729999999998</v>
-      </c>
-      <c r="C125">
-        <v>7809.68</v>
-      </c>
-      <c r="D125">
-        <v>309.10000000000002</v>
-      </c>
-      <c r="E125">
-        <v>4028.23</v>
-      </c>
-      <c r="F125">
-        <v>153.07</v>
-      </c>
-      <c r="G125">
-        <v>110.6224</v>
-      </c>
-      <c r="H125">
-        <v>157.65</v>
-      </c>
-      <c r="I125">
-        <v>93.122900000000001</v>
-      </c>
-      <c r="J125">
-        <v>95.2881</v>
-      </c>
-      <c r="K125">
-        <v>128.35980000000001</v>
-      </c>
-      <c r="L125">
-        <v>905.27</v>
-      </c>
-      <c r="M125">
-        <v>1151.96</v>
-      </c>
-      <c r="N125">
-        <v>287.1431</v>
-      </c>
-      <c r="O125">
-        <v>280.23</v>
-      </c>
-      <c r="P125">
-        <v>355.7</v>
-      </c>
-      <c r="Q125">
-        <v>331.79</v>
-      </c>
-      <c r="R125">
-        <v>170.09</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B126">
-        <v>8012.6750000000002</v>
-      </c>
-      <c r="C126">
-        <v>7745.78</v>
-      </c>
-      <c r="D126">
-        <v>310.47000000000003</v>
-      </c>
-      <c r="E126">
-        <v>4050.48</v>
-      </c>
-      <c r="F126">
-        <v>154.78</v>
-      </c>
-      <c r="G126">
-        <v>110.97799999999999</v>
-      </c>
-      <c r="H126">
-        <v>159.47</v>
-      </c>
-      <c r="I126">
-        <v>93.082899999999995</v>
-      </c>
-      <c r="J126">
-        <v>95.198499999999996</v>
-      </c>
-      <c r="K126">
-        <v>128.2911</v>
-      </c>
-      <c r="L126">
-        <v>903</v>
-      </c>
-      <c r="M126">
-        <v>1151.94</v>
-      </c>
-      <c r="N126">
-        <v>286.12720000000002</v>
-      </c>
-      <c r="O126">
-        <v>280.5</v>
-      </c>
-      <c r="P126">
-        <v>356.06</v>
-      </c>
-      <c r="Q126">
-        <v>331.75</v>
-      </c>
-      <c r="R126">
-        <v>169.88</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>44736</v>
-      </c>
-      <c r="B127">
-        <v>8257.723</v>
-      </c>
-      <c r="C127">
-        <v>7964.15</v>
-      </c>
-      <c r="D127">
-        <v>318.63</v>
-      </c>
-      <c r="E127">
-        <v>4031.65</v>
-      </c>
-      <c r="F127">
-        <v>151.78</v>
-      </c>
-      <c r="G127">
-        <v>112.5175</v>
-      </c>
-      <c r="H127">
-        <v>164.04</v>
-      </c>
-      <c r="I127">
-        <v>92.758200000000002</v>
-      </c>
-      <c r="J127">
-        <v>94.878500000000003</v>
-      </c>
-      <c r="K127">
-        <v>128.0573</v>
-      </c>
-      <c r="L127">
-        <v>895.01</v>
-      </c>
-      <c r="M127">
-        <v>1147.28</v>
-      </c>
-      <c r="N127">
-        <v>287.80189999999999</v>
-      </c>
-      <c r="O127">
-        <v>280.39</v>
-      </c>
-      <c r="P127">
-        <v>356.08</v>
-      </c>
-      <c r="Q127">
-        <v>331.87</v>
-      </c>
-      <c r="R127">
-        <v>169.35</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>44739</v>
-      </c>
-      <c r="B128">
-        <v>8233.4210000000003</v>
-      </c>
-      <c r="C128">
-        <v>7977.03</v>
-      </c>
-      <c r="D128">
-        <v>319.64</v>
-      </c>
-      <c r="E128">
-        <v>4002.53</v>
-      </c>
-      <c r="F128">
-        <v>150.22999999999999</v>
-      </c>
-      <c r="G128">
-        <v>111.9072</v>
-      </c>
-      <c r="H128">
-        <v>163.54</v>
-      </c>
-      <c r="I128">
-        <v>92.659000000000006</v>
-      </c>
-      <c r="J128">
-        <v>94.802199999999999</v>
-      </c>
-      <c r="K128">
-        <v>127.98569999999999</v>
-      </c>
-      <c r="L128">
-        <v>896.96</v>
-      </c>
-      <c r="M128">
-        <v>1148.3399999999999</v>
-      </c>
-      <c r="N128">
-        <v>284.53309999999999</v>
-      </c>
-      <c r="O128">
-        <v>280.75</v>
-      </c>
-      <c r="P128">
-        <v>356.54</v>
-      </c>
-      <c r="Q128">
-        <v>332.18</v>
-      </c>
-      <c r="R128">
-        <v>169.59</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>44740</v>
-      </c>
-      <c r="B129">
-        <v>8067.558</v>
-      </c>
-      <c r="C129">
-        <v>8000.5</v>
-      </c>
-      <c r="D129">
-        <v>315.55</v>
-      </c>
-      <c r="E129">
-        <v>4001.91</v>
-      </c>
-      <c r="F129">
-        <v>151.11000000000001</v>
-      </c>
-      <c r="G129">
-        <v>111.3095</v>
-      </c>
-      <c r="H129">
-        <v>160.51</v>
-      </c>
-      <c r="I129">
-        <v>92.689599999999999</v>
-      </c>
-      <c r="J129">
-        <v>94.776899999999998</v>
-      </c>
-      <c r="K129">
-        <v>128.0222</v>
-      </c>
-      <c r="L129">
-        <v>902.32</v>
-      </c>
-      <c r="M129">
-        <v>1152.18</v>
-      </c>
-      <c r="N129">
-        <v>285.69220000000001</v>
-      </c>
-      <c r="O129">
-        <v>280.39</v>
-      </c>
-      <c r="P129">
-        <v>355.77</v>
-      </c>
-      <c r="Q129">
-        <v>332.05</v>
-      </c>
-      <c r="R129">
-        <v>169.78</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>44741</v>
-      </c>
-      <c r="B130">
-        <v>8062.7160000000003</v>
-      </c>
-      <c r="C130">
-        <v>7921.66</v>
-      </c>
-      <c r="D130">
-        <v>314</v>
-      </c>
-      <c r="E130">
-        <v>4035.07</v>
-      </c>
-      <c r="F130">
-        <v>154.1</v>
-      </c>
-      <c r="G130">
-        <v>111.2119</v>
-      </c>
-      <c r="H130">
-        <v>160.46</v>
-      </c>
-      <c r="I130">
-        <v>92.822100000000006</v>
-      </c>
-      <c r="J130">
-        <v>94.894499999999994</v>
-      </c>
-      <c r="K130">
-        <v>128.09729999999999</v>
-      </c>
-      <c r="L130">
-        <v>902.93</v>
-      </c>
-      <c r="M130">
-        <v>1154.01</v>
-      </c>
-      <c r="N130">
-        <v>285.67520000000002</v>
-      </c>
-      <c r="O130">
-        <v>280.72000000000003</v>
-      </c>
-      <c r="P130">
-        <v>356.26</v>
-      </c>
-      <c r="Q130">
-        <v>332.39</v>
-      </c>
-      <c r="R130">
-        <v>170.05</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>44742</v>
-      </c>
-      <c r="B131">
-        <v>7993.4309999999996</v>
-      </c>
-      <c r="C131">
-        <v>7787.65</v>
-      </c>
-      <c r="D131">
-        <v>310.52999999999997</v>
-      </c>
-      <c r="E131">
-        <v>4043.14</v>
-      </c>
-      <c r="F131">
-        <v>155.53</v>
-      </c>
-      <c r="G131">
-        <v>111.0522</v>
-      </c>
-      <c r="H131">
-        <v>158.94</v>
-      </c>
-      <c r="I131">
-        <v>92.837500000000006</v>
-      </c>
-      <c r="J131">
-        <v>95.083399999999997</v>
-      </c>
-      <c r="K131">
-        <v>128.1704</v>
-      </c>
-      <c r="L131">
-        <v>903.49</v>
-      </c>
-      <c r="M131">
-        <v>1155.82</v>
-      </c>
-      <c r="N131">
-        <v>285.72050000000002</v>
-      </c>
-      <c r="O131">
-        <v>280.33</v>
-      </c>
-      <c r="P131">
-        <v>355.74</v>
-      </c>
-      <c r="Q131">
-        <v>331.33</v>
-      </c>
-      <c r="R131">
-        <v>169.57</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>44743</v>
-      </c>
-      <c r="B132">
-        <v>8077.8919999999998</v>
-      </c>
-      <c r="C132">
-        <v>7772.86</v>
-      </c>
-      <c r="D132">
-        <v>311.73</v>
-      </c>
-      <c r="E132">
-        <v>4067.56</v>
-      </c>
-      <c r="F132">
-        <v>156.43</v>
-      </c>
-      <c r="G132">
-        <v>111.1767</v>
-      </c>
-      <c r="H132">
-        <v>160.80000000000001</v>
-      </c>
-      <c r="I132">
-        <v>92.722399999999993</v>
-      </c>
-      <c r="J132">
-        <v>94.889799999999994</v>
-      </c>
-      <c r="K132">
-        <v>128.06899999999999</v>
-      </c>
-      <c r="L132">
-        <v>902.1</v>
-      </c>
-      <c r="M132">
-        <v>1155.33</v>
-      </c>
-      <c r="N132">
-        <v>286.02019999999999</v>
-      </c>
-      <c r="O132">
-        <v>280.37</v>
-      </c>
-      <c r="P132">
-        <v>356.08</v>
-      </c>
-      <c r="Q132">
-        <v>332.06</v>
-      </c>
-      <c r="R132">
-        <v>169.94</v>
       </c>
     </row>
   </sheetData>
@@ -7783,10 +6495,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3611"/>
   <sheetViews>
-    <sheetView topLeftCell="A3603" workbookViewId="0">
+    <sheetView topLeftCell="A3573" workbookViewId="0">
       <selection activeCell="C3611" sqref="C3611"/>
     </sheetView>
   </sheetViews>
@@ -58355,11 +57067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R283"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:R289"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115:R137"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58383,7 +57095,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1">
@@ -58391,18 +57103,14 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>44743</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+        <v>44712</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -58456,7 +57164,6 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
       <c r="B5" t="str">
         <f>_xll.BFieldInfo(B$6)</f>
         <v>Last Price</v>
@@ -58527,7 +57234,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -58584,74 +57291,74 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=131")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=108")</f>
         <v>44561</v>
       </c>
       <c r="B7">
         <v>9986.6980000000003</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>9491.1</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>389.04</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>5233.6899999999996</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>214.08</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>122.8967</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>175.14</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>98.672499999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>101.2684</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>135.21369999999999</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>835.24</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>1088</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>297.6395</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>287.23</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>368.34</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>345.76</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=131")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=108")</f>
         <v>169.35</v>
       </c>
     </row>
@@ -64648,1312 +63355,93 @@
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>44713</v>
-      </c>
-      <c r="B115">
-        <v>8648.2839999999997</v>
-      </c>
-      <c r="C115">
-        <v>8468.5300000000007</v>
-      </c>
-      <c r="D115">
-        <v>336.59</v>
-      </c>
-      <c r="E115">
-        <v>4221.5200000000004</v>
-      </c>
-      <c r="F115">
-        <v>158.27000000000001</v>
-      </c>
-      <c r="G115">
-        <v>114.67310000000001</v>
-      </c>
-      <c r="H115">
-        <v>167.5</v>
-      </c>
-      <c r="I115">
-        <v>93.948700000000002</v>
-      </c>
-      <c r="J115">
-        <v>95.638400000000004</v>
-      </c>
-      <c r="K115">
-        <v>128.96019999999999</v>
-      </c>
-      <c r="L115">
-        <v>880.76</v>
-      </c>
-      <c r="M115">
-        <v>1169.79</v>
-      </c>
-      <c r="N115">
-        <v>293.82600000000002</v>
-      </c>
-      <c r="O115">
-        <v>280.49</v>
-      </c>
-      <c r="P115">
-        <v>355.45</v>
-      </c>
-      <c r="Q115">
-        <v>333.44</v>
-      </c>
-      <c r="R115">
-        <v>171.3</v>
-      </c>
+      <c r="A115" s="1"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>44714</v>
-      </c>
-      <c r="B116">
-        <v>8809.1790000000001</v>
-      </c>
-      <c r="C116">
-        <v>8550.3799999999992</v>
-      </c>
-      <c r="D116">
-        <v>341.08</v>
-      </c>
-      <c r="E116">
-        <v>4222.55</v>
-      </c>
-      <c r="F116">
-        <v>158.16</v>
-      </c>
-      <c r="G116">
-        <v>115.17359999999999</v>
-      </c>
-      <c r="H116">
-        <v>168.74</v>
-      </c>
-      <c r="I116">
-        <v>93.763599999999997</v>
-      </c>
-      <c r="J116">
-        <v>95.5458</v>
-      </c>
-      <c r="K116">
-        <v>128.86750000000001</v>
-      </c>
-      <c r="L116">
-        <v>874.38</v>
-      </c>
-      <c r="M116">
-        <v>1169.43</v>
-      </c>
-      <c r="N116">
-        <v>292.9896</v>
-      </c>
-      <c r="O116">
-        <v>280.70999999999998</v>
-      </c>
-      <c r="P116">
-        <v>355.78</v>
-      </c>
-      <c r="Q116">
-        <v>333.63</v>
-      </c>
-      <c r="R116">
-        <v>171.17</v>
-      </c>
+      <c r="A116" s="1"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>44715</v>
-      </c>
-      <c r="B117">
-        <v>8665.8009999999995</v>
-      </c>
-      <c r="C117">
-        <v>8524.5400000000009</v>
-      </c>
-      <c r="D117">
-        <v>337.31</v>
-      </c>
-      <c r="E117">
-        <v>4209</v>
-      </c>
-      <c r="F117">
-        <v>157.80000000000001</v>
-      </c>
-      <c r="G117">
-        <v>114.6434</v>
-      </c>
-      <c r="H117">
-        <v>167.83</v>
-      </c>
-      <c r="I117">
-        <v>93.801100000000005</v>
-      </c>
-      <c r="J117">
-        <v>95.553799999999995</v>
-      </c>
-      <c r="K117">
-        <v>128.89189999999999</v>
-      </c>
-      <c r="L117">
-        <v>880.41</v>
-      </c>
-      <c r="M117">
-        <v>1171.57</v>
-      </c>
-      <c r="N117">
-        <v>292.38049999999998</v>
-      </c>
-      <c r="O117">
-        <v>280.87</v>
-      </c>
-      <c r="P117">
-        <v>355.98</v>
-      </c>
-      <c r="Q117">
-        <v>333.82</v>
-      </c>
-      <c r="R117">
-        <v>171.6</v>
-      </c>
+      <c r="A117" s="1"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>44718</v>
-      </c>
-      <c r="B118">
-        <v>8693.0570000000007</v>
-      </c>
-      <c r="C118">
-        <v>8647.91</v>
-      </c>
-      <c r="D118">
-        <v>338.87</v>
-      </c>
-      <c r="E118">
-        <v>4159.0600000000004</v>
-      </c>
-      <c r="F118">
-        <v>154.12</v>
-      </c>
-      <c r="G118">
-        <v>114.5215</v>
-      </c>
-      <c r="H118">
-        <v>168.06</v>
-      </c>
-      <c r="I118">
-        <v>93.754999999999995</v>
-      </c>
-      <c r="J118">
-        <v>95.502300000000005</v>
-      </c>
-      <c r="K118">
-        <v>128.86089999999999</v>
-      </c>
-      <c r="L118">
-        <v>879.61</v>
-      </c>
-      <c r="M118">
-        <v>1169.26</v>
-      </c>
-      <c r="N118">
-        <v>292.55739999999997</v>
-      </c>
-      <c r="O118">
-        <v>280.56</v>
-      </c>
-      <c r="P118">
-        <v>355.64</v>
-      </c>
-      <c r="Q118">
-        <v>333.57</v>
-      </c>
-      <c r="R118">
-        <v>171.44</v>
-      </c>
+      <c r="A118" s="1"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>44719</v>
-      </c>
-      <c r="B119">
-        <v>8776.0889999999999</v>
-      </c>
-      <c r="C119">
-        <v>8576.5400000000009</v>
-      </c>
-      <c r="D119">
-        <v>340.17</v>
-      </c>
-      <c r="E119">
-        <v>4189.1099999999997</v>
-      </c>
-      <c r="F119">
-        <v>156.15</v>
-      </c>
-      <c r="G119">
-        <v>114.7586</v>
-      </c>
-      <c r="H119">
-        <v>168.58</v>
-      </c>
-      <c r="I119">
-        <v>93.699600000000004</v>
-      </c>
-      <c r="J119">
-        <v>95.497900000000001</v>
-      </c>
-      <c r="K119">
-        <v>128.83879999999999</v>
-      </c>
-      <c r="L119">
-        <v>876.67</v>
-      </c>
-      <c r="M119">
-        <v>1166.43</v>
-      </c>
-      <c r="N119">
-        <v>292.2568</v>
-      </c>
-      <c r="O119">
-        <v>280.72000000000003</v>
-      </c>
-      <c r="P119">
-        <v>355.72</v>
-      </c>
-      <c r="Q119">
-        <v>333.68</v>
-      </c>
-      <c r="R119">
-        <v>171.12</v>
-      </c>
+      <c r="A119" s="1"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>44720</v>
-      </c>
-      <c r="B120">
-        <v>8681.6839999999993</v>
-      </c>
-      <c r="C120">
-        <v>8536.41</v>
-      </c>
-      <c r="D120">
-        <v>338.28</v>
-      </c>
-      <c r="E120">
-        <v>4163.7700000000004</v>
-      </c>
-      <c r="F120">
-        <v>154.5</v>
-      </c>
-      <c r="G120">
-        <v>114.1202</v>
-      </c>
-      <c r="H120">
-        <v>168.04</v>
-      </c>
-      <c r="I120">
-        <v>93.687200000000004</v>
-      </c>
-      <c r="J120">
-        <v>95.4452</v>
-      </c>
-      <c r="K120">
-        <v>128.82140000000001</v>
-      </c>
-      <c r="L120">
-        <v>880.71</v>
-      </c>
-      <c r="M120">
-        <v>1165.82</v>
-      </c>
-      <c r="N120">
-        <v>292.07150000000001</v>
-      </c>
-      <c r="O120">
-        <v>280.81</v>
-      </c>
-      <c r="P120">
-        <v>355.86</v>
-      </c>
-      <c r="Q120">
-        <v>333.78</v>
-      </c>
-      <c r="R120">
-        <v>170.97</v>
-      </c>
+      <c r="A120" s="1"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>44721</v>
-      </c>
-      <c r="B121">
-        <v>8475.9120000000003</v>
-      </c>
-      <c r="C121">
-        <v>8391.15</v>
-      </c>
-      <c r="D121">
-        <v>331.46</v>
-      </c>
-      <c r="E121">
-        <v>4155.17</v>
-      </c>
-      <c r="F121">
-        <v>155.22999999999999</v>
-      </c>
-      <c r="G121">
-        <v>113.5078</v>
-      </c>
-      <c r="H121">
-        <v>166.16</v>
-      </c>
-      <c r="I121">
-        <v>93.726100000000002</v>
-      </c>
-      <c r="J121">
-        <v>95.442700000000002</v>
-      </c>
-      <c r="K121">
-        <v>128.83369999999999</v>
-      </c>
-      <c r="L121">
-        <v>888</v>
-      </c>
-      <c r="M121">
-        <v>1163.27</v>
-      </c>
-      <c r="N121">
-        <v>292.18700000000001</v>
-      </c>
-      <c r="O121">
-        <v>279.95999999999998</v>
-      </c>
-      <c r="P121">
-        <v>354.69</v>
-      </c>
-      <c r="Q121">
-        <v>331.73</v>
-      </c>
-      <c r="R121">
-        <v>170.95</v>
-      </c>
+      <c r="A121" s="1"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>44722</v>
-      </c>
-      <c r="B122">
-        <v>8229.4259999999995</v>
-      </c>
-      <c r="C122">
-        <v>8108.95</v>
-      </c>
-      <c r="D122">
-        <v>322.39</v>
-      </c>
-      <c r="E122">
-        <v>4103.08</v>
-      </c>
-      <c r="F122">
-        <v>154.51</v>
-      </c>
-      <c r="G122">
-        <v>112.6748</v>
-      </c>
-      <c r="H122">
-        <v>163.11000000000001</v>
-      </c>
-      <c r="I122">
-        <v>93.967500000000001</v>
-      </c>
-      <c r="J122">
-        <v>95.713200000000001</v>
-      </c>
-      <c r="K122">
-        <v>128.9804</v>
-      </c>
-      <c r="L122">
-        <v>896.63</v>
-      </c>
-      <c r="M122">
-        <v>1163.08</v>
-      </c>
-      <c r="N122">
-        <v>291.24810000000002</v>
-      </c>
-      <c r="O122">
-        <v>279.89999999999998</v>
-      </c>
-      <c r="P122">
-        <v>354.12</v>
-      </c>
-      <c r="Q122">
-        <v>330.55</v>
-      </c>
-      <c r="R122">
-        <v>170.76</v>
-      </c>
+      <c r="A122" s="1"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>44725</v>
-      </c>
-      <c r="B123">
-        <v>7910.4279999999999</v>
-      </c>
-      <c r="C123">
-        <v>7891.09</v>
-      </c>
-      <c r="D123">
-        <v>310.61</v>
-      </c>
-      <c r="E123">
-        <v>3971.49</v>
-      </c>
-      <c r="F123">
-        <v>148.51</v>
-      </c>
-      <c r="G123">
-        <v>112.6353</v>
-      </c>
-      <c r="H123">
-        <v>158.22999999999999</v>
-      </c>
-      <c r="I123">
-        <v>94.820599999999999</v>
-      </c>
-      <c r="J123">
-        <v>96.454300000000003</v>
-      </c>
-      <c r="K123">
-        <v>129.51150000000001</v>
-      </c>
-      <c r="L123">
-        <v>902.34</v>
-      </c>
-      <c r="M123">
-        <v>1155.43</v>
-      </c>
-      <c r="N123">
-        <v>287.24950000000001</v>
-      </c>
-      <c r="O123">
-        <v>277.58999999999997</v>
-      </c>
-      <c r="P123">
-        <v>354.05</v>
-      </c>
-      <c r="Q123">
-        <v>328.14</v>
-      </c>
-      <c r="R123">
-        <v>171.27</v>
-      </c>
+      <c r="A123" s="1"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>44726</v>
-      </c>
-      <c r="B124">
-        <v>7883.3410000000003</v>
-      </c>
-      <c r="C124">
-        <v>7829.55</v>
-      </c>
-      <c r="D124">
-        <v>308.64999999999998</v>
-      </c>
-      <c r="E124">
-        <v>3934.82</v>
-      </c>
-      <c r="F124">
-        <v>146.13</v>
-      </c>
-      <c r="G124">
-        <v>111.511</v>
-      </c>
-      <c r="H124">
-        <v>157.59</v>
-      </c>
-      <c r="I124">
-        <v>94.619900000000001</v>
-      </c>
-      <c r="J124">
-        <v>96.593000000000004</v>
-      </c>
-      <c r="K124">
-        <v>129.4881</v>
-      </c>
-      <c r="L124">
-        <v>904.89</v>
-      </c>
-      <c r="M124">
-        <v>1155.54</v>
-      </c>
-      <c r="N124">
-        <v>287.84039999999999</v>
-      </c>
-      <c r="O124">
-        <v>278.66000000000003</v>
-      </c>
-      <c r="P124">
-        <v>354.4</v>
-      </c>
-      <c r="Q124">
-        <v>330.22</v>
-      </c>
-      <c r="R124">
-        <v>170.85</v>
-      </c>
+      <c r="A124" s="1"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>44727</v>
-      </c>
-      <c r="B125">
-        <v>7998.6189999999997</v>
-      </c>
-      <c r="C125">
-        <v>7958.29</v>
-      </c>
-      <c r="D125">
-        <v>312.06</v>
-      </c>
-      <c r="E125">
-        <v>4009.71</v>
-      </c>
-      <c r="F125">
-        <v>149.38</v>
-      </c>
-      <c r="G125">
-        <v>111.1835</v>
-      </c>
-      <c r="H125">
-        <v>159.43</v>
-      </c>
-      <c r="I125">
-        <v>93.5017</v>
-      </c>
-      <c r="J125">
-        <v>95.749600000000001</v>
-      </c>
-      <c r="K125">
-        <v>128.69110000000001</v>
-      </c>
-      <c r="L125">
-        <v>902.75</v>
-      </c>
-      <c r="M125">
-        <v>1155.08</v>
-      </c>
-      <c r="N125">
-        <v>287.88510000000002</v>
-      </c>
-      <c r="O125">
-        <v>279.43</v>
-      </c>
-      <c r="P125">
-        <v>355.16</v>
-      </c>
-      <c r="Q125">
-        <v>331.32</v>
-      </c>
-      <c r="R125">
-        <v>170.18</v>
-      </c>
+      <c r="A125" s="1"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>44728</v>
-      </c>
-      <c r="B126">
-        <v>7739.3879999999999</v>
-      </c>
-      <c r="C126">
-        <v>7723.05</v>
-      </c>
-      <c r="D126">
-        <v>304.55</v>
-      </c>
-      <c r="E126">
-        <v>4008.65</v>
-      </c>
-      <c r="F126">
-        <v>150.53</v>
-      </c>
-      <c r="G126">
-        <v>111.1417</v>
-      </c>
-      <c r="H126">
-        <v>154.57</v>
-      </c>
-      <c r="I126">
-        <v>94.153099999999995</v>
-      </c>
-      <c r="J126">
-        <v>96.234099999999998</v>
-      </c>
-      <c r="K126">
-        <v>129.26</v>
-      </c>
-      <c r="L126">
-        <v>907.41</v>
-      </c>
-      <c r="M126">
-        <v>1154.82</v>
-      </c>
-      <c r="N126">
-        <v>290.25220000000002</v>
-      </c>
-      <c r="O126">
-        <v>279.32</v>
-      </c>
-      <c r="P126">
-        <v>354.68</v>
-      </c>
-      <c r="Q126">
-        <v>329.89</v>
-      </c>
-      <c r="R126">
-        <v>170.73</v>
-      </c>
+      <c r="A126" s="1"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>44729</v>
-      </c>
-      <c r="B127">
-        <v>7756.5950000000003</v>
-      </c>
-      <c r="C127">
-        <v>7746.82</v>
-      </c>
-      <c r="D127">
-        <v>303.92</v>
-      </c>
-      <c r="E127">
-        <v>4024.97</v>
-      </c>
-      <c r="F127">
-        <v>151.54</v>
-      </c>
-      <c r="G127">
-        <v>110.34229999999999</v>
-      </c>
-      <c r="H127">
-        <v>154.12</v>
-      </c>
-      <c r="I127">
-        <v>93.622399999999999</v>
-      </c>
-      <c r="J127">
-        <v>95.996899999999997</v>
-      </c>
-      <c r="K127">
-        <v>128.7765</v>
-      </c>
-      <c r="L127">
-        <v>908.48</v>
-      </c>
-      <c r="M127">
-        <v>1152.6199999999999</v>
-      </c>
-      <c r="N127">
-        <v>291.83569999999997</v>
-      </c>
-      <c r="O127">
-        <v>279.94</v>
-      </c>
-      <c r="P127">
-        <v>355.87</v>
-      </c>
-      <c r="Q127">
-        <v>331.71</v>
-      </c>
-      <c r="R127">
-        <v>170.12</v>
-      </c>
+      <c r="A127" s="1"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>44732</v>
-      </c>
-      <c r="B128">
-        <v>7756.5950000000003</v>
-      </c>
-      <c r="C128">
-        <v>7817.5</v>
-      </c>
-      <c r="D128">
-        <v>304.77</v>
-      </c>
-      <c r="E128">
-        <v>4024.97</v>
-      </c>
-      <c r="F128">
-        <v>151.54</v>
-      </c>
-      <c r="G128">
-        <v>110.34229999999999</v>
-      </c>
-      <c r="H128">
-        <v>154.12</v>
-      </c>
-      <c r="I128">
-        <v>93.622399999999999</v>
-      </c>
-      <c r="J128">
-        <v>95.996899999999997</v>
-      </c>
-      <c r="K128">
-        <v>128.7765</v>
-      </c>
-      <c r="L128">
-        <v>908.48</v>
-      </c>
-      <c r="M128">
-        <v>1152.6199999999999</v>
-      </c>
-      <c r="N128">
-        <v>291.83569999999997</v>
-      </c>
-      <c r="O128">
-        <v>279.94</v>
-      </c>
-      <c r="P128">
-        <v>355.87</v>
-      </c>
-      <c r="Q128">
-        <v>331.71</v>
-      </c>
-      <c r="R128">
-        <v>170.12</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>44733</v>
-      </c>
-      <c r="B129">
-        <v>7946.8860000000004</v>
-      </c>
-      <c r="C129">
-        <v>7875.87</v>
-      </c>
-      <c r="D129">
-        <v>310.60000000000002</v>
-      </c>
-      <c r="E129">
-        <v>3978.55</v>
-      </c>
-      <c r="F129">
-        <v>147.91999999999999</v>
-      </c>
-      <c r="G129">
-        <v>110.9615</v>
-      </c>
-      <c r="H129">
-        <v>158.63999999999999</v>
-      </c>
-      <c r="I129">
-        <v>93.200299999999999</v>
-      </c>
-      <c r="J129">
-        <v>95.279600000000002</v>
-      </c>
-      <c r="K129">
-        <v>128.37100000000001</v>
-      </c>
-      <c r="L129">
-        <v>903.68</v>
-      </c>
-      <c r="M129">
-        <v>1150.4100000000001</v>
-      </c>
-      <c r="N129">
-        <v>290.11020000000002</v>
-      </c>
-      <c r="O129">
-        <v>279.94</v>
-      </c>
-      <c r="P129">
-        <v>355.35</v>
-      </c>
-      <c r="Q129">
-        <v>331.44</v>
-      </c>
-      <c r="R129">
-        <v>169.56</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>44734</v>
-      </c>
-      <c r="B130">
-        <v>7936.6729999999998</v>
-      </c>
-      <c r="C130">
-        <v>7809.68</v>
-      </c>
-      <c r="D130">
-        <v>309.10000000000002</v>
-      </c>
-      <c r="E130">
-        <v>4028.23</v>
-      </c>
-      <c r="F130">
-        <v>153.07</v>
-      </c>
-      <c r="G130">
-        <v>110.6224</v>
-      </c>
-      <c r="H130">
-        <v>157.65</v>
-      </c>
-      <c r="I130">
-        <v>93.122900000000001</v>
-      </c>
-      <c r="J130">
-        <v>95.2881</v>
-      </c>
-      <c r="K130">
-        <v>128.35980000000001</v>
-      </c>
-      <c r="L130">
-        <v>905.27</v>
-      </c>
-      <c r="M130">
-        <v>1151.96</v>
-      </c>
-      <c r="N130">
-        <v>287.1431</v>
-      </c>
-      <c r="O130">
-        <v>280.23</v>
-      </c>
-      <c r="P130">
-        <v>355.7</v>
-      </c>
-      <c r="Q130">
-        <v>331.79</v>
-      </c>
-      <c r="R130">
-        <v>170.09</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B131">
-        <v>8012.6750000000002</v>
-      </c>
-      <c r="C131">
-        <v>7745.78</v>
-      </c>
-      <c r="D131">
-        <v>310.47000000000003</v>
-      </c>
-      <c r="E131">
-        <v>4050.48</v>
-      </c>
-      <c r="F131">
-        <v>154.78</v>
-      </c>
-      <c r="G131">
-        <v>110.97799999999999</v>
-      </c>
-      <c r="H131">
-        <v>159.47</v>
-      </c>
-      <c r="I131">
-        <v>93.082899999999995</v>
-      </c>
-      <c r="J131">
-        <v>95.198499999999996</v>
-      </c>
-      <c r="K131">
-        <v>128.2911</v>
-      </c>
-      <c r="L131">
-        <v>903</v>
-      </c>
-      <c r="M131">
-        <v>1151.94</v>
-      </c>
-      <c r="N131">
-        <v>286.12720000000002</v>
-      </c>
-      <c r="O131">
-        <v>280.5</v>
-      </c>
-      <c r="P131">
-        <v>356.06</v>
-      </c>
-      <c r="Q131">
-        <v>331.75</v>
-      </c>
-      <c r="R131">
-        <v>169.88</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>44736</v>
-      </c>
-      <c r="B132">
-        <v>8257.723</v>
-      </c>
-      <c r="C132">
-        <v>7964.15</v>
-      </c>
-      <c r="D132">
-        <v>318.63</v>
-      </c>
-      <c r="E132">
-        <v>4031.65</v>
-      </c>
-      <c r="F132">
-        <v>151.78</v>
-      </c>
-      <c r="G132">
-        <v>112.5175</v>
-      </c>
-      <c r="H132">
-        <v>164.04</v>
-      </c>
-      <c r="I132">
-        <v>92.758200000000002</v>
-      </c>
-      <c r="J132">
-        <v>94.878500000000003</v>
-      </c>
-      <c r="K132">
-        <v>128.0573</v>
-      </c>
-      <c r="L132">
-        <v>895.01</v>
-      </c>
-      <c r="M132">
-        <v>1147.28</v>
-      </c>
-      <c r="N132">
-        <v>287.80189999999999</v>
-      </c>
-      <c r="O132">
-        <v>280.39</v>
-      </c>
-      <c r="P132">
-        <v>356.08</v>
-      </c>
-      <c r="Q132">
-        <v>331.87</v>
-      </c>
-      <c r="R132">
-        <v>169.35</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>44739</v>
-      </c>
-      <c r="B133">
-        <v>8233.4210000000003</v>
-      </c>
-      <c r="C133">
-        <v>7977.03</v>
-      </c>
-      <c r="D133">
-        <v>319.64</v>
-      </c>
-      <c r="E133">
-        <v>4002.53</v>
-      </c>
-      <c r="F133">
-        <v>150.22999999999999</v>
-      </c>
-      <c r="G133">
-        <v>111.9072</v>
-      </c>
-      <c r="H133">
-        <v>163.54</v>
-      </c>
-      <c r="I133">
-        <v>92.659000000000006</v>
-      </c>
-      <c r="J133">
-        <v>94.802199999999999</v>
-      </c>
-      <c r="K133">
-        <v>127.98569999999999</v>
-      </c>
-      <c r="L133">
-        <v>896.96</v>
-      </c>
-      <c r="M133">
-        <v>1148.3399999999999</v>
-      </c>
-      <c r="N133">
-        <v>284.53309999999999</v>
-      </c>
-      <c r="O133">
-        <v>280.75</v>
-      </c>
-      <c r="P133">
-        <v>356.54</v>
-      </c>
-      <c r="Q133">
-        <v>332.18</v>
-      </c>
-      <c r="R133">
-        <v>169.59</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>44740</v>
-      </c>
-      <c r="B134">
-        <v>8067.558</v>
-      </c>
-      <c r="C134">
-        <v>8000.5</v>
-      </c>
-      <c r="D134">
-        <v>315.55</v>
-      </c>
-      <c r="E134">
-        <v>4001.91</v>
-      </c>
-      <c r="F134">
-        <v>151.11000000000001</v>
-      </c>
-      <c r="G134">
-        <v>111.3095</v>
-      </c>
-      <c r="H134">
-        <v>160.51</v>
-      </c>
-      <c r="I134">
-        <v>92.689599999999999</v>
-      </c>
-      <c r="J134">
-        <v>94.776899999999998</v>
-      </c>
-      <c r="K134">
-        <v>128.0222</v>
-      </c>
-      <c r="L134">
-        <v>902.32</v>
-      </c>
-      <c r="M134">
-        <v>1152.18</v>
-      </c>
-      <c r="N134">
-        <v>285.69220000000001</v>
-      </c>
-      <c r="O134">
-        <v>280.39</v>
-      </c>
-      <c r="P134">
-        <v>355.77</v>
-      </c>
-      <c r="Q134">
-        <v>332.05</v>
-      </c>
-      <c r="R134">
-        <v>169.78</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>44741</v>
-      </c>
-      <c r="B135">
-        <v>8062.7160000000003</v>
-      </c>
-      <c r="C135">
-        <v>7921.66</v>
-      </c>
-      <c r="D135">
-        <v>314</v>
-      </c>
-      <c r="E135">
-        <v>4035.07</v>
-      </c>
-      <c r="F135">
-        <v>154.1</v>
-      </c>
-      <c r="G135">
-        <v>111.2119</v>
-      </c>
-      <c r="H135">
-        <v>160.46</v>
-      </c>
-      <c r="I135">
-        <v>92.822100000000006</v>
-      </c>
-      <c r="J135">
-        <v>94.894499999999994</v>
-      </c>
-      <c r="K135">
-        <v>128.09729999999999</v>
-      </c>
-      <c r="L135">
-        <v>902.93</v>
-      </c>
-      <c r="M135">
-        <v>1154.01</v>
-      </c>
-      <c r="N135">
-        <v>285.67520000000002</v>
-      </c>
-      <c r="O135">
-        <v>280.72000000000003</v>
-      </c>
-      <c r="P135">
-        <v>356.26</v>
-      </c>
-      <c r="Q135">
-        <v>332.39</v>
-      </c>
-      <c r="R135">
-        <v>170.05</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
-        <v>44742</v>
-      </c>
-      <c r="B136">
-        <v>7993.4309999999996</v>
-      </c>
-      <c r="C136">
-        <v>7787.65</v>
-      </c>
-      <c r="D136">
-        <v>310.52999999999997</v>
-      </c>
-      <c r="E136">
-        <v>4043.14</v>
-      </c>
-      <c r="F136">
-        <v>155.53</v>
-      </c>
-      <c r="G136">
-        <v>111.0522</v>
-      </c>
-      <c r="H136">
-        <v>158.94</v>
-      </c>
-      <c r="I136">
-        <v>92.837500000000006</v>
-      </c>
-      <c r="J136">
-        <v>95.083399999999997</v>
-      </c>
-      <c r="K136">
-        <v>128.1704</v>
-      </c>
-      <c r="L136">
-        <v>903.49</v>
-      </c>
-      <c r="M136">
-        <v>1155.82</v>
-      </c>
-      <c r="N136">
-        <v>285.72050000000002</v>
-      </c>
-      <c r="O136">
-        <v>280.33</v>
-      </c>
-      <c r="P136">
-        <v>355.74</v>
-      </c>
-      <c r="Q136">
-        <v>331.33</v>
-      </c>
-      <c r="R136">
-        <v>169.57</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>44743</v>
-      </c>
-      <c r="B137">
-        <v>8077.8919999999998</v>
-      </c>
-      <c r="C137">
-        <v>7772.86</v>
-      </c>
-      <c r="D137">
-        <v>311.73</v>
-      </c>
-      <c r="E137">
-        <v>4067.56</v>
-      </c>
-      <c r="F137">
-        <v>156.43</v>
-      </c>
-      <c r="G137">
-        <v>111.1767</v>
-      </c>
-      <c r="H137">
-        <v>160.80000000000001</v>
-      </c>
-      <c r="I137">
-        <v>92.722399999999993</v>
-      </c>
-      <c r="J137">
-        <v>94.889799999999994</v>
-      </c>
-      <c r="K137">
-        <v>128.06899999999999</v>
-      </c>
-      <c r="L137">
-        <v>902.1</v>
-      </c>
-      <c r="M137">
-        <v>1155.33</v>
-      </c>
-      <c r="N137">
-        <v>286.02019999999999</v>
-      </c>
-      <c r="O137">
-        <v>280.37</v>
-      </c>
-      <c r="P137">
-        <v>356.08</v>
-      </c>
-      <c r="Q137">
-        <v>332.06</v>
-      </c>
-      <c r="R137">
-        <v>169.94</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
@@ -66372,6 +63860,24 @@
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="1"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="1"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="1"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="1"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="1"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -66379,11 +63885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'Maddie'"
This reverts commit 6563a6a306fa1c463afd83ed0885e26ae0342031, reversing
changes made to 0eaafa34d95aa4634d2cb9a16d23784ceea7fe2f.
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643D30D-9FB0-48F9-A594-8C0065B30B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27DECF7-23E3-47CA-9EBA-D3F71AD177AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1485" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2490" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="SpreadsheetBuilder_2" hidden="1">#REF!</definedName>
     <definedName name="SpreadsheetBuilder_3" localSheetId="3" hidden="1">data_original!$A$1:$Q$1</definedName>
     <definedName name="SpreadsheetBuilder_3" hidden="1">data!$A$1:$Q$1</definedName>
-    <definedName name="SpreadsheetBuilder_6" hidden="1">bbg!$A$1:$R$7</definedName>
+    <definedName name="SpreadsheetBuilder_5" hidden="1">bbg!$A$1:$R$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -171,259 +171,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A Requesting Data...4289900897</v>
-        <stp/>
-        <stp>BDH|10392637733247614934</stp>
-        <tr r="O7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4210468981</v>
-        <stp/>
-        <stp>BDH|18235601751692783007</stp>
-        <tr r="D7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4243158146</v>
-        <stp/>
-        <stp>BDH|18188246218903434165</stp>
-        <tr r="G7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4262598056</v>
-        <stp/>
-        <stp>BDH|11430656411198540119</stp>
-        <tr r="J7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4203105617</v>
-        <stp/>
-        <stp>BDH|17468979122695054421</stp>
-        <tr r="N7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A Requesting Data...4279992330</v>
-        <stp/>
-        <stp>BDH|8854940670218968242</stp>
-        <tr r="E7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4246880534</v>
-        <stp/>
-        <stp>BDH|2134898534232693655</stp>
-        <tr r="M7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4194138881</v>
-        <stp/>
-        <stp>BDH|9968624828340503099</stp>
-        <tr r="P7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4263258258</v>
-        <stp/>
-        <stp>BDH|6524104830009952361</stp>
-        <tr r="A7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4276869603</v>
-        <stp/>
-        <stp>BDH|2379303510707076919</stp>
-        <tr r="H7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4225196147</v>
-        <stp/>
-        <stp>BDH|8869210834791755717</stp>
-        <tr r="I7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4287235548</v>
-        <stp/>
-        <stp>BDH|2377856097898302104</stp>
-        <tr r="L7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4285226797</v>
-        <stp/>
-        <stp>BDH|7445316363007831343</stp>
-        <tr r="Q7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4264218600</v>
-        <stp/>
-        <stp>BDH|3095106220459993904</stp>
-        <tr r="F7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4227452786</v>
-        <stp/>
-        <stp>BDH|4741199751841169303</stp>
-        <tr r="R7" s="4"/>
-      </tp>
-    </main>
-    <main first="bloomberg.rtd">
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C13</stp>
-        <stp>PX_LAST</stp>
-        <tr r="M5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C12</stp>
-        <stp>PX_LAST</stp>
-        <tr r="L5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C11</stp>
-        <stp>PX_LAST</stp>
-        <tr r="K5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C10</stp>
-        <stp>PX_LAST</stp>
-        <tr r="J5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C17</stp>
-        <stp>PX_LAST</stp>
-        <tr r="Q5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C16</stp>
-        <stp>PX_LAST</stp>
-        <tr r="P5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C15</stp>
-        <stp>PX_LAST</stp>
-        <tr r="O5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C14</stp>
-        <stp>PX_LAST</stp>
-        <tr r="N5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C18</stp>
-        <stp>PX_LAST</stp>
-        <tr r="R5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C9</stp>
-        <stp>PX_LAST</stp>
-        <tr r="I5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C8</stp>
-        <stp>PX_LAST</stp>
-        <tr r="H5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C3</stp>
-        <stp>PX_LAST</stp>
-        <tr r="C5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C2</stp>
-        <stp>PX_LAST</stp>
-        <tr r="B5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C7</stp>
-        <stp>PX_LAST</stp>
-        <tr r="G5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C6</stp>
-        <stp>PX_LAST</stp>
-        <tr r="F5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C5</stp>
-        <stp>PX_LAST</stp>
-        <tr r="E5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C4</stp>
-        <stp>PX_LAST</stp>
-        <tr r="D5" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A Requesting Data...1334743677</v>
-        <stp/>
-        <stp>BDH|274322730555081536</stp>
-        <tr r="K7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...2240291399</v>
-        <stp/>
-        <stp>BDH|882341662994038285</stp>
-        <tr r="C7" s="4"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q175"/>
+  <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B140" workbookViewId="0">
-      <selection activeCell="R154" sqref="R154:R175"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8769,1225 +8516,6 @@
         <v>334.43</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A153" s="1">
-        <v>44774</v>
-      </c>
-      <c r="B153">
-        <v>8705.8739999999998</v>
-      </c>
-      <c r="C153">
-        <v>8363.6200000000008</v>
-      </c>
-      <c r="D153">
-        <v>332.58</v>
-      </c>
-      <c r="E153">
-        <v>4296.6899999999996</v>
-      </c>
-      <c r="F153">
-        <v>164.74</v>
-      </c>
-      <c r="G153">
-        <v>112.66970000000001</v>
-      </c>
-      <c r="H153">
-        <v>164.17</v>
-      </c>
-      <c r="I153">
-        <v>91.878799999999998</v>
-      </c>
-      <c r="J153">
-        <v>93.916300000000007</v>
-      </c>
-      <c r="K153">
-        <v>127.5063</v>
-      </c>
-      <c r="L153">
-        <v>883.27</v>
-      </c>
-      <c r="M153">
-        <v>1142.3699999999999</v>
-      </c>
-      <c r="N153">
-        <v>283.7835</v>
-      </c>
-      <c r="O153">
-        <v>281.25</v>
-      </c>
-      <c r="P153">
-        <v>357.93</v>
-      </c>
-      <c r="Q153">
-        <v>334.82</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A154" s="1">
-        <v>44775</v>
-      </c>
-      <c r="B154">
-        <v>8647.9089999999997</v>
-      </c>
-      <c r="C154">
-        <v>8314.01</v>
-      </c>
-      <c r="D154">
-        <v>329.93</v>
-      </c>
-      <c r="E154">
-        <v>4220.7</v>
-      </c>
-      <c r="F154">
-        <v>160.71</v>
-      </c>
-      <c r="G154">
-        <v>112.7552</v>
-      </c>
-      <c r="H154">
-        <v>164.11</v>
-      </c>
-      <c r="I154">
-        <v>91.885199999999998</v>
-      </c>
-      <c r="J154">
-        <v>93.963099999999997</v>
-      </c>
-      <c r="K154">
-        <v>127.5134</v>
-      </c>
-      <c r="L154">
-        <v>884.32</v>
-      </c>
-      <c r="M154">
-        <v>1143.08</v>
-      </c>
-      <c r="N154">
-        <v>283.39949999999999</v>
-      </c>
-      <c r="O154">
-        <v>281.45</v>
-      </c>
-      <c r="P154">
-        <v>357.92</v>
-      </c>
-      <c r="Q154">
-        <v>335.23</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A155" s="1">
-        <v>44776</v>
-      </c>
-      <c r="B155">
-        <v>8783.2839999999997</v>
-      </c>
-      <c r="C155">
-        <v>8422.1200000000008</v>
-      </c>
-      <c r="D155">
-        <v>332.9</v>
-      </c>
-      <c r="E155">
-        <v>4277.07</v>
-      </c>
-      <c r="F155">
-        <v>164.16</v>
-      </c>
-      <c r="G155">
-        <v>112.8616</v>
-      </c>
-      <c r="H155">
-        <v>164.17</v>
-      </c>
-      <c r="I155">
-        <v>91.796300000000002</v>
-      </c>
-      <c r="J155">
-        <v>93.831400000000002</v>
-      </c>
-      <c r="K155">
-        <v>127.47369999999999</v>
-      </c>
-      <c r="L155">
-        <v>881.43</v>
-      </c>
-      <c r="M155">
-        <v>1144.95</v>
-      </c>
-      <c r="N155">
-        <v>283.7593</v>
-      </c>
-      <c r="O155">
-        <v>281.41000000000003</v>
-      </c>
-      <c r="P155">
-        <v>358.02</v>
-      </c>
-      <c r="Q155">
-        <v>334.95</v>
-      </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A156" s="1">
-        <v>44777</v>
-      </c>
-      <c r="B156">
-        <v>8777.2270000000008</v>
-      </c>
-      <c r="C156">
-        <v>8473.32</v>
-      </c>
-      <c r="D156">
-        <v>333.95</v>
-      </c>
-      <c r="E156">
-        <v>4277.0200000000004</v>
-      </c>
-      <c r="F156">
-        <v>163.69</v>
-      </c>
-      <c r="G156">
-        <v>112.8156</v>
-      </c>
-      <c r="H156">
-        <v>164.23</v>
-      </c>
-      <c r="I156">
-        <v>91.813800000000001</v>
-      </c>
-      <c r="J156">
-        <v>93.827100000000002</v>
-      </c>
-      <c r="K156">
-        <v>127.4787</v>
-      </c>
-      <c r="L156">
-        <v>881.65</v>
-      </c>
-      <c r="M156">
-        <v>1146.56</v>
-      </c>
-      <c r="N156">
-        <v>283.81979999999999</v>
-      </c>
-      <c r="O156">
-        <v>281.73</v>
-      </c>
-      <c r="P156">
-        <v>358.45</v>
-      </c>
-      <c r="Q156">
-        <v>335.16</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A157" s="1">
-        <v>44778</v>
-      </c>
-      <c r="B157">
-        <v>8764.0820000000003</v>
-      </c>
-      <c r="C157">
-        <v>8407.4</v>
-      </c>
-      <c r="D157">
-        <v>333.24</v>
-      </c>
-      <c r="E157">
-        <v>4197.07</v>
-      </c>
-      <c r="F157">
-        <v>159.1</v>
-      </c>
-      <c r="G157">
-        <v>112.5962</v>
-      </c>
-      <c r="H157">
-        <v>164.17</v>
-      </c>
-      <c r="I157">
-        <v>91.774100000000004</v>
-      </c>
-      <c r="J157">
-        <v>93.788799999999995</v>
-      </c>
-      <c r="K157">
-        <v>127.4599</v>
-      </c>
-      <c r="L157">
-        <v>882.16</v>
-      </c>
-      <c r="M157">
-        <v>1144.69</v>
-      </c>
-      <c r="N157">
-        <v>283.7833</v>
-      </c>
-      <c r="O157">
-        <v>281.98</v>
-      </c>
-      <c r="P157">
-        <v>358.77</v>
-      </c>
-      <c r="Q157">
-        <v>335.51</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A158" s="1">
-        <v>44781</v>
-      </c>
-      <c r="B158">
-        <v>8753.393</v>
-      </c>
-      <c r="C158">
-        <v>8480.9599999999991</v>
-      </c>
-      <c r="D158">
-        <v>333.93</v>
-      </c>
-      <c r="E158">
-        <v>4238.93</v>
-      </c>
-      <c r="F158">
-        <v>162.30000000000001</v>
-      </c>
-      <c r="G158">
-        <v>112.59910000000001</v>
-      </c>
-      <c r="H158">
-        <v>164.19</v>
-      </c>
-      <c r="I158">
-        <v>91.7637</v>
-      </c>
-      <c r="J158">
-        <v>93.765199999999993</v>
-      </c>
-      <c r="K158">
-        <v>127.44280000000001</v>
-      </c>
-      <c r="L158">
-        <v>882.2</v>
-      </c>
-      <c r="M158">
-        <v>1143.3399999999999</v>
-      </c>
-      <c r="N158">
-        <v>283.74579999999997</v>
-      </c>
-      <c r="O158">
-        <v>282.18</v>
-      </c>
-      <c r="P158">
-        <v>359.11</v>
-      </c>
-      <c r="Q158">
-        <v>335.75</v>
-      </c>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A159" s="1">
-        <v>44782</v>
-      </c>
-      <c r="B159">
-        <v>8716.7510000000002</v>
-      </c>
-      <c r="C159">
-        <v>8386.49</v>
-      </c>
-      <c r="D159">
-        <v>332.31</v>
-      </c>
-      <c r="E159">
-        <v>4217.03</v>
-      </c>
-      <c r="F159">
-        <v>161.62</v>
-      </c>
-      <c r="G159">
-        <v>112.4363</v>
-      </c>
-      <c r="H159">
-        <v>164.2</v>
-      </c>
-      <c r="I159">
-        <v>91.772300000000001</v>
-      </c>
-      <c r="J159">
-        <v>93.783199999999994</v>
-      </c>
-      <c r="K159">
-        <v>127.4515</v>
-      </c>
-      <c r="L159">
-        <v>882.85</v>
-      </c>
-      <c r="M159">
-        <v>1144.8499999999999</v>
-      </c>
-      <c r="N159">
-        <v>283.67189999999999</v>
-      </c>
-      <c r="O159">
-        <v>282.29000000000002</v>
-      </c>
-      <c r="P159">
-        <v>359.06</v>
-      </c>
-      <c r="Q159">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A160" s="1">
-        <v>44783</v>
-      </c>
-      <c r="B160">
-        <v>8902.723</v>
-      </c>
-      <c r="C160">
-        <v>8463.18</v>
-      </c>
-      <c r="D160">
-        <v>338.6</v>
-      </c>
-      <c r="E160">
-        <v>4228.0600000000004</v>
-      </c>
-      <c r="F160">
-        <v>160</v>
-      </c>
-      <c r="G160">
-        <v>112.8806</v>
-      </c>
-      <c r="H160">
-        <v>164.25</v>
-      </c>
-      <c r="I160">
-        <v>91.653800000000004</v>
-      </c>
-      <c r="J160">
-        <v>93.670699999999997</v>
-      </c>
-      <c r="K160">
-        <v>127.38979999999999</v>
-      </c>
-      <c r="L160">
-        <v>879.76</v>
-      </c>
-      <c r="M160">
-        <v>1141.68</v>
-      </c>
-      <c r="N160">
-        <v>283.73329999999999</v>
-      </c>
-      <c r="O160">
-        <v>282.02</v>
-      </c>
-      <c r="P160">
-        <v>358.84</v>
-      </c>
-      <c r="Q160">
-        <v>335.55</v>
-      </c>
-    </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A161" s="1">
-        <v>44784</v>
-      </c>
-      <c r="B161">
-        <v>8898.8369999999995</v>
-      </c>
-      <c r="C161">
-        <v>8480.57</v>
-      </c>
-      <c r="D161">
-        <v>339.2</v>
-      </c>
-      <c r="E161">
-        <v>4182.1499999999996</v>
-      </c>
-      <c r="F161">
-        <v>155.05000000000001</v>
-      </c>
-      <c r="G161">
-        <v>113.005</v>
-      </c>
-      <c r="H161">
-        <v>164.25</v>
-      </c>
-      <c r="I161">
-        <v>91.656999999999996</v>
-      </c>
-      <c r="J161">
-        <v>93.661299999999997</v>
-      </c>
-      <c r="K161">
-        <v>127.3886</v>
-      </c>
-      <c r="L161">
-        <v>879.67</v>
-      </c>
-      <c r="M161">
-        <v>1143.45</v>
-      </c>
-      <c r="N161">
-        <v>284.00580000000002</v>
-      </c>
-      <c r="O161">
-        <v>281.82</v>
-      </c>
-      <c r="P161">
-        <v>358.55</v>
-      </c>
-      <c r="Q161">
-        <v>335.15</v>
-      </c>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A162" s="1">
-        <v>44785</v>
-      </c>
-      <c r="B162">
-        <v>9054.1380000000008</v>
-      </c>
-      <c r="C162">
-        <v>8526.42</v>
-      </c>
-      <c r="D162">
-        <v>342.89</v>
-      </c>
-      <c r="E162">
-        <v>4227.76</v>
-      </c>
-      <c r="F162">
-        <v>157.05000000000001</v>
-      </c>
-      <c r="G162">
-        <v>113.5121</v>
-      </c>
-      <c r="H162">
-        <v>164.38</v>
-      </c>
-      <c r="I162">
-        <v>91.620500000000007</v>
-      </c>
-      <c r="J162">
-        <v>93.633799999999994</v>
-      </c>
-      <c r="K162">
-        <v>127.36879999999999</v>
-      </c>
-      <c r="L162">
-        <v>877.68</v>
-      </c>
-      <c r="M162">
-        <v>1138.8599999999999</v>
-      </c>
-      <c r="N162">
-        <v>284.35640000000001</v>
-      </c>
-      <c r="O162">
-        <v>281.73</v>
-      </c>
-      <c r="P162">
-        <v>358.53</v>
-      </c>
-      <c r="Q162">
-        <v>335.23</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A163" s="1">
-        <v>44788</v>
-      </c>
-      <c r="B163">
-        <v>9090.3610000000008</v>
-      </c>
-      <c r="C163">
-        <v>8555.33</v>
-      </c>
-      <c r="D163">
-        <v>343.69</v>
-      </c>
-      <c r="E163">
-        <v>4237.04</v>
-      </c>
-      <c r="F163">
-        <v>156.78</v>
-      </c>
-      <c r="G163">
-        <v>113.54300000000001</v>
-      </c>
-      <c r="H163">
-        <v>164.28</v>
-      </c>
-      <c r="I163">
-        <v>91.620999999999995</v>
-      </c>
-      <c r="J163">
-        <v>93.638400000000004</v>
-      </c>
-      <c r="K163">
-        <v>127.3695</v>
-      </c>
-      <c r="L163">
-        <v>877.44</v>
-      </c>
-      <c r="M163">
-        <v>1138.67</v>
-      </c>
-      <c r="N163">
-        <v>283.9357</v>
-      </c>
-      <c r="O163">
-        <v>281.91000000000003</v>
-      </c>
-      <c r="P163">
-        <v>358.73</v>
-      </c>
-      <c r="Q163">
-        <v>335.44</v>
-      </c>
-    </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A164" s="1">
-        <v>44789</v>
-      </c>
-      <c r="B164">
-        <v>9107.8670000000002</v>
-      </c>
-      <c r="C164">
-        <v>8590.56</v>
-      </c>
-      <c r="D164">
-        <v>343.89</v>
-      </c>
-      <c r="E164">
-        <v>4237.16</v>
-      </c>
-      <c r="F164">
-        <v>157.85</v>
-      </c>
-      <c r="G164">
-        <v>113.5821</v>
-      </c>
-      <c r="H164">
-        <v>164.29</v>
-      </c>
-      <c r="I164">
-        <v>91.624799999999993</v>
-      </c>
-      <c r="J164">
-        <v>93.634299999999996</v>
-      </c>
-      <c r="K164">
-        <v>127.37260000000001</v>
-      </c>
-      <c r="L164">
-        <v>877.33</v>
-      </c>
-      <c r="M164">
-        <v>1137.5899999999999</v>
-      </c>
-      <c r="N164">
-        <v>283.93880000000001</v>
-      </c>
-      <c r="O164">
-        <v>282.08999999999997</v>
-      </c>
-      <c r="P164">
-        <v>358.89</v>
-      </c>
-      <c r="Q164">
-        <v>335.68</v>
-      </c>
-    </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A165" s="1">
-        <v>44790</v>
-      </c>
-      <c r="B165">
-        <v>9043.5889999999999</v>
-      </c>
-      <c r="C165">
-        <v>8479.58</v>
-      </c>
-      <c r="D165">
-        <v>341.66</v>
-      </c>
-      <c r="E165">
-        <v>4188.9799999999996</v>
-      </c>
-      <c r="F165">
-        <v>155.69</v>
-      </c>
-      <c r="G165">
-        <v>113.5885</v>
-      </c>
-      <c r="H165">
-        <v>164.08</v>
-      </c>
-      <c r="I165">
-        <v>91.628600000000006</v>
-      </c>
-      <c r="J165">
-        <v>93.632599999999996</v>
-      </c>
-      <c r="K165">
-        <v>127.377</v>
-      </c>
-      <c r="L165">
-        <v>878.03</v>
-      </c>
-      <c r="M165">
-        <v>1138.46</v>
-      </c>
-      <c r="N165">
-        <v>283.50299999999999</v>
-      </c>
-      <c r="O165">
-        <v>282.12</v>
-      </c>
-      <c r="P165">
-        <v>358.88</v>
-      </c>
-      <c r="Q165">
-        <v>335.82</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A166" s="1">
-        <v>44791</v>
-      </c>
-      <c r="B166">
-        <v>9065.49</v>
-      </c>
-      <c r="C166">
-        <v>8527.7000000000007</v>
-      </c>
-      <c r="D166">
-        <v>341.89</v>
-      </c>
-      <c r="E166">
-        <v>4195.88</v>
-      </c>
-      <c r="F166">
-        <v>155.88999999999999</v>
-      </c>
-      <c r="G166">
-        <v>113.4795</v>
-      </c>
-      <c r="H166">
-        <v>164.13</v>
-      </c>
-      <c r="I166">
-        <v>91.601500000000001</v>
-      </c>
-      <c r="J166">
-        <v>93.622600000000006</v>
-      </c>
-      <c r="K166">
-        <v>127.35680000000001</v>
-      </c>
-      <c r="L166">
-        <v>877.94</v>
-      </c>
-      <c r="M166">
-        <v>1138.22</v>
-      </c>
-      <c r="N166">
-        <v>283.584</v>
-      </c>
-      <c r="O166">
-        <v>282.27999999999997</v>
-      </c>
-      <c r="P166">
-        <v>359.17</v>
-      </c>
-      <c r="Q166">
-        <v>336.14</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A167" s="1">
-        <v>44792</v>
-      </c>
-      <c r="B167">
-        <v>8948.8179999999993</v>
-      </c>
-      <c r="C167">
-        <v>8421.4699999999993</v>
-      </c>
-      <c r="D167">
-        <v>337.42</v>
-      </c>
-      <c r="E167">
-        <v>4132.21</v>
-      </c>
-      <c r="F167">
-        <v>152.77000000000001</v>
-      </c>
-      <c r="G167">
-        <v>113.3695</v>
-      </c>
-      <c r="H167">
-        <v>164.09</v>
-      </c>
-      <c r="I167">
-        <v>91.6524</v>
-      </c>
-      <c r="J167">
-        <v>93.679500000000004</v>
-      </c>
-      <c r="K167">
-        <v>127.3942</v>
-      </c>
-      <c r="L167">
-        <v>879.18</v>
-      </c>
-      <c r="M167">
-        <v>1137.3699999999999</v>
-      </c>
-      <c r="N167">
-        <v>283.77629999999999</v>
-      </c>
-      <c r="O167">
-        <v>282.26</v>
-      </c>
-      <c r="P167">
-        <v>359.09</v>
-      </c>
-      <c r="Q167">
-        <v>335.99</v>
-      </c>
-    </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A168" s="1">
-        <v>44795</v>
-      </c>
-      <c r="B168">
-        <v>8758.2430000000004</v>
-      </c>
-      <c r="C168">
-        <v>8258.69</v>
-      </c>
-      <c r="D168">
-        <v>331.53</v>
-      </c>
-      <c r="E168">
-        <v>4100.78</v>
-      </c>
-      <c r="F168">
-        <v>152.16</v>
-      </c>
-      <c r="G168">
-        <v>112.8489</v>
-      </c>
-      <c r="H168">
-        <v>163.65</v>
-      </c>
-      <c r="I168">
-        <v>91.783199999999994</v>
-      </c>
-      <c r="J168">
-        <v>93.810299999999998</v>
-      </c>
-      <c r="K168">
-        <v>127.4551</v>
-      </c>
-      <c r="L168">
-        <v>881.66</v>
-      </c>
-      <c r="M168">
-        <v>1137.31</v>
-      </c>
-      <c r="N168">
-        <v>282.39870000000002</v>
-      </c>
-      <c r="O168">
-        <v>281.58</v>
-      </c>
-      <c r="P168">
-        <v>359.12</v>
-      </c>
-      <c r="Q168">
-        <v>335.71</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A169" s="1">
-        <v>44796</v>
-      </c>
-      <c r="B169">
-        <v>8738.7630000000008</v>
-      </c>
-      <c r="C169">
-        <v>8245.83</v>
-      </c>
-      <c r="D169">
-        <v>330.83</v>
-      </c>
-      <c r="E169">
-        <v>4090.63</v>
-      </c>
-      <c r="F169">
-        <v>151.13</v>
-      </c>
-      <c r="G169">
-        <v>112.38030000000001</v>
-      </c>
-      <c r="H169">
-        <v>163.33000000000001</v>
-      </c>
-      <c r="I169">
-        <v>91.73</v>
-      </c>
-      <c r="J169">
-        <v>93.707599999999999</v>
-      </c>
-      <c r="K169">
-        <v>127.4281</v>
-      </c>
-      <c r="L169">
-        <v>882.34</v>
-      </c>
-      <c r="M169">
-        <v>1136.7</v>
-      </c>
-      <c r="N169">
-        <v>282.93119999999999</v>
-      </c>
-      <c r="O169">
-        <v>281.99</v>
-      </c>
-      <c r="P169">
-        <v>359.29</v>
-      </c>
-      <c r="Q169">
-        <v>336.35</v>
-      </c>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A170" s="1">
-        <v>44797</v>
-      </c>
-      <c r="B170">
-        <v>8764.42</v>
-      </c>
-      <c r="C170">
-        <v>8279.5499999999993</v>
-      </c>
-      <c r="D170">
-        <v>331.29</v>
-      </c>
-      <c r="E170">
-        <v>4076.99</v>
-      </c>
-      <c r="F170">
-        <v>149.65</v>
-      </c>
-      <c r="G170">
-        <v>112.1097</v>
-      </c>
-      <c r="H170">
-        <v>163.25</v>
-      </c>
-      <c r="I170">
-        <v>91.584100000000007</v>
-      </c>
-      <c r="J170">
-        <v>93.628100000000003</v>
-      </c>
-      <c r="K170">
-        <v>127.3526</v>
-      </c>
-      <c r="L170">
-        <v>882.25</v>
-      </c>
-      <c r="M170">
-        <v>1136.58</v>
-      </c>
-      <c r="N170">
-        <v>283.32589999999999</v>
-      </c>
-      <c r="O170">
-        <v>282.39999999999998</v>
-      </c>
-      <c r="P170">
-        <v>359.77</v>
-      </c>
-      <c r="Q170">
-        <v>336.56</v>
-      </c>
-    </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A171" s="1">
-        <v>44798</v>
-      </c>
-      <c r="B171">
-        <v>8888.1280000000006</v>
-      </c>
-      <c r="C171">
-        <v>8295.5400000000009</v>
-      </c>
-      <c r="D171">
-        <v>335.48</v>
-      </c>
-      <c r="E171">
-        <v>4127.1400000000003</v>
-      </c>
-      <c r="F171">
-        <v>152.35</v>
-      </c>
-      <c r="G171">
-        <v>112.3784</v>
-      </c>
-      <c r="H171">
-        <v>163.52000000000001</v>
-      </c>
-      <c r="I171">
-        <v>91.489199999999997</v>
-      </c>
-      <c r="J171">
-        <v>93.480199999999996</v>
-      </c>
-      <c r="K171">
-        <v>127.29259999999999</v>
-      </c>
-      <c r="L171">
-        <v>879.89</v>
-      </c>
-      <c r="M171">
-        <v>1134.26</v>
-      </c>
-      <c r="N171">
-        <v>282.47680000000003</v>
-      </c>
-      <c r="O171">
-        <v>281.86</v>
-      </c>
-      <c r="P171">
-        <v>359.18</v>
-      </c>
-      <c r="Q171">
-        <v>335.96</v>
-      </c>
-    </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A172" s="1">
-        <v>44799</v>
-      </c>
-      <c r="B172">
-        <v>8588.9459999999999</v>
-      </c>
-      <c r="C172">
-        <v>8135.58</v>
-      </c>
-      <c r="D172">
-        <v>327.63</v>
-      </c>
-      <c r="E172">
-        <v>4131.16</v>
-      </c>
-      <c r="F172">
-        <v>154.22</v>
-      </c>
-      <c r="G172">
-        <v>112.1219</v>
-      </c>
-      <c r="H172">
-        <v>162.63</v>
-      </c>
-      <c r="I172">
-        <v>91.706000000000003</v>
-      </c>
-      <c r="J172">
-        <v>93.591999999999999</v>
-      </c>
-      <c r="K172">
-        <v>127.38809999999999</v>
-      </c>
-      <c r="L172">
-        <v>885.23</v>
-      </c>
-      <c r="M172">
-        <v>1135.52</v>
-      </c>
-      <c r="N172">
-        <v>284.0487</v>
-      </c>
-      <c r="O172">
-        <v>282.58</v>
-      </c>
-      <c r="P172">
-        <v>359.94</v>
-      </c>
-      <c r="Q172">
-        <v>336.02</v>
-      </c>
-    </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A173" s="1">
-        <v>44802</v>
-      </c>
-      <c r="B173">
-        <v>8532.1020000000008</v>
-      </c>
-      <c r="C173">
-        <v>8060.68</v>
-      </c>
-      <c r="D173">
-        <v>324.31</v>
-      </c>
-      <c r="E173">
-        <v>4088.08</v>
-      </c>
-      <c r="F173">
-        <v>152.58000000000001</v>
-      </c>
-      <c r="G173">
-        <v>111.52509999999999</v>
-      </c>
-      <c r="H173">
-        <v>162.13999999999999</v>
-      </c>
-      <c r="I173">
-        <v>91.723500000000001</v>
-      </c>
-      <c r="J173">
-        <v>93.755799999999994</v>
-      </c>
-      <c r="K173">
-        <v>127.4524</v>
-      </c>
-      <c r="L173">
-        <v>887.12</v>
-      </c>
-      <c r="M173">
-        <v>1133.95</v>
-      </c>
-      <c r="N173">
-        <v>284.16669999999999</v>
-      </c>
-      <c r="O173">
-        <v>283.06</v>
-      </c>
-      <c r="P173">
-        <v>360.56</v>
-      </c>
-      <c r="Q173">
-        <v>337.07</v>
-      </c>
-    </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A174" s="1">
-        <v>44803</v>
-      </c>
-      <c r="B174">
-        <v>8438.6869999999999</v>
-      </c>
-      <c r="C174">
-        <v>8041.3</v>
-      </c>
-      <c r="D174">
-        <v>321.83999999999997</v>
-      </c>
-      <c r="E174">
-        <v>4090.08</v>
-      </c>
-      <c r="F174">
-        <v>153.38999999999999</v>
-      </c>
-      <c r="G174">
-        <v>110.976</v>
-      </c>
-      <c r="H174">
-        <v>161.75</v>
-      </c>
-      <c r="I174">
-        <v>91.882199999999997</v>
-      </c>
-      <c r="J174">
-        <v>93.805899999999994</v>
-      </c>
-      <c r="K174">
-        <v>127.5065</v>
-      </c>
-      <c r="L174">
-        <v>889.74</v>
-      </c>
-      <c r="M174">
-        <v>1133.72</v>
-      </c>
-      <c r="N174">
-        <v>284.59399999999999</v>
-      </c>
-      <c r="O174">
-        <v>282.89999999999998</v>
-      </c>
-      <c r="P174">
-        <v>360.03</v>
-      </c>
-      <c r="Q174">
-        <v>336.89</v>
-      </c>
-    </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A175" s="1">
-        <v>44804</v>
-      </c>
-      <c r="B175">
-        <v>8374.4159999999993</v>
-      </c>
-      <c r="C175">
-        <v>7940.45</v>
-      </c>
-      <c r="D175">
-        <v>319.98</v>
-      </c>
-      <c r="E175">
-        <v>4046.99</v>
-      </c>
-      <c r="F175">
-        <v>151.47</v>
-      </c>
-      <c r="G175">
-        <v>110.51479999999999</v>
-      </c>
-      <c r="H175">
-        <v>161.09</v>
-      </c>
-      <c r="I175">
-        <v>91.6631</v>
-      </c>
-      <c r="J175">
-        <v>93.6631</v>
-      </c>
-      <c r="K175">
-        <v>127.4104</v>
-      </c>
-      <c r="L175">
-        <v>892.53</v>
-      </c>
-      <c r="M175">
-        <v>1134.3499999999999</v>
-      </c>
-      <c r="N175">
-        <v>285.5609</v>
-      </c>
-      <c r="O175">
-        <v>283.08999999999997</v>
-      </c>
-      <c r="P175">
-        <v>360.47</v>
-      </c>
-      <c r="Q175">
-        <v>337.21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60569,8 +59097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R283"/>
   <sheetViews>
-    <sheetView topLeftCell="M145" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17:Q180"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -60606,7 +59134,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>44804</v>
+        <v>44774</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -60664,72 +59192,72 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" t="e">
-        <f>_xll.BFieldInfo(B$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(B$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="C5" t="e">
-        <f>_xll.BFieldInfo(C$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(C$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="D5" t="e">
-        <f>_xll.BFieldInfo(D$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(D$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="E5" t="e">
-        <f>_xll.BFieldInfo(E$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(E$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F5" t="e">
-        <f>_xll.BFieldInfo(F$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(F$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="G5" t="e">
-        <f>_xll.BFieldInfo(G$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(G$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="H5" t="e">
-        <f>_xll.BFieldInfo(H$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(H$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I5" t="e">
-        <f>_xll.BFieldInfo(I$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(I$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="J5" t="e">
-        <f>_xll.BFieldInfo(J$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(J$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="K5" t="e">
-        <f>_xll.BFieldInfo(K$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(K$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="L5" t="e">
-        <f>_xll.BFieldInfo(L$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(L$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="M5" t="e">
-        <f>_xll.BFieldInfo(M$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(M$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N5" t="e">
-        <f>_xll.BFieldInfo(N$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(N$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="O5" t="e">
-        <f>_xll.BFieldInfo(O$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(O$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P5" t="e">
-        <f>_xll.BFieldInfo(P$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(P$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="Q5" t="e">
-        <f>_xll.BFieldInfo(Q$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(Q$6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R5" t="e">
-        <f>_xll.BFieldInfo(R$6)</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.BFieldInfo(R$6)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -60789,76 +59317,76 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="str">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
+      <c r="A7" s="1" t="e">
+        <f ca="1">_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=152")</f>
+        <v>#NAME?</v>
       </c>
       <c r="B7">
         <v>9986.6980000000003</v>
       </c>
-      <c r="C7" t="str">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="E7" t="str">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="F7" t="str">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="G7" t="str">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="H7" t="str">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="I7" t="str">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="J7" t="str">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="K7" t="str">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="L7" t="str">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="M7" t="str">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="N7" t="str">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="O7" t="str">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="P7" t="str">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="Q7" t="str">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
-      </c>
-      <c r="R7" t="str">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=174")</f>
-        <v>#N/A Requesting Data...</v>
+      <c r="C7" t="e">
+        <f ca="1">_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D7" t="e">
+        <f ca="1">_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E7" t="e">
+        <f ca="1">_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F7" t="e">
+        <f ca="1">_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G7" t="e">
+        <f ca="1">_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H7" t="e">
+        <f ca="1">_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I7" t="e">
+        <f ca="1">_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J7" t="e">
+        <f ca="1">_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K7" t="e">
+        <f ca="1">_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L7" t="e">
+        <f ca="1">_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M7" t="e">
+        <f ca="1">_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N7" t="e">
+        <f ca="1">_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O7" t="e">
+        <f ca="1">_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P7" t="e">
+        <f ca="1">_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q7" t="e">
+        <f ca="1">_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R7" t="e">
+        <f ca="1">_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=152")</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -69318,1271 +67846,105 @@
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A159" s="1">
-        <v>44775</v>
-      </c>
-      <c r="B159">
-        <v>8647.9089999999997</v>
-      </c>
-      <c r="C159">
-        <v>8314.01</v>
-      </c>
-      <c r="D159">
-        <v>329.93</v>
-      </c>
-      <c r="E159">
-        <v>4220.7</v>
-      </c>
-      <c r="F159">
-        <v>160.71</v>
-      </c>
-      <c r="G159">
-        <v>112.7552</v>
-      </c>
-      <c r="H159">
-        <v>164.11</v>
-      </c>
-      <c r="I159">
-        <v>91.885199999999998</v>
-      </c>
-      <c r="J159">
-        <v>93.963099999999997</v>
-      </c>
-      <c r="K159">
-        <v>127.5134</v>
-      </c>
-      <c r="L159">
-        <v>884.32</v>
-      </c>
-      <c r="M159">
-        <v>1143.08</v>
-      </c>
-      <c r="N159">
-        <v>283.39949999999999</v>
-      </c>
-      <c r="O159">
-        <v>281.45</v>
-      </c>
-      <c r="P159">
-        <v>357.92</v>
-      </c>
-      <c r="Q159">
-        <v>335.23</v>
-      </c>
-      <c r="R159">
-        <v>168.75</v>
-      </c>
+      <c r="A159" s="1"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A160" s="1">
-        <v>44776</v>
-      </c>
-      <c r="B160">
-        <v>8783.2839999999997</v>
-      </c>
-      <c r="C160">
-        <v>8422.1200000000008</v>
-      </c>
-      <c r="D160">
-        <v>332.9</v>
-      </c>
-      <c r="E160">
-        <v>4277.07</v>
-      </c>
-      <c r="F160">
-        <v>164.16</v>
-      </c>
-      <c r="G160">
-        <v>112.8616</v>
-      </c>
-      <c r="H160">
-        <v>164.17</v>
-      </c>
-      <c r="I160">
-        <v>91.796300000000002</v>
-      </c>
-      <c r="J160">
-        <v>93.831400000000002</v>
-      </c>
-      <c r="K160">
-        <v>127.47369999999999</v>
-      </c>
-      <c r="L160">
-        <v>881.43</v>
-      </c>
-      <c r="M160">
-        <v>1144.95</v>
-      </c>
-      <c r="N160">
-        <v>283.7593</v>
-      </c>
-      <c r="O160">
-        <v>281.41000000000003</v>
-      </c>
-      <c r="P160">
-        <v>358.02</v>
-      </c>
-      <c r="Q160">
-        <v>334.95</v>
-      </c>
-      <c r="R160">
-        <v>169.23</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A161" s="1">
-        <v>44777</v>
-      </c>
-      <c r="B161">
-        <v>8777.2270000000008</v>
-      </c>
-      <c r="C161">
-        <v>8473.32</v>
-      </c>
-      <c r="D161">
-        <v>333.95</v>
-      </c>
-      <c r="E161">
-        <v>4277.0200000000004</v>
-      </c>
-      <c r="F161">
-        <v>163.69</v>
-      </c>
-      <c r="G161">
-        <v>112.8156</v>
-      </c>
-      <c r="H161">
-        <v>164.23</v>
-      </c>
-      <c r="I161">
-        <v>91.813800000000001</v>
-      </c>
-      <c r="J161">
-        <v>93.827100000000002</v>
-      </c>
-      <c r="K161">
-        <v>127.4787</v>
-      </c>
-      <c r="L161">
-        <v>881.65</v>
-      </c>
-      <c r="M161">
-        <v>1146.56</v>
-      </c>
-      <c r="N161">
-        <v>283.81979999999999</v>
-      </c>
-      <c r="O161">
-        <v>281.73</v>
-      </c>
-      <c r="P161">
-        <v>358.45</v>
-      </c>
-      <c r="Q161">
-        <v>335.16</v>
-      </c>
-      <c r="R161">
-        <v>169.34</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A162" s="1">
-        <v>44778</v>
-      </c>
-      <c r="B162">
-        <v>8764.0820000000003</v>
-      </c>
-      <c r="C162">
-        <v>8407.4</v>
-      </c>
-      <c r="D162">
-        <v>333.24</v>
-      </c>
-      <c r="E162">
-        <v>4197.07</v>
-      </c>
-      <c r="F162">
-        <v>159.1</v>
-      </c>
-      <c r="G162">
-        <v>112.5962</v>
-      </c>
-      <c r="H162">
-        <v>164.17</v>
-      </c>
-      <c r="I162">
-        <v>91.774100000000004</v>
-      </c>
-      <c r="J162">
-        <v>93.788799999999995</v>
-      </c>
-      <c r="K162">
-        <v>127.4599</v>
-      </c>
-      <c r="L162">
-        <v>882.16</v>
-      </c>
-      <c r="M162">
-        <v>1144.69</v>
-      </c>
-      <c r="N162">
-        <v>283.7833</v>
-      </c>
-      <c r="O162">
-        <v>281.98</v>
-      </c>
-      <c r="P162">
-        <v>358.77</v>
-      </c>
-      <c r="Q162">
-        <v>335.51</v>
-      </c>
-      <c r="R162">
-        <v>169.48</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A163" s="1">
-        <v>44781</v>
-      </c>
-      <c r="B163">
-        <v>8753.393</v>
-      </c>
-      <c r="C163">
-        <v>8480.9599999999991</v>
-      </c>
-      <c r="D163">
-        <v>333.93</v>
-      </c>
-      <c r="E163">
-        <v>4238.93</v>
-      </c>
-      <c r="F163">
-        <v>162.30000000000001</v>
-      </c>
-      <c r="G163">
-        <v>112.59910000000001</v>
-      </c>
-      <c r="H163">
-        <v>164.19</v>
-      </c>
-      <c r="I163">
-        <v>91.7637</v>
-      </c>
-      <c r="J163">
-        <v>93.765199999999993</v>
-      </c>
-      <c r="K163">
-        <v>127.44280000000001</v>
-      </c>
-      <c r="L163">
-        <v>882.2</v>
-      </c>
-      <c r="M163">
-        <v>1143.3399999999999</v>
-      </c>
-      <c r="N163">
-        <v>283.74579999999997</v>
-      </c>
-      <c r="O163">
-        <v>282.18</v>
-      </c>
-      <c r="P163">
-        <v>359.11</v>
-      </c>
-      <c r="Q163">
-        <v>335.75</v>
-      </c>
-      <c r="R163">
-        <v>169.45</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A164" s="1">
-        <v>44782</v>
-      </c>
-      <c r="B164">
-        <v>8716.7510000000002</v>
-      </c>
-      <c r="C164">
-        <v>8386.49</v>
-      </c>
-      <c r="D164">
-        <v>332.31</v>
-      </c>
-      <c r="E164">
-        <v>4217.03</v>
-      </c>
-      <c r="F164">
-        <v>161.62</v>
-      </c>
-      <c r="G164">
-        <v>112.4363</v>
-      </c>
-      <c r="H164">
-        <v>164.2</v>
-      </c>
-      <c r="I164">
-        <v>91.772300000000001</v>
-      </c>
-      <c r="J164">
-        <v>93.783199999999994</v>
-      </c>
-      <c r="K164">
-        <v>127.4515</v>
-      </c>
-      <c r="L164">
-        <v>882.85</v>
-      </c>
-      <c r="M164">
-        <v>1144.8499999999999</v>
-      </c>
-      <c r="N164">
-        <v>283.67189999999999</v>
-      </c>
-      <c r="O164">
-        <v>282.29000000000002</v>
-      </c>
-      <c r="P164">
-        <v>359.06</v>
-      </c>
-      <c r="Q164">
-        <v>336</v>
-      </c>
-      <c r="R164">
-        <v>169.45</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A165" s="1">
-        <v>44783</v>
-      </c>
-      <c r="B165">
-        <v>8902.723</v>
-      </c>
-      <c r="C165">
-        <v>8463.18</v>
-      </c>
-      <c r="D165">
-        <v>338.6</v>
-      </c>
-      <c r="E165">
-        <v>4228.0600000000004</v>
-      </c>
-      <c r="F165">
-        <v>160</v>
-      </c>
-      <c r="G165">
-        <v>112.8806</v>
-      </c>
-      <c r="H165">
-        <v>164.25</v>
-      </c>
-      <c r="I165">
-        <v>91.653800000000004</v>
-      </c>
-      <c r="J165">
-        <v>93.670699999999997</v>
-      </c>
-      <c r="K165">
-        <v>127.38979999999999</v>
-      </c>
-      <c r="L165">
-        <v>879.76</v>
-      </c>
-      <c r="M165">
-        <v>1141.68</v>
-      </c>
-      <c r="N165">
-        <v>283.73329999999999</v>
-      </c>
-      <c r="O165">
-        <v>282.02</v>
-      </c>
-      <c r="P165">
-        <v>358.84</v>
-      </c>
-      <c r="Q165">
-        <v>335.55</v>
-      </c>
-      <c r="R165">
-        <v>169.36</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A166" s="1">
-        <v>44784</v>
-      </c>
-      <c r="B166">
-        <v>8898.8369999999995</v>
-      </c>
-      <c r="C166">
-        <v>8480.57</v>
-      </c>
-      <c r="D166">
-        <v>339.2</v>
-      </c>
-      <c r="E166">
-        <v>4182.1499999999996</v>
-      </c>
-      <c r="F166">
-        <v>155.05000000000001</v>
-      </c>
-      <c r="G166">
-        <v>113.005</v>
-      </c>
-      <c r="H166">
-        <v>164.25</v>
-      </c>
-      <c r="I166">
-        <v>91.656999999999996</v>
-      </c>
-      <c r="J166">
-        <v>93.661299999999997</v>
-      </c>
-      <c r="K166">
-        <v>127.3886</v>
-      </c>
-      <c r="L166">
-        <v>879.67</v>
-      </c>
-      <c r="M166">
-        <v>1143.45</v>
-      </c>
-      <c r="N166">
-        <v>284.00580000000002</v>
-      </c>
-      <c r="O166">
-        <v>281.82</v>
-      </c>
-      <c r="P166">
-        <v>358.55</v>
-      </c>
-      <c r="Q166">
-        <v>335.15</v>
-      </c>
-      <c r="R166">
-        <v>169.25</v>
-      </c>
-    </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A167" s="1">
-        <v>44785</v>
-      </c>
-      <c r="B167">
-        <v>9054.1380000000008</v>
-      </c>
-      <c r="C167">
-        <v>8526.42</v>
-      </c>
-      <c r="D167">
-        <v>342.89</v>
-      </c>
-      <c r="E167">
-        <v>4227.76</v>
-      </c>
-      <c r="F167">
-        <v>157.05000000000001</v>
-      </c>
-      <c r="G167">
-        <v>113.5121</v>
-      </c>
-      <c r="H167">
-        <v>164.38</v>
-      </c>
-      <c r="I167">
-        <v>91.620500000000007</v>
-      </c>
-      <c r="J167">
-        <v>93.633799999999994</v>
-      </c>
-      <c r="K167">
-        <v>127.36879999999999</v>
-      </c>
-      <c r="L167">
-        <v>877.68</v>
-      </c>
-      <c r="M167">
-        <v>1138.8599999999999</v>
-      </c>
-      <c r="N167">
-        <v>284.35640000000001</v>
-      </c>
-      <c r="O167">
-        <v>281.73</v>
-      </c>
-      <c r="P167">
-        <v>358.53</v>
-      </c>
-      <c r="Q167">
-        <v>335.23</v>
-      </c>
-      <c r="R167">
-        <v>169.25</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A168" s="1">
-        <v>44788</v>
-      </c>
-      <c r="B168">
-        <v>9090.3610000000008</v>
-      </c>
-      <c r="C168">
-        <v>8555.33</v>
-      </c>
-      <c r="D168">
-        <v>343.69</v>
-      </c>
-      <c r="E168">
-        <v>4237.04</v>
-      </c>
-      <c r="F168">
-        <v>156.78</v>
-      </c>
-      <c r="G168">
-        <v>113.54300000000001</v>
-      </c>
-      <c r="H168">
-        <v>164.28</v>
-      </c>
-      <c r="I168">
-        <v>91.620999999999995</v>
-      </c>
-      <c r="J168">
-        <v>93.638400000000004</v>
-      </c>
-      <c r="K168">
-        <v>127.3695</v>
-      </c>
-      <c r="L168">
-        <v>877.44</v>
-      </c>
-      <c r="M168">
-        <v>1138.67</v>
-      </c>
-      <c r="N168">
-        <v>283.9357</v>
-      </c>
-      <c r="O168">
-        <v>281.91000000000003</v>
-      </c>
-      <c r="P168">
-        <v>358.73</v>
-      </c>
-      <c r="Q168">
-        <v>335.44</v>
-      </c>
-      <c r="R168">
-        <v>169.24</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A169" s="1">
-        <v>44789</v>
-      </c>
-      <c r="B169">
-        <v>9107.8670000000002</v>
-      </c>
-      <c r="C169">
-        <v>8590.56</v>
-      </c>
-      <c r="D169">
-        <v>343.89</v>
-      </c>
-      <c r="E169">
-        <v>4237.16</v>
-      </c>
-      <c r="F169">
-        <v>157.85</v>
-      </c>
-      <c r="G169">
-        <v>113.5821</v>
-      </c>
-      <c r="H169">
-        <v>164.29</v>
-      </c>
-      <c r="I169">
-        <v>91.624799999999993</v>
-      </c>
-      <c r="J169">
-        <v>93.634299999999996</v>
-      </c>
-      <c r="K169">
-        <v>127.37260000000001</v>
-      </c>
-      <c r="L169">
-        <v>877.33</v>
-      </c>
-      <c r="M169">
-        <v>1137.5899999999999</v>
-      </c>
-      <c r="N169">
-        <v>283.93880000000001</v>
-      </c>
-      <c r="O169">
-        <v>282.08999999999997</v>
-      </c>
-      <c r="P169">
-        <v>358.89</v>
-      </c>
-      <c r="Q169">
-        <v>335.68</v>
-      </c>
-      <c r="R169">
-        <v>169.29</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A170" s="1">
-        <v>44790</v>
-      </c>
-      <c r="B170">
-        <v>9043.5889999999999</v>
-      </c>
-      <c r="C170">
-        <v>8479.58</v>
-      </c>
-      <c r="D170">
-        <v>341.66</v>
-      </c>
-      <c r="E170">
-        <v>4188.9799999999996</v>
-      </c>
-      <c r="F170">
-        <v>155.69</v>
-      </c>
-      <c r="G170">
-        <v>113.5885</v>
-      </c>
-      <c r="H170">
-        <v>164.08</v>
-      </c>
-      <c r="I170">
-        <v>91.628600000000006</v>
-      </c>
-      <c r="J170">
-        <v>93.632599999999996</v>
-      </c>
-      <c r="K170">
-        <v>127.377</v>
-      </c>
-      <c r="L170">
-        <v>878.03</v>
-      </c>
-      <c r="M170">
-        <v>1138.46</v>
-      </c>
-      <c r="N170">
-        <v>283.50299999999999</v>
-      </c>
-      <c r="O170">
-        <v>282.12</v>
-      </c>
-      <c r="P170">
-        <v>358.88</v>
-      </c>
-      <c r="Q170">
-        <v>335.82</v>
-      </c>
-      <c r="R170">
-        <v>169.37</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A171" s="1">
-        <v>44791</v>
-      </c>
-      <c r="B171">
-        <v>9065.49</v>
-      </c>
-      <c r="C171">
-        <v>8527.7000000000007</v>
-      </c>
-      <c r="D171">
-        <v>341.89</v>
-      </c>
-      <c r="E171">
-        <v>4195.88</v>
-      </c>
-      <c r="F171">
-        <v>155.88999999999999</v>
-      </c>
-      <c r="G171">
-        <v>113.4795</v>
-      </c>
-      <c r="H171">
-        <v>164.13</v>
-      </c>
-      <c r="I171">
-        <v>91.601500000000001</v>
-      </c>
-      <c r="J171">
-        <v>93.622600000000006</v>
-      </c>
-      <c r="K171">
-        <v>127.35680000000001</v>
-      </c>
-      <c r="L171">
-        <v>877.94</v>
-      </c>
-      <c r="M171">
-        <v>1138.22</v>
-      </c>
-      <c r="N171">
-        <v>283.584</v>
-      </c>
-      <c r="O171">
-        <v>282.27999999999997</v>
-      </c>
-      <c r="P171">
-        <v>359.17</v>
-      </c>
-      <c r="Q171">
-        <v>336.14</v>
-      </c>
-      <c r="R171">
-        <v>169.45</v>
-      </c>
-    </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A172" s="1">
-        <v>44792</v>
-      </c>
-      <c r="B172">
-        <v>8948.8179999999993</v>
-      </c>
-      <c r="C172">
-        <v>8421.4699999999993</v>
-      </c>
-      <c r="D172">
-        <v>337.42</v>
-      </c>
-      <c r="E172">
-        <v>4132.21</v>
-      </c>
-      <c r="F172">
-        <v>152.77000000000001</v>
-      </c>
-      <c r="G172">
-        <v>113.3695</v>
-      </c>
-      <c r="H172">
-        <v>164.09</v>
-      </c>
-      <c r="I172">
-        <v>91.6524</v>
-      </c>
-      <c r="J172">
-        <v>93.679500000000004</v>
-      </c>
-      <c r="K172">
-        <v>127.3942</v>
-      </c>
-      <c r="L172">
-        <v>879.18</v>
-      </c>
-      <c r="M172">
-        <v>1137.3699999999999</v>
-      </c>
-      <c r="N172">
-        <v>283.77629999999999</v>
-      </c>
-      <c r="O172">
-        <v>282.26</v>
-      </c>
-      <c r="P172">
-        <v>359.09</v>
-      </c>
-      <c r="Q172">
-        <v>335.99</v>
-      </c>
-      <c r="R172">
-        <v>169.49</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A173" s="1">
-        <v>44795</v>
-      </c>
-      <c r="B173">
-        <v>8758.2430000000004</v>
-      </c>
-      <c r="C173">
-        <v>8258.69</v>
-      </c>
-      <c r="D173">
-        <v>331.53</v>
-      </c>
-      <c r="E173">
-        <v>4100.78</v>
-      </c>
-      <c r="F173">
-        <v>152.16</v>
-      </c>
-      <c r="G173">
-        <v>112.8489</v>
-      </c>
-      <c r="H173">
-        <v>163.65</v>
-      </c>
-      <c r="I173">
-        <v>91.783199999999994</v>
-      </c>
-      <c r="J173">
-        <v>93.810299999999998</v>
-      </c>
-      <c r="K173">
-        <v>127.4551</v>
-      </c>
-      <c r="L173">
-        <v>881.66</v>
-      </c>
-      <c r="M173">
-        <v>1137.31</v>
-      </c>
-      <c r="N173">
-        <v>282.39870000000002</v>
-      </c>
-      <c r="O173">
-        <v>281.58</v>
-      </c>
-      <c r="P173">
-        <v>359.12</v>
-      </c>
-      <c r="Q173">
-        <v>335.71</v>
-      </c>
-      <c r="R173">
-        <v>169.18</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A174" s="1">
-        <v>44796</v>
-      </c>
-      <c r="B174">
-        <v>8738.7630000000008</v>
-      </c>
-      <c r="C174">
-        <v>8245.83</v>
-      </c>
-      <c r="D174">
-        <v>330.83</v>
-      </c>
-      <c r="E174">
-        <v>4090.63</v>
-      </c>
-      <c r="F174">
-        <v>151.13</v>
-      </c>
-      <c r="G174">
-        <v>112.38030000000001</v>
-      </c>
-      <c r="H174">
-        <v>163.33000000000001</v>
-      </c>
-      <c r="I174">
-        <v>91.73</v>
-      </c>
-      <c r="J174">
-        <v>93.707599999999999</v>
-      </c>
-      <c r="K174">
-        <v>127.4281</v>
-      </c>
-      <c r="L174">
-        <v>882.34</v>
-      </c>
-      <c r="M174">
-        <v>1136.7</v>
-      </c>
-      <c r="N174">
-        <v>282.93119999999999</v>
-      </c>
-      <c r="O174">
-        <v>281.99</v>
-      </c>
-      <c r="P174">
-        <v>359.29</v>
-      </c>
-      <c r="Q174">
-        <v>336.35</v>
-      </c>
-      <c r="R174">
-        <v>169.35</v>
-      </c>
-    </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A175" s="1">
-        <v>44797</v>
-      </c>
-      <c r="B175">
-        <v>8764.42</v>
-      </c>
-      <c r="C175">
-        <v>8279.5499999999993</v>
-      </c>
-      <c r="D175">
-        <v>331.29</v>
-      </c>
-      <c r="E175">
-        <v>4076.99</v>
-      </c>
-      <c r="F175">
-        <v>149.65</v>
-      </c>
-      <c r="G175">
-        <v>112.1097</v>
-      </c>
-      <c r="H175">
-        <v>163.25</v>
-      </c>
-      <c r="I175">
-        <v>91.584100000000007</v>
-      </c>
-      <c r="J175">
-        <v>93.628100000000003</v>
-      </c>
-      <c r="K175">
-        <v>127.3526</v>
-      </c>
-      <c r="L175">
-        <v>882.25</v>
-      </c>
-      <c r="M175">
-        <v>1136.58</v>
-      </c>
-      <c r="N175">
-        <v>283.32589999999999</v>
-      </c>
-      <c r="O175">
-        <v>282.39999999999998</v>
-      </c>
-      <c r="P175">
-        <v>359.77</v>
-      </c>
-      <c r="Q175">
-        <v>336.56</v>
-      </c>
-      <c r="R175">
-        <v>169.55</v>
-      </c>
-    </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A176" s="1">
-        <v>44798</v>
-      </c>
-      <c r="B176">
-        <v>8888.1280000000006</v>
-      </c>
-      <c r="C176">
-        <v>8295.5400000000009</v>
-      </c>
-      <c r="D176">
-        <v>335.48</v>
-      </c>
-      <c r="E176">
-        <v>4127.1400000000003</v>
-      </c>
-      <c r="F176">
-        <v>152.35</v>
-      </c>
-      <c r="G176">
-        <v>112.3784</v>
-      </c>
-      <c r="H176">
-        <v>163.52000000000001</v>
-      </c>
-      <c r="I176">
-        <v>91.489199999999997</v>
-      </c>
-      <c r="J176">
-        <v>93.480199999999996</v>
-      </c>
-      <c r="K176">
-        <v>127.29259999999999</v>
-      </c>
-      <c r="L176">
-        <v>879.89</v>
-      </c>
-      <c r="M176">
-        <v>1134.26</v>
-      </c>
-      <c r="N176">
-        <v>282.47680000000003</v>
-      </c>
-      <c r="O176">
-        <v>281.86</v>
-      </c>
-      <c r="P176">
-        <v>359.18</v>
-      </c>
-      <c r="Q176">
-        <v>335.96</v>
-      </c>
-      <c r="R176">
-        <v>169.53</v>
-      </c>
-    </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A177" s="1">
-        <v>44799</v>
-      </c>
-      <c r="B177">
-        <v>8588.9459999999999</v>
-      </c>
-      <c r="C177">
-        <v>8135.58</v>
-      </c>
-      <c r="D177">
-        <v>327.63</v>
-      </c>
-      <c r="E177">
-        <v>4131.16</v>
-      </c>
-      <c r="F177">
-        <v>154.22</v>
-      </c>
-      <c r="G177">
-        <v>112.1219</v>
-      </c>
-      <c r="H177">
-        <v>162.63</v>
-      </c>
-      <c r="I177">
-        <v>91.706000000000003</v>
-      </c>
-      <c r="J177">
-        <v>93.591999999999999</v>
-      </c>
-      <c r="K177">
-        <v>127.38809999999999</v>
-      </c>
-      <c r="L177">
-        <v>885.23</v>
-      </c>
-      <c r="M177">
-        <v>1135.52</v>
-      </c>
-      <c r="N177">
-        <v>284.0487</v>
-      </c>
-      <c r="O177">
-        <v>282.58</v>
-      </c>
-      <c r="P177">
-        <v>359.94</v>
-      </c>
-      <c r="Q177">
-        <v>336.02</v>
-      </c>
-      <c r="R177">
-        <v>169.43</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A178" s="1">
-        <v>44802</v>
-      </c>
-      <c r="B178">
-        <v>8532.1020000000008</v>
-      </c>
-      <c r="C178">
-        <v>8060.68</v>
-      </c>
-      <c r="D178">
-        <v>324.31</v>
-      </c>
-      <c r="E178">
-        <v>4088.08</v>
-      </c>
-      <c r="F178">
-        <v>152.58000000000001</v>
-      </c>
-      <c r="G178">
-        <v>111.52509999999999</v>
-      </c>
-      <c r="H178">
-        <v>162.13999999999999</v>
-      </c>
-      <c r="I178">
-        <v>91.723500000000001</v>
-      </c>
-      <c r="J178">
-        <v>93.755799999999994</v>
-      </c>
-      <c r="K178">
-        <v>127.4524</v>
-      </c>
-      <c r="L178">
-        <v>887.12</v>
-      </c>
-      <c r="M178">
-        <v>1133.95</v>
-      </c>
-      <c r="N178">
-        <v>284.16669999999999</v>
-      </c>
-      <c r="O178">
-        <v>283.06</v>
-      </c>
-      <c r="P178">
-        <v>360.56</v>
-      </c>
-      <c r="Q178">
-        <v>337.07</v>
-      </c>
-      <c r="R178">
-        <v>169.42</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A179" s="1">
-        <v>44803</v>
-      </c>
-      <c r="B179">
-        <v>8438.6869999999999</v>
-      </c>
-      <c r="C179">
-        <v>8041.3</v>
-      </c>
-      <c r="D179">
-        <v>321.83999999999997</v>
-      </c>
-      <c r="E179">
-        <v>4090.08</v>
-      </c>
-      <c r="F179">
-        <v>153.38999999999999</v>
-      </c>
-      <c r="G179">
-        <v>110.976</v>
-      </c>
-      <c r="H179">
-        <v>161.75</v>
-      </c>
-      <c r="I179">
-        <v>91.882199999999997</v>
-      </c>
-      <c r="J179">
-        <v>93.805899999999994</v>
-      </c>
-      <c r="K179">
-        <v>127.5065</v>
-      </c>
-      <c r="L179">
-        <v>889.74</v>
-      </c>
-      <c r="M179">
-        <v>1133.72</v>
-      </c>
-      <c r="N179">
-        <v>284.59399999999999</v>
-      </c>
-      <c r="O179">
-        <v>282.89999999999998</v>
-      </c>
-      <c r="P179">
-        <v>360.03</v>
-      </c>
-      <c r="Q179">
-        <v>336.89</v>
-      </c>
-      <c r="R179">
-        <v>169.49</v>
-      </c>
-    </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A180" s="1">
-        <v>44804</v>
-      </c>
-      <c r="B180">
-        <v>8374.4159999999993</v>
-      </c>
-      <c r="C180">
-        <v>7940.45</v>
-      </c>
-      <c r="D180">
-        <v>319.98</v>
-      </c>
-      <c r="E180">
-        <v>4046.99</v>
-      </c>
-      <c r="F180">
-        <v>151.47</v>
-      </c>
-      <c r="G180">
-        <v>110.51479999999999</v>
-      </c>
-      <c r="H180">
-        <v>161.09</v>
-      </c>
-      <c r="I180">
-        <v>91.6631</v>
-      </c>
-      <c r="J180">
-        <v>93.6631</v>
-      </c>
-      <c r="K180">
-        <v>127.4104</v>
-      </c>
-      <c r="L180">
-        <v>892.53</v>
-      </c>
-      <c r="M180">
-        <v>1134.3499999999999</v>
-      </c>
-      <c r="N180">
-        <v>285.5609</v>
-      </c>
-      <c r="O180">
-        <v>283.08999999999997</v>
-      </c>
-      <c r="P180">
-        <v>360.47</v>
-      </c>
-      <c r="Q180">
-        <v>337.21</v>
-      </c>
-      <c r="R180">
-        <v>169.7</v>
-      </c>
-    </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update ups data 10/31/22
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/ups_data.xlsx
+++ b/EquityHedging/data/update_strats/ups_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0245A813-3EED-4C29-9AEE-C965252CD140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C71BE9-6D50-453D-B1B1-63B1FBDB2913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7710" yWindow="850" windowWidth="10420" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7790" yWindow="80" windowWidth="10420" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="SpreadsheetBuilder_2" hidden="1">#REF!</definedName>
     <definedName name="SpreadsheetBuilder_3" localSheetId="3" hidden="1">data_original!$A$1:$Q$1</definedName>
     <definedName name="SpreadsheetBuilder_3" hidden="1">data!$A$1:$Q$1</definedName>
-    <definedName name="SpreadsheetBuilder_7" hidden="1">bbg!$A$1:$R$7</definedName>
+    <definedName name="SpreadsheetBuilder_8" hidden="1">bbg!$A$1:$R$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,100 +180,108 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16727583087644445504</stp>
-        <tr r="M7" s="4"/>
+        <stp>BDH|13293675286086157145</stp>
+        <tr r="L7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14234006623429924125</stp>
-        <tr r="F7" s="4"/>
+        <stp>BDH|15788701446229380587</stp>
+        <tr r="C7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|11664350796143255550</stp>
-        <tr r="E7" s="4"/>
+        <stp>BDH|14280945124953536224</stp>
+        <tr r="K7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12131352925380315342</stp>
-        <tr r="P7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12059809901744298878</stp>
-        <tr r="Q7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17414422510344432232</stp>
+        <stp>BDH|13347777784543565070</stp>
         <tr r="I7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12559626127843371028</stp>
-        <tr r="C7" s="4"/>
+        <stp>BDH|16394412001637310856</stp>
+        <tr r="N7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13464868775189878053</stp>
-        <tr r="H7" s="4"/>
+        <stp>BDH|15504497475315608268</stp>
+        <tr r="O7" s="4"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4101088581556967483</stp>
+        <stp>BDH|1917867544945112410</stp>
+        <tr r="G7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8563230619231295451</stp>
+        <tr r="M7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9581376854922930221</stp>
+        <tr r="Q7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8482114415071448600</stp>
+        <tr r="J7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4571599057655611840</stp>
+        <tr r="D7" s="4"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5607615982440028195</stp>
+        <tr r="F7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9292105084307128386</stp>
+        <tr r="P7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5756576771104393674</stp>
         <tr r="R7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2635583659919476254</stp>
-        <tr r="L7" s="4"/>
+        <stp>BDH|4748537713371872184</stp>
+        <tr r="H7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|6875801268774536502</stp>
-        <tr r="G7" s="4"/>
+        <stp>BDH|1798201725663483214</stp>
+        <tr r="E7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8640915654669239780</stp>
-        <tr r="N7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6570479873420035104</stp>
+        <stp>BDH|4121516891908523273</stp>
         <tr r="A7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3029848534948596642</stp>
-        <tr r="K7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6553308138291344783</stp>
-        <tr r="O7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6835677029197799680</stp>
-        <tr r="D7" s="4"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -412,14 +420,6 @@
         <stp>[ups_data.xlsx]bbg!R5C4</stp>
         <stp>PX_LAST</stp>
         <tr r="D5" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|932440353916099480</stp>
-        <tr r="J7" s="4"/>
       </tp>
     </main>
   </volType>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R197"/>
+  <dimension ref="A1:R218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="I171" sqref="I171"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:R218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11223,6 +11223,1182 @@
         <v>167.83</v>
       </c>
     </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A198" s="1">
+        <v>44837</v>
+      </c>
+      <c r="B198">
+        <v>7799.9989999999998</v>
+      </c>
+      <c r="C198">
+        <v>7552.7</v>
+      </c>
+      <c r="D198">
+        <v>294.91000000000003</v>
+      </c>
+      <c r="E198">
+        <v>3768.34</v>
+      </c>
+      <c r="F198">
+        <v>138.41999999999999</v>
+      </c>
+      <c r="G198">
+        <v>107.4717</v>
+      </c>
+      <c r="H198">
+        <v>155.1</v>
+      </c>
+      <c r="I198">
+        <v>91.95</v>
+      </c>
+      <c r="J198">
+        <v>93.663799999999995</v>
+      </c>
+      <c r="K198">
+        <v>127.3352</v>
+      </c>
+      <c r="L198">
+        <v>912.89</v>
+      </c>
+      <c r="M198">
+        <v>1129.33</v>
+      </c>
+      <c r="N198">
+        <v>285.77569999999997</v>
+      </c>
+      <c r="O198">
+        <v>283.67</v>
+      </c>
+      <c r="P198">
+        <v>360.89</v>
+      </c>
+      <c r="Q198">
+        <v>337.97</v>
+      </c>
+      <c r="R198">
+        <v>168.15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A199" s="1">
+        <v>44838</v>
+      </c>
+      <c r="B199">
+        <v>8039.2479999999996</v>
+      </c>
+      <c r="C199">
+        <v>7874.3</v>
+      </c>
+      <c r="D199">
+        <v>304.41000000000003</v>
+      </c>
+      <c r="E199">
+        <v>3787.21</v>
+      </c>
+      <c r="F199">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="G199">
+        <v>108.80970000000001</v>
+      </c>
+      <c r="H199">
+        <v>158.22</v>
+      </c>
+      <c r="I199">
+        <v>91.649699999999996</v>
+      </c>
+      <c r="J199">
+        <v>93.378299999999996</v>
+      </c>
+      <c r="K199">
+        <v>127.1418</v>
+      </c>
+      <c r="L199">
+        <v>901.17</v>
+      </c>
+      <c r="M199">
+        <v>1124.07</v>
+      </c>
+      <c r="N199">
+        <v>285.27210000000002</v>
+      </c>
+      <c r="O199">
+        <v>282.93</v>
+      </c>
+      <c r="P199">
+        <v>359.86</v>
+      </c>
+      <c r="Q199">
+        <v>337.21</v>
+      </c>
+      <c r="R199">
+        <v>167.52</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A200" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B200">
+        <v>8023.8059999999996</v>
+      </c>
+      <c r="C200">
+        <v>7791.22</v>
+      </c>
+      <c r="D200">
+        <v>303.75</v>
+      </c>
+      <c r="E200">
+        <v>3749.77</v>
+      </c>
+      <c r="F200">
+        <v>136.03</v>
+      </c>
+      <c r="G200">
+        <v>108.8232</v>
+      </c>
+      <c r="H200">
+        <v>157.88</v>
+      </c>
+      <c r="I200">
+        <v>91.686599999999999</v>
+      </c>
+      <c r="J200">
+        <v>93.567899999999995</v>
+      </c>
+      <c r="K200">
+        <v>127.23180000000001</v>
+      </c>
+      <c r="L200">
+        <v>901.78</v>
+      </c>
+      <c r="M200">
+        <v>1127.03</v>
+      </c>
+      <c r="N200">
+        <v>285.2944</v>
+      </c>
+      <c r="O200">
+        <v>282.56</v>
+      </c>
+      <c r="P200">
+        <v>359.35</v>
+      </c>
+      <c r="Q200">
+        <v>336.62</v>
+      </c>
+      <c r="R200">
+        <v>167.56</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A201" s="1">
+        <v>44840</v>
+      </c>
+      <c r="B201">
+        <v>7943.6319999999996</v>
+      </c>
+      <c r="C201">
+        <v>7758.96</v>
+      </c>
+      <c r="D201">
+        <v>301.49</v>
+      </c>
+      <c r="E201">
+        <v>3748.44</v>
+      </c>
+      <c r="F201">
+        <v>135.25</v>
+      </c>
+      <c r="G201">
+        <v>108.6734</v>
+      </c>
+      <c r="H201">
+        <v>157.12</v>
+      </c>
+      <c r="I201">
+        <v>91.7727</v>
+      </c>
+      <c r="J201">
+        <v>93.487499999999997</v>
+      </c>
+      <c r="K201">
+        <v>127.2026</v>
+      </c>
+      <c r="L201">
+        <v>905.09</v>
+      </c>
+      <c r="M201">
+        <v>1127.3399999999999</v>
+      </c>
+      <c r="N201">
+        <v>285.14319999999998</v>
+      </c>
+      <c r="O201">
+        <v>282.74</v>
+      </c>
+      <c r="P201">
+        <v>359.45</v>
+      </c>
+      <c r="Q201">
+        <v>336.46</v>
+      </c>
+      <c r="R201">
+        <v>167.64</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A202" s="1">
+        <v>44841</v>
+      </c>
+      <c r="B202">
+        <v>7721.44</v>
+      </c>
+      <c r="C202">
+        <v>7629.67</v>
+      </c>
+      <c r="D202">
+        <v>294.45999999999998</v>
+      </c>
+      <c r="E202">
+        <v>3707.28</v>
+      </c>
+      <c r="F202">
+        <v>133.49</v>
+      </c>
+      <c r="G202">
+        <v>107.8449</v>
+      </c>
+      <c r="H202">
+        <v>154.28</v>
+      </c>
+      <c r="I202">
+        <v>92.298199999999994</v>
+      </c>
+      <c r="J202">
+        <v>93.977900000000005</v>
+      </c>
+      <c r="K202">
+        <v>127.58329999999999</v>
+      </c>
+      <c r="L202">
+        <v>915.5</v>
+      </c>
+      <c r="M202">
+        <v>1130.76</v>
+      </c>
+      <c r="N202">
+        <v>284.07690000000002</v>
+      </c>
+      <c r="O202">
+        <v>282.94</v>
+      </c>
+      <c r="P202">
+        <v>359.78</v>
+      </c>
+      <c r="Q202">
+        <v>336.72</v>
+      </c>
+      <c r="R202">
+        <v>167.57</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A203" s="1">
+        <v>44844</v>
+      </c>
+      <c r="B203">
+        <v>7663.5820000000003</v>
+      </c>
+      <c r="C203">
+        <v>7587.66</v>
+      </c>
+      <c r="D203">
+        <v>291.60000000000002</v>
+      </c>
+      <c r="E203">
+        <v>3707.28</v>
+      </c>
+      <c r="F203">
+        <v>133.49</v>
+      </c>
+      <c r="G203">
+        <v>107.6786</v>
+      </c>
+      <c r="H203">
+        <v>153.43</v>
+      </c>
+      <c r="I203">
+        <v>92.628900000000002</v>
+      </c>
+      <c r="J203">
+        <v>94.2744</v>
+      </c>
+      <c r="K203">
+        <v>127.9342</v>
+      </c>
+      <c r="L203">
+        <v>917.96</v>
+      </c>
+      <c r="M203">
+        <v>1129.47</v>
+      </c>
+      <c r="N203">
+        <v>283.1961</v>
+      </c>
+      <c r="O203">
+        <v>282.94</v>
+      </c>
+      <c r="P203">
+        <v>359.96</v>
+      </c>
+      <c r="Q203">
+        <v>337.03</v>
+      </c>
+      <c r="R203">
+        <v>167.35</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A204" s="1">
+        <v>44845</v>
+      </c>
+      <c r="B204">
+        <v>7613.7529999999997</v>
+      </c>
+      <c r="C204">
+        <v>7550.3</v>
+      </c>
+      <c r="D204">
+        <v>288.77</v>
+      </c>
+      <c r="E204">
+        <v>3651.3</v>
+      </c>
+      <c r="F204">
+        <v>131.44999999999999</v>
+      </c>
+      <c r="G204">
+        <v>107.4308</v>
+      </c>
+      <c r="H204">
+        <v>152.30000000000001</v>
+      </c>
+      <c r="I204">
+        <v>92.529499999999999</v>
+      </c>
+      <c r="J204">
+        <v>94.415599999999998</v>
+      </c>
+      <c r="K204">
+        <v>127.8561</v>
+      </c>
+      <c r="L204">
+        <v>919.72</v>
+      </c>
+      <c r="M204">
+        <v>1129.6400000000001</v>
+      </c>
+      <c r="N204">
+        <v>283.03289999999998</v>
+      </c>
+      <c r="O204">
+        <v>282.97000000000003</v>
+      </c>
+      <c r="P204">
+        <v>359.52</v>
+      </c>
+      <c r="Q204">
+        <v>337.51</v>
+      </c>
+      <c r="R204">
+        <v>167.32</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A205" s="1">
+        <v>44846</v>
+      </c>
+      <c r="B205">
+        <v>7588.9009999999998</v>
+      </c>
+      <c r="C205">
+        <v>7530.36</v>
+      </c>
+      <c r="D205">
+        <v>287.87</v>
+      </c>
+      <c r="E205">
+        <v>3645.6</v>
+      </c>
+      <c r="F205">
+        <v>132.33000000000001</v>
+      </c>
+      <c r="G205">
+        <v>107.0826</v>
+      </c>
+      <c r="H205">
+        <v>151.38999999999999</v>
+      </c>
+      <c r="I205">
+        <v>92.517899999999997</v>
+      </c>
+      <c r="J205">
+        <v>94.445899999999995</v>
+      </c>
+      <c r="K205">
+        <v>127.8738</v>
+      </c>
+      <c r="L205">
+        <v>921.38</v>
+      </c>
+      <c r="M205">
+        <v>1130.51</v>
+      </c>
+      <c r="N205">
+        <v>283.2722</v>
+      </c>
+      <c r="O205">
+        <v>283.23</v>
+      </c>
+      <c r="P205">
+        <v>359.81</v>
+      </c>
+      <c r="Q205">
+        <v>338.05</v>
+      </c>
+      <c r="R205">
+        <v>167.47</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A206" s="1">
+        <v>44847</v>
+      </c>
+      <c r="B206">
+        <v>7786.9560000000001</v>
+      </c>
+      <c r="C206">
+        <v>7600.13</v>
+      </c>
+      <c r="D206">
+        <v>292.25</v>
+      </c>
+      <c r="E206">
+        <v>3626.85</v>
+      </c>
+      <c r="F206">
+        <v>130.62</v>
+      </c>
+      <c r="G206">
+        <v>107.8008</v>
+      </c>
+      <c r="H206">
+        <v>154.27000000000001</v>
+      </c>
+      <c r="I206">
+        <v>92.213899999999995</v>
+      </c>
+      <c r="J206">
+        <v>94.251300000000001</v>
+      </c>
+      <c r="K206">
+        <v>127.62309999999999</v>
+      </c>
+      <c r="L206">
+        <v>913.3</v>
+      </c>
+      <c r="M206">
+        <v>1128.18</v>
+      </c>
+      <c r="N206">
+        <v>282.20999999999998</v>
+      </c>
+      <c r="O206">
+        <v>282.43</v>
+      </c>
+      <c r="P206">
+        <v>358.52</v>
+      </c>
+      <c r="Q206">
+        <v>335.61</v>
+      </c>
+      <c r="R206">
+        <v>167.18</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A207" s="1">
+        <v>44848</v>
+      </c>
+      <c r="B207">
+        <v>7602.9880000000003</v>
+      </c>
+      <c r="C207">
+        <v>7643.82</v>
+      </c>
+      <c r="D207">
+        <v>288.79000000000002</v>
+      </c>
+      <c r="E207">
+        <v>3601.78</v>
+      </c>
+      <c r="F207">
+        <v>129.24</v>
+      </c>
+      <c r="G207">
+        <v>106.96559999999999</v>
+      </c>
+      <c r="H207">
+        <v>151.13999999999999</v>
+      </c>
+      <c r="I207">
+        <v>92.507999999999996</v>
+      </c>
+      <c r="J207">
+        <v>94.310100000000006</v>
+      </c>
+      <c r="K207">
+        <v>127.8613</v>
+      </c>
+      <c r="L207">
+        <v>920.98</v>
+      </c>
+      <c r="M207">
+        <v>1126.3</v>
+      </c>
+      <c r="N207">
+        <v>280.7312</v>
+      </c>
+      <c r="O207">
+        <v>282.77</v>
+      </c>
+      <c r="P207">
+        <v>359.24</v>
+      </c>
+      <c r="Q207">
+        <v>336.79</v>
+      </c>
+      <c r="R207">
+        <v>167.06</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A208" s="1">
+        <v>44851</v>
+      </c>
+      <c r="B208">
+        <v>7804.326</v>
+      </c>
+      <c r="C208">
+        <v>7779.25</v>
+      </c>
+      <c r="D208">
+        <v>294.85000000000002</v>
+      </c>
+      <c r="E208">
+        <v>3603.71</v>
+      </c>
+      <c r="F208">
+        <v>128.24</v>
+      </c>
+      <c r="G208">
+        <v>107.6793</v>
+      </c>
+      <c r="H208">
+        <v>154.51</v>
+      </c>
+      <c r="I208">
+        <v>92.000799999999998</v>
+      </c>
+      <c r="J208">
+        <v>93.8352</v>
+      </c>
+      <c r="K208">
+        <v>127.3467</v>
+      </c>
+      <c r="L208">
+        <v>913.51</v>
+      </c>
+      <c r="M208">
+        <v>1127.1099999999999</v>
+      </c>
+      <c r="N208">
+        <v>279.83269999999999</v>
+      </c>
+      <c r="O208">
+        <v>282.45999999999998</v>
+      </c>
+      <c r="P208">
+        <v>358.5</v>
+      </c>
+      <c r="Q208">
+        <v>336.22</v>
+      </c>
+      <c r="R208">
+        <v>167.46</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A209" s="1">
+        <v>44852</v>
+      </c>
+      <c r="B209">
+        <v>7893.6769999999997</v>
+      </c>
+      <c r="C209">
+        <v>7829.4</v>
+      </c>
+      <c r="D209">
+        <v>298.16000000000003</v>
+      </c>
+      <c r="E209">
+        <v>3624.94</v>
+      </c>
+      <c r="F209">
+        <v>128.65</v>
+      </c>
+      <c r="G209">
+        <v>107.91079999999999</v>
+      </c>
+      <c r="H209">
+        <v>155.69</v>
+      </c>
+      <c r="I209">
+        <v>91.972399999999993</v>
+      </c>
+      <c r="J209">
+        <v>93.803299999999993</v>
+      </c>
+      <c r="K209">
+        <v>127.3798</v>
+      </c>
+      <c r="L209">
+        <v>909.8</v>
+      </c>
+      <c r="M209">
+        <v>1125.47</v>
+      </c>
+      <c r="N209">
+        <v>279.613</v>
+      </c>
+      <c r="O209">
+        <v>281.89999999999998</v>
+      </c>
+      <c r="P209">
+        <v>357.71</v>
+      </c>
+      <c r="Q209">
+        <v>335.1</v>
+      </c>
+      <c r="R209">
+        <v>167.24</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A210" s="1">
+        <v>44853</v>
+      </c>
+      <c r="B210">
+        <v>7840.9939999999997</v>
+      </c>
+      <c r="C210">
+        <v>7846.16</v>
+      </c>
+      <c r="D210">
+        <v>295.67</v>
+      </c>
+      <c r="E210">
+        <v>3569.45</v>
+      </c>
+      <c r="F210">
+        <v>125.47</v>
+      </c>
+      <c r="G210">
+        <v>107.7871</v>
+      </c>
+      <c r="H210">
+        <v>154.51</v>
+      </c>
+      <c r="I210">
+        <v>91.997100000000003</v>
+      </c>
+      <c r="J210">
+        <v>93.832899999999995</v>
+      </c>
+      <c r="K210">
+        <v>127.3573</v>
+      </c>
+      <c r="L210">
+        <v>912.84</v>
+      </c>
+      <c r="M210">
+        <v>1127.3</v>
+      </c>
+      <c r="N210">
+        <v>279.58870000000002</v>
+      </c>
+      <c r="O210">
+        <v>282.04000000000002</v>
+      </c>
+      <c r="P210">
+        <v>357.83</v>
+      </c>
+      <c r="Q210">
+        <v>335.49</v>
+      </c>
+      <c r="R210">
+        <v>167.45</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A211" s="1">
+        <v>44854</v>
+      </c>
+      <c r="B211">
+        <v>7779.5249999999996</v>
+      </c>
+      <c r="C211">
+        <v>7894.99</v>
+      </c>
+      <c r="D211">
+        <v>294.56</v>
+      </c>
+      <c r="E211">
+        <v>3530.66</v>
+      </c>
+      <c r="F211">
+        <v>122.79</v>
+      </c>
+      <c r="G211">
+        <v>107.1893</v>
+      </c>
+      <c r="H211">
+        <v>152.91999999999999</v>
+      </c>
+      <c r="I211">
+        <v>91.853200000000001</v>
+      </c>
+      <c r="J211">
+        <v>93.733999999999995</v>
+      </c>
+      <c r="K211">
+        <v>127.2277</v>
+      </c>
+      <c r="L211">
+        <v>916.29</v>
+      </c>
+      <c r="M211">
+        <v>1126.33</v>
+      </c>
+      <c r="N211">
+        <v>279.94369999999998</v>
+      </c>
+      <c r="O211">
+        <v>282.23</v>
+      </c>
+      <c r="P211">
+        <v>358.14</v>
+      </c>
+      <c r="Q211">
+        <v>335.54</v>
+      </c>
+      <c r="R211">
+        <v>167.43</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A212" s="1">
+        <v>44855</v>
+      </c>
+      <c r="B212">
+        <v>7964.2479999999996</v>
+      </c>
+      <c r="C212">
+        <v>7858.34</v>
+      </c>
+      <c r="D212">
+        <v>298.16000000000003</v>
+      </c>
+      <c r="E212">
+        <v>3496.25</v>
+      </c>
+      <c r="F212">
+        <v>119.14</v>
+      </c>
+      <c r="G212">
+        <v>108.43380000000001</v>
+      </c>
+      <c r="H212">
+        <v>156.51</v>
+      </c>
+      <c r="I212">
+        <v>91.776399999999995</v>
+      </c>
+      <c r="J212">
+        <v>93.625900000000001</v>
+      </c>
+      <c r="K212">
+        <v>127.1782</v>
+      </c>
+      <c r="L212">
+        <v>908.08</v>
+      </c>
+      <c r="M212">
+        <v>1122.72</v>
+      </c>
+      <c r="N212">
+        <v>277.82429999999999</v>
+      </c>
+      <c r="O212">
+        <v>282.33</v>
+      </c>
+      <c r="P212">
+        <v>358.21</v>
+      </c>
+      <c r="Q212">
+        <v>335.55</v>
+      </c>
+      <c r="R212">
+        <v>167.08</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A213" s="1">
+        <v>44858</v>
+      </c>
+      <c r="B213">
+        <v>8058.8789999999999</v>
+      </c>
+      <c r="C213">
+        <v>7974.19</v>
+      </c>
+      <c r="D213">
+        <v>300.64999999999998</v>
+      </c>
+      <c r="E213">
+        <v>3496.08</v>
+      </c>
+      <c r="F213">
+        <v>117.85</v>
+      </c>
+      <c r="G213">
+        <v>108.6968</v>
+      </c>
+      <c r="H213">
+        <v>157.82</v>
+      </c>
+      <c r="I213">
+        <v>91.783000000000001</v>
+      </c>
+      <c r="J213">
+        <v>93.701599999999999</v>
+      </c>
+      <c r="K213">
+        <v>127.2093</v>
+      </c>
+      <c r="L213">
+        <v>904.57</v>
+      </c>
+      <c r="M213">
+        <v>1123.1199999999999</v>
+      </c>
+      <c r="N213">
+        <v>278.11470000000003</v>
+      </c>
+      <c r="O213">
+        <v>282.42</v>
+      </c>
+      <c r="P213">
+        <v>358.28</v>
+      </c>
+      <c r="Q213">
+        <v>335.66</v>
+      </c>
+      <c r="R213">
+        <v>166.92</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
+        <v>44859</v>
+      </c>
+      <c r="B214">
+        <v>8190.018</v>
+      </c>
+      <c r="C214">
+        <v>8104.81</v>
+      </c>
+      <c r="D214">
+        <v>305.52999999999997</v>
+      </c>
+      <c r="E214">
+        <v>3571.48</v>
+      </c>
+      <c r="F214">
+        <v>122.56</v>
+      </c>
+      <c r="G214">
+        <v>108.93219999999999</v>
+      </c>
+      <c r="H214">
+        <v>159.36000000000001</v>
+      </c>
+      <c r="I214">
+        <v>91.517799999999994</v>
+      </c>
+      <c r="J214">
+        <v>93.432900000000004</v>
+      </c>
+      <c r="K214">
+        <v>126.99250000000001</v>
+      </c>
+      <c r="L214">
+        <v>899.98</v>
+      </c>
+      <c r="M214">
+        <v>1121.57</v>
+      </c>
+      <c r="N214">
+        <v>277.6687</v>
+      </c>
+      <c r="O214">
+        <v>282.5</v>
+      </c>
+      <c r="P214">
+        <v>358.21</v>
+      </c>
+      <c r="Q214">
+        <v>335.6</v>
+      </c>
+      <c r="R214">
+        <v>166.88</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A215" s="1">
+        <v>44860</v>
+      </c>
+      <c r="B215">
+        <v>8129.6229999999996</v>
+      </c>
+      <c r="C215">
+        <v>8149.42</v>
+      </c>
+      <c r="D215">
+        <v>305.60000000000002</v>
+      </c>
+      <c r="E215">
+        <v>3607.71</v>
+      </c>
+      <c r="F215">
+        <v>125.04</v>
+      </c>
+      <c r="G215">
+        <v>108.39</v>
+      </c>
+      <c r="H215">
+        <v>158.46</v>
+      </c>
+      <c r="I215">
+        <v>91.381600000000006</v>
+      </c>
+      <c r="J215">
+        <v>93.253</v>
+      </c>
+      <c r="K215">
+        <v>126.8927</v>
+      </c>
+      <c r="L215">
+        <v>903.32</v>
+      </c>
+      <c r="M215">
+        <v>1125.82</v>
+      </c>
+      <c r="N215">
+        <v>277.39920000000001</v>
+      </c>
+      <c r="O215">
+        <v>282.8</v>
+      </c>
+      <c r="P215">
+        <v>358.71</v>
+      </c>
+      <c r="Q215">
+        <v>335.66</v>
+      </c>
+      <c r="R215">
+        <v>166.87</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A216" s="1">
+        <v>44861</v>
+      </c>
+      <c r="B216">
+        <v>8080.32</v>
+      </c>
+      <c r="C216">
+        <v>8147.6</v>
+      </c>
+      <c r="D216">
+        <v>304.58999999999997</v>
+      </c>
+      <c r="E216">
+        <v>3636.54</v>
+      </c>
+      <c r="F216">
+        <v>126.73</v>
+      </c>
+      <c r="G216">
+        <v>107.7576</v>
+      </c>
+      <c r="H216">
+        <v>157.78</v>
+      </c>
+      <c r="I216">
+        <v>91.307299999999998</v>
+      </c>
+      <c r="J216">
+        <v>93.159300000000002</v>
+      </c>
+      <c r="K216">
+        <v>126.8373</v>
+      </c>
+      <c r="L216">
+        <v>906</v>
+      </c>
+      <c r="M216">
+        <v>1132.9000000000001</v>
+      </c>
+      <c r="N216">
+        <v>278.57459999999998</v>
+      </c>
+      <c r="O216">
+        <v>282.94</v>
+      </c>
+      <c r="P216">
+        <v>358.95</v>
+      </c>
+      <c r="Q216">
+        <v>335.91</v>
+      </c>
+      <c r="R216">
+        <v>167.2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A217" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B217">
+        <v>8280.1059999999998</v>
+      </c>
+      <c r="C217">
+        <v>8166.85</v>
+      </c>
+      <c r="D217">
+        <v>308.14</v>
+      </c>
+      <c r="E217">
+        <v>3625.9</v>
+      </c>
+      <c r="F217">
+        <v>125.73</v>
+      </c>
+      <c r="G217">
+        <v>108.592</v>
+      </c>
+      <c r="H217">
+        <v>160.18</v>
+      </c>
+      <c r="I217">
+        <v>91.210499999999996</v>
+      </c>
+      <c r="J217">
+        <v>93.089299999999994</v>
+      </c>
+      <c r="K217">
+        <v>126.7839</v>
+      </c>
+      <c r="L217">
+        <v>897.8</v>
+      </c>
+      <c r="M217">
+        <v>1127.23</v>
+      </c>
+      <c r="N217">
+        <v>277.21319999999997</v>
+      </c>
+      <c r="O217">
+        <v>282.98</v>
+      </c>
+      <c r="P217">
+        <v>359.13</v>
+      </c>
+      <c r="Q217">
+        <v>336.09</v>
+      </c>
+      <c r="R217">
+        <v>167.25</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A218" s="1">
+        <v>44865</v>
+      </c>
+      <c r="B218">
+        <v>8218.7049999999999</v>
+      </c>
+      <c r="C218">
+        <v>8179.88</v>
+      </c>
+      <c r="D218">
+        <v>306.81</v>
+      </c>
+      <c r="E218">
+        <v>3610.31</v>
+      </c>
+      <c r="F218">
+        <v>124.25</v>
+      </c>
+      <c r="G218">
+        <v>108.08839999999999</v>
+      </c>
+      <c r="H218">
+        <v>159.6</v>
+      </c>
+      <c r="I218">
+        <v>91.190600000000003</v>
+      </c>
+      <c r="J218">
+        <v>93.060400000000001</v>
+      </c>
+      <c r="K218">
+        <v>126.7722</v>
+      </c>
+      <c r="L218">
+        <v>901.15</v>
+      </c>
+      <c r="M218">
+        <v>1128.26</v>
+      </c>
+      <c r="N218">
+        <v>275.762</v>
+      </c>
+      <c r="O218">
+        <v>283.58</v>
+      </c>
+      <c r="P218">
+        <v>359.44</v>
+      </c>
+      <c r="Q218">
+        <v>336.89</v>
+      </c>
+      <c r="R218">
+        <v>167.37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -61804,8 +62980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R283"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="R202" sqref="A180:R202"/>
+    <sheetView topLeftCell="K201" workbookViewId="0">
+      <selection activeCell="A223" sqref="A202:R223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -61841,7 +63017,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>44834</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -62025,74 +63201,74 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=196")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=217")</f>
         <v>44561</v>
       </c>
       <c r="B7">
         <v>9986.6980000000003</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>9491.1</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>389.04</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>5233.6899999999996</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>214.08</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>122.8967</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>175.14</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>98.672499999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>101.2684</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>135.21369999999999</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>835.24</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>1088</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>297.6395</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>287.23</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>368.34</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>345.76</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=196")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=217")</f>
         <v>169.35</v>
       </c>
     </row>
@@ -73017,69 +74193,1182 @@
       </c>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A203" s="1"/>
+      <c r="A203" s="1">
+        <v>44837</v>
+      </c>
+      <c r="B203">
+        <v>7799.9989999999998</v>
+      </c>
+      <c r="C203">
+        <v>7552.7</v>
+      </c>
+      <c r="D203">
+        <v>294.91000000000003</v>
+      </c>
+      <c r="E203">
+        <v>3768.34</v>
+      </c>
+      <c r="F203">
+        <v>138.41999999999999</v>
+      </c>
+      <c r="G203">
+        <v>107.4717</v>
+      </c>
+      <c r="H203">
+        <v>155.1</v>
+      </c>
+      <c r="I203">
+        <v>91.95</v>
+      </c>
+      <c r="J203">
+        <v>93.663799999999995</v>
+      </c>
+      <c r="K203">
+        <v>127.3352</v>
+      </c>
+      <c r="L203">
+        <v>912.89</v>
+      </c>
+      <c r="M203">
+        <v>1129.33</v>
+      </c>
+      <c r="N203">
+        <v>285.77569999999997</v>
+      </c>
+      <c r="O203">
+        <v>283.67</v>
+      </c>
+      <c r="P203">
+        <v>360.89</v>
+      </c>
+      <c r="Q203">
+        <v>337.97</v>
+      </c>
+      <c r="R203">
+        <v>168.15</v>
+      </c>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1">
+        <v>44838</v>
+      </c>
+      <c r="B204">
+        <v>8039.2479999999996</v>
+      </c>
+      <c r="C204">
+        <v>7874.3</v>
+      </c>
+      <c r="D204">
+        <v>304.41000000000003</v>
+      </c>
+      <c r="E204">
+        <v>3787.21</v>
+      </c>
+      <c r="F204">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="G204">
+        <v>108.80970000000001</v>
+      </c>
+      <c r="H204">
+        <v>158.22</v>
+      </c>
+      <c r="I204">
+        <v>91.649699999999996</v>
+      </c>
+      <c r="J204">
+        <v>93.378299999999996</v>
+      </c>
+      <c r="K204">
+        <v>127.1418</v>
+      </c>
+      <c r="L204">
+        <v>901.17</v>
+      </c>
+      <c r="M204">
+        <v>1124.07</v>
+      </c>
+      <c r="N204">
+        <v>285.27210000000002</v>
+      </c>
+      <c r="O204">
+        <v>282.93</v>
+      </c>
+      <c r="P204">
+        <v>359.86</v>
+      </c>
+      <c r="Q204">
+        <v>337.21</v>
+      </c>
+      <c r="R204">
+        <v>167.52</v>
+      </c>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A205" s="1"/>
+      <c r="A205" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B205">
+        <v>8023.8059999999996</v>
+      </c>
+      <c r="C205">
+        <v>7791.22</v>
+      </c>
+      <c r="D205">
+        <v>303.75</v>
+      </c>
+      <c r="E205">
+        <v>3749.77</v>
+      </c>
+      <c r="F205">
+        <v>136.03</v>
+      </c>
+      <c r="G205">
+        <v>108.8232</v>
+      </c>
+      <c r="H205">
+        <v>157.88</v>
+      </c>
+      <c r="I205">
+        <v>91.686599999999999</v>
+      </c>
+      <c r="J205">
+        <v>93.567899999999995</v>
+      </c>
+      <c r="K205">
+        <v>127.23180000000001</v>
+      </c>
+      <c r="L205">
+        <v>901.78</v>
+      </c>
+      <c r="M205">
+        <v>1127.03</v>
+      </c>
+      <c r="N205">
+        <v>285.2944</v>
+      </c>
+      <c r="O205">
+        <v>282.56</v>
+      </c>
+      <c r="P205">
+        <v>359.35</v>
+      </c>
+      <c r="Q205">
+        <v>336.62</v>
+      </c>
+      <c r="R205">
+        <v>167.56</v>
+      </c>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A206" s="1"/>
+      <c r="A206" s="1">
+        <v>44840</v>
+      </c>
+      <c r="B206">
+        <v>7943.6319999999996</v>
+      </c>
+      <c r="C206">
+        <v>7758.96</v>
+      </c>
+      <c r="D206">
+        <v>301.49</v>
+      </c>
+      <c r="E206">
+        <v>3748.44</v>
+      </c>
+      <c r="F206">
+        <v>135.25</v>
+      </c>
+      <c r="G206">
+        <v>108.6734</v>
+      </c>
+      <c r="H206">
+        <v>157.12</v>
+      </c>
+      <c r="I206">
+        <v>91.7727</v>
+      </c>
+      <c r="J206">
+        <v>93.487499999999997</v>
+      </c>
+      <c r="K206">
+        <v>127.2026</v>
+      </c>
+      <c r="L206">
+        <v>905.09</v>
+      </c>
+      <c r="M206">
+        <v>1127.3399999999999</v>
+      </c>
+      <c r="N206">
+        <v>285.14319999999998</v>
+      </c>
+      <c r="O206">
+        <v>282.74</v>
+      </c>
+      <c r="P206">
+        <v>359.45</v>
+      </c>
+      <c r="Q206">
+        <v>336.46</v>
+      </c>
+      <c r="R206">
+        <v>167.64</v>
+      </c>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A207" s="1"/>
+      <c r="A207" s="1">
+        <v>44841</v>
+      </c>
+      <c r="B207">
+        <v>7721.44</v>
+      </c>
+      <c r="C207">
+        <v>7629.67</v>
+      </c>
+      <c r="D207">
+        <v>294.45999999999998</v>
+      </c>
+      <c r="E207">
+        <v>3707.28</v>
+      </c>
+      <c r="F207">
+        <v>133.49</v>
+      </c>
+      <c r="G207">
+        <v>107.8449</v>
+      </c>
+      <c r="H207">
+        <v>154.28</v>
+      </c>
+      <c r="I207">
+        <v>92.298199999999994</v>
+      </c>
+      <c r="J207">
+        <v>93.977900000000005</v>
+      </c>
+      <c r="K207">
+        <v>127.58329999999999</v>
+      </c>
+      <c r="L207">
+        <v>915.5</v>
+      </c>
+      <c r="M207">
+        <v>1130.76</v>
+      </c>
+      <c r="N207">
+        <v>284.07690000000002</v>
+      </c>
+      <c r="O207">
+        <v>282.94</v>
+      </c>
+      <c r="P207">
+        <v>359.78</v>
+      </c>
+      <c r="Q207">
+        <v>336.72</v>
+      </c>
+      <c r="R207">
+        <v>167.57</v>
+      </c>
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A208" s="1"/>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A209" s="1"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A210" s="1"/>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A211" s="1"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A212" s="1"/>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A214" s="1"/>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A217" s="1"/>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A222" s="1"/>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" s="1">
+        <v>44844</v>
+      </c>
+      <c r="B208">
+        <v>7663.5820000000003</v>
+      </c>
+      <c r="C208">
+        <v>7587.66</v>
+      </c>
+      <c r="D208">
+        <v>291.60000000000002</v>
+      </c>
+      <c r="E208">
+        <v>3707.28</v>
+      </c>
+      <c r="F208">
+        <v>133.49</v>
+      </c>
+      <c r="G208">
+        <v>107.6786</v>
+      </c>
+      <c r="H208">
+        <v>153.43</v>
+      </c>
+      <c r="I208">
+        <v>92.628900000000002</v>
+      </c>
+      <c r="J208">
+        <v>94.2744</v>
+      </c>
+      <c r="K208">
+        <v>127.9342</v>
+      </c>
+      <c r="L208">
+        <v>917.96</v>
+      </c>
+      <c r="M208">
+        <v>1129.47</v>
+      </c>
+      <c r="N208">
+        <v>283.1961</v>
+      </c>
+      <c r="O208">
+        <v>282.94</v>
+      </c>
+      <c r="P208">
+        <v>359.96</v>
+      </c>
+      <c r="Q208">
+        <v>337.03</v>
+      </c>
+      <c r="R208">
+        <v>167.35</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A209" s="1">
+        <v>44845</v>
+      </c>
+      <c r="B209">
+        <v>7613.7529999999997</v>
+      </c>
+      <c r="C209">
+        <v>7550.3</v>
+      </c>
+      <c r="D209">
+        <v>288.77</v>
+      </c>
+      <c r="E209">
+        <v>3651.3</v>
+      </c>
+      <c r="F209">
+        <v>131.44999999999999</v>
+      </c>
+      <c r="G209">
+        <v>107.4308</v>
+      </c>
+      <c r="H209">
+        <v>152.30000000000001</v>
+      </c>
+      <c r="I209">
+        <v>92.529499999999999</v>
+      </c>
+      <c r="J209">
+        <v>94.415599999999998</v>
+      </c>
+      <c r="K209">
+        <v>127.8561</v>
+      </c>
+      <c r="L209">
+        <v>919.72</v>
+      </c>
+      <c r="M209">
+        <v>1129.6400000000001</v>
+      </c>
+      <c r="N209">
+        <v>283.03289999999998</v>
+      </c>
+      <c r="O209">
+        <v>282.97000000000003</v>
+      </c>
+      <c r="P209">
+        <v>359.52</v>
+      </c>
+      <c r="Q209">
+        <v>337.51</v>
+      </c>
+      <c r="R209">
+        <v>167.32</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A210" s="1">
+        <v>44846</v>
+      </c>
+      <c r="B210">
+        <v>7588.9009999999998</v>
+      </c>
+      <c r="C210">
+        <v>7530.36</v>
+      </c>
+      <c r="D210">
+        <v>287.87</v>
+      </c>
+      <c r="E210">
+        <v>3645.6</v>
+      </c>
+      <c r="F210">
+        <v>132.33000000000001</v>
+      </c>
+      <c r="G210">
+        <v>107.0826</v>
+      </c>
+      <c r="H210">
+        <v>151.38999999999999</v>
+      </c>
+      <c r="I210">
+        <v>92.517899999999997</v>
+      </c>
+      <c r="J210">
+        <v>94.445899999999995</v>
+      </c>
+      <c r="K210">
+        <v>127.8738</v>
+      </c>
+      <c r="L210">
+        <v>921.38</v>
+      </c>
+      <c r="M210">
+        <v>1130.51</v>
+      </c>
+      <c r="N210">
+        <v>283.2722</v>
+      </c>
+      <c r="O210">
+        <v>283.23</v>
+      </c>
+      <c r="P210">
+        <v>359.81</v>
+      </c>
+      <c r="Q210">
+        <v>338.05</v>
+      </c>
+      <c r="R210">
+        <v>167.47</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A211" s="1">
+        <v>44847</v>
+      </c>
+      <c r="B211">
+        <v>7786.9560000000001</v>
+      </c>
+      <c r="C211">
+        <v>7600.13</v>
+      </c>
+      <c r="D211">
+        <v>292.25</v>
+      </c>
+      <c r="E211">
+        <v>3626.85</v>
+      </c>
+      <c r="F211">
+        <v>130.62</v>
+      </c>
+      <c r="G211">
+        <v>107.8008</v>
+      </c>
+      <c r="H211">
+        <v>154.27000000000001</v>
+      </c>
+      <c r="I211">
+        <v>92.213899999999995</v>
+      </c>
+      <c r="J211">
+        <v>94.251300000000001</v>
+      </c>
+      <c r="K211">
+        <v>127.62309999999999</v>
+      </c>
+      <c r="L211">
+        <v>913.3</v>
+      </c>
+      <c r="M211">
+        <v>1128.18</v>
+      </c>
+      <c r="N211">
+        <v>282.20999999999998</v>
+      </c>
+      <c r="O211">
+        <v>282.43</v>
+      </c>
+      <c r="P211">
+        <v>358.52</v>
+      </c>
+      <c r="Q211">
+        <v>335.61</v>
+      </c>
+      <c r="R211">
+        <v>167.18</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A212" s="1">
+        <v>44848</v>
+      </c>
+      <c r="B212">
+        <v>7602.9880000000003</v>
+      </c>
+      <c r="C212">
+        <v>7643.82</v>
+      </c>
+      <c r="D212">
+        <v>288.79000000000002</v>
+      </c>
+      <c r="E212">
+        <v>3601.78</v>
+      </c>
+      <c r="F212">
+        <v>129.24</v>
+      </c>
+      <c r="G212">
+        <v>106.96559999999999</v>
+      </c>
+      <c r="H212">
+        <v>151.13999999999999</v>
+      </c>
+      <c r="I212">
+        <v>92.507999999999996</v>
+      </c>
+      <c r="J212">
+        <v>94.310100000000006</v>
+      </c>
+      <c r="K212">
+        <v>127.8613</v>
+      </c>
+      <c r="L212">
+        <v>920.98</v>
+      </c>
+      <c r="M212">
+        <v>1126.3</v>
+      </c>
+      <c r="N212">
+        <v>280.7312</v>
+      </c>
+      <c r="O212">
+        <v>282.77</v>
+      </c>
+      <c r="P212">
+        <v>359.24</v>
+      </c>
+      <c r="Q212">
+        <v>336.79</v>
+      </c>
+      <c r="R212">
+        <v>167.06</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A213" s="1">
+        <v>44851</v>
+      </c>
+      <c r="B213">
+        <v>7804.326</v>
+      </c>
+      <c r="C213">
+        <v>7779.25</v>
+      </c>
+      <c r="D213">
+        <v>294.85000000000002</v>
+      </c>
+      <c r="E213">
+        <v>3603.71</v>
+      </c>
+      <c r="F213">
+        <v>128.24</v>
+      </c>
+      <c r="G213">
+        <v>107.6793</v>
+      </c>
+      <c r="H213">
+        <v>154.51</v>
+      </c>
+      <c r="I213">
+        <v>92.000799999999998</v>
+      </c>
+      <c r="J213">
+        <v>93.8352</v>
+      </c>
+      <c r="K213">
+        <v>127.3467</v>
+      </c>
+      <c r="L213">
+        <v>913.51</v>
+      </c>
+      <c r="M213">
+        <v>1127.1099999999999</v>
+      </c>
+      <c r="N213">
+        <v>279.83269999999999</v>
+      </c>
+      <c r="O213">
+        <v>282.45999999999998</v>
+      </c>
+      <c r="P213">
+        <v>358.5</v>
+      </c>
+      <c r="Q213">
+        <v>336.22</v>
+      </c>
+      <c r="R213">
+        <v>167.46</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
+        <v>44852</v>
+      </c>
+      <c r="B214">
+        <v>7893.6769999999997</v>
+      </c>
+      <c r="C214">
+        <v>7829.4</v>
+      </c>
+      <c r="D214">
+        <v>298.16000000000003</v>
+      </c>
+      <c r="E214">
+        <v>3624.94</v>
+      </c>
+      <c r="F214">
+        <v>128.65</v>
+      </c>
+      <c r="G214">
+        <v>107.91079999999999</v>
+      </c>
+      <c r="H214">
+        <v>155.69</v>
+      </c>
+      <c r="I214">
+        <v>91.972399999999993</v>
+      </c>
+      <c r="J214">
+        <v>93.803299999999993</v>
+      </c>
+      <c r="K214">
+        <v>127.3798</v>
+      </c>
+      <c r="L214">
+        <v>909.8</v>
+      </c>
+      <c r="M214">
+        <v>1125.47</v>
+      </c>
+      <c r="N214">
+        <v>279.613</v>
+      </c>
+      <c r="O214">
+        <v>281.89999999999998</v>
+      </c>
+      <c r="P214">
+        <v>357.71</v>
+      </c>
+      <c r="Q214">
+        <v>335.1</v>
+      </c>
+      <c r="R214">
+        <v>167.24</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A215" s="1">
+        <v>44853</v>
+      </c>
+      <c r="B215">
+        <v>7840.9939999999997</v>
+      </c>
+      <c r="C215">
+        <v>7846.16</v>
+      </c>
+      <c r="D215">
+        <v>295.67</v>
+      </c>
+      <c r="E215">
+        <v>3569.45</v>
+      </c>
+      <c r="F215">
+        <v>125.47</v>
+      </c>
+      <c r="G215">
+        <v>107.7871</v>
+      </c>
+      <c r="H215">
+        <v>154.51</v>
+      </c>
+      <c r="I215">
+        <v>91.997100000000003</v>
+      </c>
+      <c r="J215">
+        <v>93.832899999999995</v>
+      </c>
+      <c r="K215">
+        <v>127.3573</v>
+      </c>
+      <c r="L215">
+        <v>912.84</v>
+      </c>
+      <c r="M215">
+        <v>1127.3</v>
+      </c>
+      <c r="N215">
+        <v>279.58870000000002</v>
+      </c>
+      <c r="O215">
+        <v>282.04000000000002</v>
+      </c>
+      <c r="P215">
+        <v>357.83</v>
+      </c>
+      <c r="Q215">
+        <v>335.49</v>
+      </c>
+      <c r="R215">
+        <v>167.45</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A216" s="1">
+        <v>44854</v>
+      </c>
+      <c r="B216">
+        <v>7779.5249999999996</v>
+      </c>
+      <c r="C216">
+        <v>7894.99</v>
+      </c>
+      <c r="D216">
+        <v>294.56</v>
+      </c>
+      <c r="E216">
+        <v>3530.66</v>
+      </c>
+      <c r="F216">
+        <v>122.79</v>
+      </c>
+      <c r="G216">
+        <v>107.1893</v>
+      </c>
+      <c r="H216">
+        <v>152.91999999999999</v>
+      </c>
+      <c r="I216">
+        <v>91.853200000000001</v>
+      </c>
+      <c r="J216">
+        <v>93.733999999999995</v>
+      </c>
+      <c r="K216">
+        <v>127.2277</v>
+      </c>
+      <c r="L216">
+        <v>916.29</v>
+      </c>
+      <c r="M216">
+        <v>1126.33</v>
+      </c>
+      <c r="N216">
+        <v>279.94369999999998</v>
+      </c>
+      <c r="O216">
+        <v>282.23</v>
+      </c>
+      <c r="P216">
+        <v>358.14</v>
+      </c>
+      <c r="Q216">
+        <v>335.54</v>
+      </c>
+      <c r="R216">
+        <v>167.43</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A217" s="1">
+        <v>44855</v>
+      </c>
+      <c r="B217">
+        <v>7964.2479999999996</v>
+      </c>
+      <c r="C217">
+        <v>7858.34</v>
+      </c>
+      <c r="D217">
+        <v>298.16000000000003</v>
+      </c>
+      <c r="E217">
+        <v>3496.25</v>
+      </c>
+      <c r="F217">
+        <v>119.14</v>
+      </c>
+      <c r="G217">
+        <v>108.43380000000001</v>
+      </c>
+      <c r="H217">
+        <v>156.51</v>
+      </c>
+      <c r="I217">
+        <v>91.776399999999995</v>
+      </c>
+      <c r="J217">
+        <v>93.625900000000001</v>
+      </c>
+      <c r="K217">
+        <v>127.1782</v>
+      </c>
+      <c r="L217">
+        <v>908.08</v>
+      </c>
+      <c r="M217">
+        <v>1122.72</v>
+      </c>
+      <c r="N217">
+        <v>277.82429999999999</v>
+      </c>
+      <c r="O217">
+        <v>282.33</v>
+      </c>
+      <c r="P217">
+        <v>358.21</v>
+      </c>
+      <c r="Q217">
+        <v>335.55</v>
+      </c>
+      <c r="R217">
+        <v>167.08</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A218" s="1">
+        <v>44858</v>
+      </c>
+      <c r="B218">
+        <v>8058.8789999999999</v>
+      </c>
+      <c r="C218">
+        <v>7974.19</v>
+      </c>
+      <c r="D218">
+        <v>300.64999999999998</v>
+      </c>
+      <c r="E218">
+        <v>3496.08</v>
+      </c>
+      <c r="F218">
+        <v>117.85</v>
+      </c>
+      <c r="G218">
+        <v>108.6968</v>
+      </c>
+      <c r="H218">
+        <v>157.82</v>
+      </c>
+      <c r="I218">
+        <v>91.783000000000001</v>
+      </c>
+      <c r="J218">
+        <v>93.701599999999999</v>
+      </c>
+      <c r="K218">
+        <v>127.2093</v>
+      </c>
+      <c r="L218">
+        <v>904.57</v>
+      </c>
+      <c r="M218">
+        <v>1123.1199999999999</v>
+      </c>
+      <c r="N218">
+        <v>278.11470000000003</v>
+      </c>
+      <c r="O218">
+        <v>282.42</v>
+      </c>
+      <c r="P218">
+        <v>358.28</v>
+      </c>
+      <c r="Q218">
+        <v>335.66</v>
+      </c>
+      <c r="R218">
+        <v>166.92</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A219" s="1">
+        <v>44859</v>
+      </c>
+      <c r="B219">
+        <v>8190.018</v>
+      </c>
+      <c r="C219">
+        <v>8104.81</v>
+      </c>
+      <c r="D219">
+        <v>305.52999999999997</v>
+      </c>
+      <c r="E219">
+        <v>3571.48</v>
+      </c>
+      <c r="F219">
+        <v>122.56</v>
+      </c>
+      <c r="G219">
+        <v>108.93219999999999</v>
+      </c>
+      <c r="H219">
+        <v>159.36000000000001</v>
+      </c>
+      <c r="I219">
+        <v>91.517799999999994</v>
+      </c>
+      <c r="J219">
+        <v>93.432900000000004</v>
+      </c>
+      <c r="K219">
+        <v>126.99250000000001</v>
+      </c>
+      <c r="L219">
+        <v>899.98</v>
+      </c>
+      <c r="M219">
+        <v>1121.57</v>
+      </c>
+      <c r="N219">
+        <v>277.6687</v>
+      </c>
+      <c r="O219">
+        <v>282.5</v>
+      </c>
+      <c r="P219">
+        <v>358.21</v>
+      </c>
+      <c r="Q219">
+        <v>335.6</v>
+      </c>
+      <c r="R219">
+        <v>166.88</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A220" s="1">
+        <v>44860</v>
+      </c>
+      <c r="B220">
+        <v>8129.6229999999996</v>
+      </c>
+      <c r="C220">
+        <v>8149.42</v>
+      </c>
+      <c r="D220">
+        <v>305.60000000000002</v>
+      </c>
+      <c r="E220">
+        <v>3607.71</v>
+      </c>
+      <c r="F220">
+        <v>125.04</v>
+      </c>
+      <c r="G220">
+        <v>108.39</v>
+      </c>
+      <c r="H220">
+        <v>158.46</v>
+      </c>
+      <c r="I220">
+        <v>91.381600000000006</v>
+      </c>
+      <c r="J220">
+        <v>93.253</v>
+      </c>
+      <c r="K220">
+        <v>126.8927</v>
+      </c>
+      <c r="L220">
+        <v>903.32</v>
+      </c>
+      <c r="M220">
+        <v>1125.82</v>
+      </c>
+      <c r="N220">
+        <v>277.39920000000001</v>
+      </c>
+      <c r="O220">
+        <v>282.8</v>
+      </c>
+      <c r="P220">
+        <v>358.71</v>
+      </c>
+      <c r="Q220">
+        <v>335.66</v>
+      </c>
+      <c r="R220">
+        <v>166.87</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A221" s="1">
+        <v>44861</v>
+      </c>
+      <c r="B221">
+        <v>8080.32</v>
+      </c>
+      <c r="C221">
+        <v>8147.6</v>
+      </c>
+      <c r="D221">
+        <v>304.58999999999997</v>
+      </c>
+      <c r="E221">
+        <v>3636.54</v>
+      </c>
+      <c r="F221">
+        <v>126.73</v>
+      </c>
+      <c r="G221">
+        <v>107.7576</v>
+      </c>
+      <c r="H221">
+        <v>157.78</v>
+      </c>
+      <c r="I221">
+        <v>91.307299999999998</v>
+      </c>
+      <c r="J221">
+        <v>93.159300000000002</v>
+      </c>
+      <c r="K221">
+        <v>126.8373</v>
+      </c>
+      <c r="L221">
+        <v>906</v>
+      </c>
+      <c r="M221">
+        <v>1132.9000000000001</v>
+      </c>
+      <c r="N221">
+        <v>278.57459999999998</v>
+      </c>
+      <c r="O221">
+        <v>282.94</v>
+      </c>
+      <c r="P221">
+        <v>358.95</v>
+      </c>
+      <c r="Q221">
+        <v>335.91</v>
+      </c>
+      <c r="R221">
+        <v>167.2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A222" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B222">
+        <v>8280.1059999999998</v>
+      </c>
+      <c r="C222">
+        <v>8166.85</v>
+      </c>
+      <c r="D222">
+        <v>308.14</v>
+      </c>
+      <c r="E222">
+        <v>3625.9</v>
+      </c>
+      <c r="F222">
+        <v>125.73</v>
+      </c>
+      <c r="G222">
+        <v>108.592</v>
+      </c>
+      <c r="H222">
+        <v>160.18</v>
+      </c>
+      <c r="I222">
+        <v>91.210499999999996</v>
+      </c>
+      <c r="J222">
+        <v>93.089299999999994</v>
+      </c>
+      <c r="K222">
+        <v>126.7839</v>
+      </c>
+      <c r="L222">
+        <v>897.8</v>
+      </c>
+      <c r="M222">
+        <v>1127.23</v>
+      </c>
+      <c r="N222">
+        <v>277.21319999999997</v>
+      </c>
+      <c r="O222">
+        <v>282.98</v>
+      </c>
+      <c r="P222">
+        <v>359.13</v>
+      </c>
+      <c r="Q222">
+        <v>336.09</v>
+      </c>
+      <c r="R222">
+        <v>167.25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A223" s="1">
+        <v>44865</v>
+      </c>
+      <c r="B223">
+        <v>8218.7049999999999</v>
+      </c>
+      <c r="C223">
+        <v>8179.88</v>
+      </c>
+      <c r="D223">
+        <v>306.81</v>
+      </c>
+      <c r="E223">
+        <v>3610.31</v>
+      </c>
+      <c r="F223">
+        <v>124.25</v>
+      </c>
+      <c r="G223">
+        <v>108.08839999999999</v>
+      </c>
+      <c r="H223">
+        <v>159.6</v>
+      </c>
+      <c r="I223">
+        <v>91.190600000000003</v>
+      </c>
+      <c r="J223">
+        <v>93.060400000000001</v>
+      </c>
+      <c r="K223">
+        <v>126.7722</v>
+      </c>
+      <c r="L223">
+        <v>901.15</v>
+      </c>
+      <c r="M223">
+        <v>1128.26</v>
+      </c>
+      <c r="N223">
+        <v>275.762</v>
+      </c>
+      <c r="O223">
+        <v>283.58</v>
+      </c>
+      <c r="P223">
+        <v>359.44</v>
+      </c>
+      <c r="Q223">
+        <v>336.89</v>
+      </c>
+      <c r="R223">
+        <v>167.37</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A224" s="1"/>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>